<commit_message>
Add Apollo 11 masses to spreadsheets
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmcal\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="Apollo 10" sheetId="1" r:id="rId1"/>
-    <sheet name="Apollo 9" sheetId="3" r:id="rId2"/>
-    <sheet name="Apollo 8" sheetId="4" r:id="rId3"/>
+    <sheet name="Apollo 11" sheetId="5" r:id="rId1"/>
+    <sheet name="Apollo 10" sheetId="1" r:id="rId2"/>
+    <sheet name="Apollo 9" sheetId="3" r:id="rId3"/>
+    <sheet name="Apollo 8" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="64">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -223,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>133344</v>
+        <v>130422</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -736,7 +732,7 @@
         <v>28</v>
       </c>
       <c r="G2">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -769,7 +765,7 @@
         <v>44</v>
       </c>
       <c r="AA2">
-        <v>11648</v>
+        <v>11273</v>
       </c>
       <c r="AB2" t="s">
         <v>13</v>
@@ -778,7 +774,7 @@
         <v>44</v>
       </c>
       <c r="AE2">
-        <v>11625</v>
+        <v>11250</v>
       </c>
       <c r="AF2" t="s">
         <v>13</v>
@@ -787,7 +783,7 @@
         <v>44</v>
       </c>
       <c r="AI2">
-        <v>11625</v>
+        <v>11250</v>
       </c>
       <c r="AJ2" t="s">
         <v>13</v>
@@ -796,7 +792,7 @@
         <v>44</v>
       </c>
       <c r="AM2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="AN2" t="s">
         <v>13</v>
@@ -805,7 +801,7 @@
         <v>44</v>
       </c>
       <c r="AQ2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="AR2" t="s">
         <v>13</v>
@@ -814,7 +810,7 @@
         <v>44</v>
       </c>
       <c r="AU2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="AV2" t="s">
         <v>13</v>
@@ -823,7 +819,7 @@
         <v>44</v>
       </c>
       <c r="AY2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="AZ2" t="s">
         <v>13</v>
@@ -832,7 +828,7 @@
         <v>44</v>
       </c>
       <c r="BC2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="BD2" t="s">
         <v>13</v>
@@ -841,7 +837,7 @@
         <v>44</v>
       </c>
       <c r="BG2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="BH2" t="s">
         <v>13</v>
@@ -850,7 +846,7 @@
         <v>44</v>
       </c>
       <c r="BK2">
-        <v>11563</v>
+        <v>11189</v>
       </c>
       <c r="BL2" t="s">
         <v>13</v>
@@ -861,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1477050</v>
+        <v>1478371</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -870,7 +866,7 @@
         <v>29</v>
       </c>
       <c r="G3">
-        <v>4033</v>
+        <v>3982</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -879,7 +875,7 @@
         <v>29</v>
       </c>
       <c r="K3">
-        <v>4033</v>
+        <v>3982</v>
       </c>
       <c r="L3" t="s">
         <v>13</v>
@@ -888,7 +884,7 @@
         <v>29</v>
       </c>
       <c r="O3">
-        <v>4033</v>
+        <v>3982</v>
       </c>
       <c r="P3" t="s">
         <v>13</v>
@@ -909,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="AA3">
-        <v>86964</v>
+        <v>87149</v>
       </c>
       <c r="AB3" t="s">
         <v>13</v>
@@ -918,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="AE3">
-        <v>86964</v>
+        <v>87149</v>
       </c>
       <c r="AF3" t="s">
         <v>13</v>
@@ -927,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="AI3">
-        <v>86801</v>
+        <v>86993</v>
       </c>
       <c r="AJ3" t="s">
         <v>13</v>
@@ -936,7 +932,7 @@
         <v>1</v>
       </c>
       <c r="AM3">
-        <v>60548</v>
+        <v>61120</v>
       </c>
       <c r="AN3" t="s">
         <v>13</v>
@@ -945,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="AQ3">
-        <v>60516</v>
+        <v>61052</v>
       </c>
       <c r="AR3" t="s">
         <v>13</v>
@@ -954,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="AU3">
-        <v>60375</v>
+        <v>60985</v>
       </c>
       <c r="AV3" t="s">
         <v>13</v>
@@ -963,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="AY3">
-        <v>60211</v>
+        <v>60857</v>
       </c>
       <c r="AZ3" t="s">
         <v>13</v>
@@ -972,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="BC3">
-        <v>2244</v>
+        <v>2308</v>
       </c>
       <c r="BD3" t="s">
         <v>13</v>
@@ -981,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="BG3">
-        <v>2212</v>
+        <v>2247</v>
       </c>
       <c r="BH3" t="s">
         <v>13</v>
@@ -990,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="BK3">
-        <v>2212</v>
+        <v>2224</v>
       </c>
       <c r="BL3" t="s">
         <v>13</v>
@@ -1001,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>21087</v>
+        <v>21108</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -1026,9 +1022,6 @@
       </c>
       <c r="N4" t="s">
         <v>30</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
       </c>
       <c r="P4" t="s">
         <v>13</v>
@@ -1141,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -1151,7 +1144,7 @@
       </c>
       <c r="G5">
         <f>SUM(G2:G4)</f>
-        <v>5254</v>
+        <v>5206</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -1161,7 +1154,7 @@
       </c>
       <c r="K5">
         <f>SUM(K2:K4)</f>
-        <v>4342</v>
+        <v>4291</v>
       </c>
       <c r="L5" t="s">
         <v>13</v>
@@ -1171,7 +1164,7 @@
       </c>
       <c r="O5">
         <f>SUM(O2:O4)</f>
-        <v>4033</v>
+        <v>3982</v>
       </c>
       <c r="P5" t="s">
         <v>13</v>
@@ -1200,7 +1193,7 @@
         <v>3</v>
       </c>
       <c r="AA5">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="AB5" t="s">
         <v>13</v>
@@ -1209,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="AE5">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="AF5" t="s">
         <v>13</v>
@@ -1218,7 +1211,7 @@
         <v>3</v>
       </c>
       <c r="AI5">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AJ5" t="s">
         <v>13</v>
@@ -1227,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="AM5">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="AN5" t="s">
         <v>13</v>
@@ -1236,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="AQ5">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="AR5" t="s">
         <v>13</v>
@@ -1245,7 +1238,7 @@
         <v>3</v>
       </c>
       <c r="AU5">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="AV5" t="s">
         <v>13</v>
@@ -1254,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="AY5">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="AZ5" t="s">
         <v>13</v>
@@ -1263,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="BC5">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="BD5" t="s">
         <v>13</v>
@@ -1272,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="BG5">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="BH5" t="s">
         <v>13</v>
@@ -1281,7 +1274,7 @@
         <v>3</v>
       </c>
       <c r="BK5">
-        <v>269</v>
+        <v>124</v>
       </c>
       <c r="BL5" t="s">
         <v>13</v>
@@ -1292,7 +1285,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>641271</v>
+        <v>642018</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1301,7 +1294,7 @@
         <v>32</v>
       </c>
       <c r="AA6">
-        <v>19659</v>
+        <v>19758</v>
       </c>
       <c r="AB6" t="s">
         <v>13</v>
@@ -1310,7 +1303,7 @@
         <v>32</v>
       </c>
       <c r="AE6">
-        <v>19654</v>
+        <v>19731</v>
       </c>
       <c r="AF6" t="s">
         <v>13</v>
@@ -1319,7 +1312,7 @@
         <v>32</v>
       </c>
       <c r="AI6">
-        <v>19598</v>
+        <v>19708</v>
       </c>
       <c r="AJ6" t="s">
         <v>13</v>
@@ -1328,7 +1321,7 @@
         <v>32</v>
       </c>
       <c r="AM6">
-        <v>14291</v>
+        <v>14369</v>
       </c>
       <c r="AN6" t="s">
         <v>13</v>
@@ -1337,7 +1330,7 @@
         <v>32</v>
       </c>
       <c r="AQ6">
-        <v>14277</v>
+        <v>14356</v>
       </c>
       <c r="AR6" t="s">
         <v>13</v>
@@ -1346,7 +1339,7 @@
         <v>32</v>
       </c>
       <c r="AU6">
-        <v>13180</v>
+        <v>13275</v>
       </c>
       <c r="AV6" t="s">
         <v>13</v>
@@ -1355,7 +1348,7 @@
         <v>32</v>
       </c>
       <c r="AY6">
-        <v>13116</v>
+        <v>13224</v>
       </c>
       <c r="AZ6" t="s">
         <v>13</v>
@@ -1364,7 +1357,7 @@
         <v>32</v>
       </c>
       <c r="BC6">
-        <v>973</v>
+        <v>944</v>
       </c>
       <c r="BD6" t="s">
         <v>13</v>
@@ -1373,7 +1366,7 @@
         <v>32</v>
       </c>
       <c r="BG6">
-        <v>961</v>
+        <v>932</v>
       </c>
       <c r="BH6" t="s">
         <v>13</v>
@@ -1382,7 +1375,7 @@
         <v>32</v>
       </c>
       <c r="BK6">
-        <v>961</v>
+        <v>391</v>
       </c>
       <c r="BL6" t="s">
         <v>13</v>
@@ -1393,7 +1386,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>4306</v>
+        <v>4301</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1402,7 +1395,7 @@
         <v>31</v>
       </c>
       <c r="G7">
-        <v>38226</v>
+        <v>36158</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -1411,7 +1404,7 @@
         <v>31</v>
       </c>
       <c r="K7">
-        <v>38226</v>
+        <v>36158</v>
       </c>
       <c r="L7" t="s">
         <v>13</v>
@@ -1420,7 +1413,7 @@
         <v>31</v>
       </c>
       <c r="O7">
-        <v>38226</v>
+        <v>36158</v>
       </c>
       <c r="P7" t="s">
         <v>13</v>
@@ -1429,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="S7">
-        <v>38226</v>
+        <v>36158</v>
       </c>
       <c r="T7" t="s">
         <v>13</v>
@@ -1438,7 +1431,7 @@
         <v>31</v>
       </c>
       <c r="W7">
-        <v>38226</v>
+        <v>36158</v>
       </c>
       <c r="X7" t="s">
         <v>13</v>
@@ -1548,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>372717</v>
+        <v>370778</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -1557,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <v>372717</v>
+        <v>370778</v>
       </c>
       <c r="L8" t="s">
         <v>13</v>
@@ -1566,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="O8">
-        <v>372270</v>
+        <v>370325</v>
       </c>
       <c r="P8" t="s">
         <v>13</v>
@@ -1584,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="W8">
-        <v>689</v>
+        <v>730</v>
       </c>
       <c r="X8" t="s">
         <v>13</v>
@@ -1593,7 +1586,7 @@
         <v>34</v>
       </c>
       <c r="AA8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AB8" t="s">
         <v>13</v>
@@ -1602,7 +1595,7 @@
         <v>34</v>
       </c>
       <c r="AE8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AF8" t="s">
         <v>13</v>
@@ -1611,7 +1604,7 @@
         <v>34</v>
       </c>
       <c r="AI8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AJ8" t="s">
         <v>13</v>
@@ -1620,7 +1613,7 @@
         <v>34</v>
       </c>
       <c r="AM8">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="AN8" t="s">
         <v>13</v>
@@ -1629,7 +1622,7 @@
         <v>34</v>
       </c>
       <c r="AQ8">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="AR8" t="s">
         <v>13</v>
@@ -1638,7 +1631,7 @@
         <v>34</v>
       </c>
       <c r="AU8">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="AV8" t="s">
         <v>13</v>
@@ -1647,7 +1640,7 @@
         <v>34</v>
       </c>
       <c r="AY8">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="AZ8" t="s">
         <v>13</v>
@@ -1656,7 +1649,7 @@
         <v>34</v>
       </c>
       <c r="BC8">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="BD8" t="s">
         <v>13</v>
@@ -1665,7 +1658,7 @@
         <v>34</v>
       </c>
       <c r="BG8">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="BH8" t="s">
         <v>13</v>
@@ -1674,7 +1667,7 @@
         <v>34</v>
       </c>
       <c r="BK8">
-        <v>274</v>
+        <v>156</v>
       </c>
       <c r="BL8" t="s">
         <v>13</v>
@@ -1831,7 +1824,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1840,7 +1833,7 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -1849,7 +1842,7 @@
         <v>3</v>
       </c>
       <c r="K10">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="L10" t="s">
         <v>13</v>
@@ -1858,7 +1851,7 @@
         <v>3</v>
       </c>
       <c r="O10">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="P10" t="s">
         <v>13</v>
@@ -1867,7 +1860,7 @@
         <v>3</v>
       </c>
       <c r="S10">
-        <v>2444</v>
+        <v>2335</v>
       </c>
       <c r="T10" t="s">
         <v>13</v>
@@ -1876,7 +1869,7 @@
         <v>3</v>
       </c>
       <c r="W10">
-        <v>2444</v>
+        <v>2335</v>
       </c>
       <c r="X10" t="s">
         <v>13</v>
@@ -1885,7 +1878,7 @@
         <v>46</v>
       </c>
       <c r="AA10">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="AB10" t="s">
         <v>13</v>
@@ -1894,7 +1887,7 @@
         <v>46</v>
       </c>
       <c r="AE10">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="AF10" t="s">
         <v>13</v>
@@ -1903,7 +1896,7 @@
         <v>46</v>
       </c>
       <c r="AI10">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="AJ10" t="s">
         <v>13</v>
@@ -1912,7 +1905,7 @@
         <v>46</v>
       </c>
       <c r="AM10">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AN10" t="s">
         <v>13</v>
@@ -1921,7 +1914,7 @@
         <v>46</v>
       </c>
       <c r="AQ10">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AR10" t="s">
         <v>13</v>
@@ -1948,7 +1941,7 @@
         <v>46</v>
       </c>
       <c r="BC10">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="BD10" t="s">
         <v>13</v>
@@ -1957,7 +1950,7 @@
         <v>46</v>
       </c>
       <c r="BG10">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="BH10" t="s">
         <v>13</v>
@@ -1966,7 +1959,7 @@
         <v>46</v>
       </c>
       <c r="BK10">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="BL10" t="s">
         <v>13</v>
@@ -1986,7 +1979,7 @@
         <v>32</v>
       </c>
       <c r="G11">
-        <v>71808</v>
+        <v>71615</v>
       </c>
       <c r="H11" t="s">
         <v>13</v>
@@ -1995,7 +1988,7 @@
         <v>32</v>
       </c>
       <c r="K11">
-        <v>17801</v>
+        <v>71608</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
@@ -2004,7 +1997,7 @@
         <v>32</v>
       </c>
       <c r="O11">
-        <v>71592</v>
+        <v>71396</v>
       </c>
       <c r="P11" t="s">
         <v>13</v>
@@ -2013,7 +2006,7 @@
         <v>32</v>
       </c>
       <c r="S11">
-        <v>1973</v>
+        <v>2572</v>
       </c>
       <c r="T11" t="s">
         <v>13</v>
@@ -2022,7 +2015,7 @@
         <v>32</v>
       </c>
       <c r="W11">
-        <v>1930</v>
+        <v>2531</v>
       </c>
       <c r="X11" t="s">
         <v>13</v>
@@ -2076,7 +2069,7 @@
         <v>47</v>
       </c>
       <c r="AU11">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AV11" t="s">
         <v>13</v>
@@ -2085,7 +2078,7 @@
         <v>47</v>
       </c>
       <c r="AY11">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AZ11" t="s">
         <v>13</v>
@@ -2094,7 +2087,7 @@
         <v>47</v>
       </c>
       <c r="BC11">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="BD11" t="s">
         <v>13</v>
@@ -2103,7 +2096,7 @@
         <v>47</v>
       </c>
       <c r="BG11">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="BH11" t="s">
         <v>13</v>
@@ -2112,7 +2105,7 @@
         <v>47</v>
       </c>
       <c r="BK11">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="BL11" t="s">
         <v>13</v>
@@ -2258,7 +2251,7 @@
         <v>36</v>
       </c>
       <c r="BK12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BL12" t="s">
         <v>13</v>
@@ -2305,7 +2298,7 @@
         <v>34</v>
       </c>
       <c r="S13">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="T13" t="s">
         <v>13</v>
@@ -2314,7 +2307,7 @@
         <v>34</v>
       </c>
       <c r="W13">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="X13" t="s">
         <v>13</v>
@@ -2416,7 +2409,7 @@
       </c>
       <c r="C14">
         <f>SUM(C2:C13)</f>
-        <v>2279547</v>
+        <v>2278688</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -2584,7 +2577,7 @@
       </c>
       <c r="AA15">
         <f>SUM(AA2:AA14)</f>
-        <v>119222</v>
+        <v>119118</v>
       </c>
       <c r="AB15" t="s">
         <v>13</v>
@@ -2594,7 +2587,7 @@
       </c>
       <c r="AE15">
         <f>SUM(AE2:AE14)</f>
-        <v>119063</v>
+        <v>118937</v>
       </c>
       <c r="AF15" t="s">
         <v>13</v>
@@ -2604,7 +2597,7 @@
       </c>
       <c r="AI15">
         <f>SUM(AI2:AI14)</f>
-        <v>118848</v>
+        <v>118763</v>
       </c>
       <c r="AJ15" t="s">
         <v>13</v>
@@ -2614,7 +2607,7 @@
       </c>
       <c r="AM15">
         <f>SUM(AM2:AM14)</f>
-        <v>87321</v>
+        <v>87550</v>
       </c>
       <c r="AN15" t="s">
         <v>13</v>
@@ -2624,7 +2617,7 @@
       </c>
       <c r="AQ15">
         <f>SUM(AQ2:AQ14)</f>
-        <v>87277</v>
+        <v>87469</v>
       </c>
       <c r="AR15" t="s">
         <v>13</v>
@@ -2634,7 +2627,7 @@
       </c>
       <c r="AU15">
         <f>SUM(AU2:AU14)</f>
-        <v>86090</v>
+        <v>86412</v>
       </c>
       <c r="AV15" t="s">
         <v>13</v>
@@ -2644,7 +2637,7 @@
       </c>
       <c r="AY15">
         <f>SUM(AY2:AY14)</f>
-        <v>85877</v>
+        <v>86249</v>
       </c>
       <c r="AZ15" t="s">
         <v>13</v>
@@ -2654,7 +2647,7 @@
       </c>
       <c r="BC15">
         <f>SUM(BC2:BC14)</f>
-        <v>15942</v>
+        <v>15556</v>
       </c>
       <c r="BD15" t="s">
         <v>13</v>
@@ -2664,7 +2657,7 @@
       </c>
       <c r="BG15">
         <f>SUM(BG2:BG14)</f>
-        <v>15898</v>
+        <v>15483</v>
       </c>
       <c r="BH15" t="s">
         <v>13</v>
@@ -2674,7 +2667,7 @@
       </c>
       <c r="BK15">
         <f>SUM(BK2:BK14)</f>
-        <v>15845</v>
+        <v>14581</v>
       </c>
       <c r="BL15" t="s">
         <v>13</v>
@@ -2685,7 +2678,7 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>5255</v>
+        <v>5206</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -2739,7 +2732,7 @@
         <v>18</v>
       </c>
       <c r="AA16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AB16" t="s">
         <v>13</v>
@@ -2748,7 +2741,7 @@
         <v>18</v>
       </c>
       <c r="AE16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AF16" t="s">
         <v>13</v>
@@ -2757,7 +2750,7 @@
         <v>18</v>
       </c>
       <c r="AI16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AJ16" t="s">
         <v>13</v>
@@ -2766,7 +2759,7 @@
         <v>18</v>
       </c>
       <c r="AM16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AN16" t="s">
         <v>13</v>
@@ -2775,7 +2768,7 @@
         <v>18</v>
       </c>
       <c r="AQ16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AR16" t="s">
         <v>13</v>
@@ -2784,7 +2777,7 @@
         <v>18</v>
       </c>
       <c r="AU16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AV16" t="s">
         <v>13</v>
@@ -2793,7 +2786,7 @@
         <v>18</v>
       </c>
       <c r="AY16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="AZ16" t="s">
         <v>13</v>
@@ -2802,7 +2795,7 @@
         <v>18</v>
       </c>
       <c r="BC16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="BD16" t="s">
         <v>13</v>
@@ -2811,7 +2804,7 @@
         <v>18</v>
       </c>
       <c r="BG16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="BH16" t="s">
         <v>13</v>
@@ -2820,7 +2813,7 @@
         <v>18</v>
       </c>
       <c r="BK16">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="BL16" t="s">
         <v>13</v>
@@ -2831,7 +2824,7 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>484159</v>
+        <v>479964</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -2885,7 +2878,7 @@
         <v>19</v>
       </c>
       <c r="AA17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AB17" t="s">
         <v>13</v>
@@ -2894,7 +2887,7 @@
         <v>19</v>
       </c>
       <c r="AE17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AF17" t="s">
         <v>13</v>
@@ -2903,7 +2896,7 @@
         <v>19</v>
       </c>
       <c r="AI17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AJ17" t="s">
         <v>13</v>
@@ -2912,7 +2905,7 @@
         <v>19</v>
       </c>
       <c r="AM17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AN17" t="s">
         <v>13</v>
@@ -2921,7 +2914,7 @@
         <v>19</v>
       </c>
       <c r="AQ17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AR17" t="s">
         <v>13</v>
@@ -2930,7 +2923,7 @@
         <v>19</v>
       </c>
       <c r="AU17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AV17" t="s">
         <v>13</v>
@@ -2939,7 +2932,7 @@
         <v>19</v>
       </c>
       <c r="AY17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="AZ17" t="s">
         <v>13</v>
@@ -2948,7 +2941,7 @@
         <v>19</v>
       </c>
       <c r="BC17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="BD17" t="s">
         <v>13</v>
@@ -2957,7 +2950,7 @@
         <v>19</v>
       </c>
       <c r="BG17">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="BH17" t="s">
         <v>13</v>
@@ -2977,7 +2970,7 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>3649</v>
+        <v>3663</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -2987,7 +2980,7 @@
       </c>
       <c r="G18">
         <f>SUM(G7:G17)</f>
-        <v>484160</v>
+        <v>479964</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -2997,7 +2990,7 @@
       </c>
       <c r="K18">
         <f>SUM(K7:K17)</f>
-        <v>429902</v>
+        <v>479706</v>
       </c>
       <c r="L18" t="s">
         <v>13</v>
@@ -3007,7 +3000,7 @@
       </c>
       <c r="O18">
         <f>SUM(O7:O17)</f>
-        <v>483316</v>
+        <v>479112</v>
       </c>
       <c r="P18" t="s">
         <v>13</v>
@@ -3017,7 +3010,7 @@
       </c>
       <c r="S18">
         <f>SUM(S7:S17)</f>
-        <v>45142</v>
+        <v>43562</v>
       </c>
       <c r="T18" t="s">
         <v>13</v>
@@ -3027,7 +3020,7 @@
       </c>
       <c r="W18">
         <f>SUM(W7:W17)</f>
-        <v>44972</v>
+        <v>43435</v>
       </c>
       <c r="X18" t="s">
         <v>13</v>
@@ -3036,7 +3029,7 @@
         <v>20</v>
       </c>
       <c r="AA18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AB18" t="s">
         <v>13</v>
@@ -3045,7 +3038,7 @@
         <v>20</v>
       </c>
       <c r="AE18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AF18" t="s">
         <v>13</v>
@@ -3054,7 +3047,7 @@
         <v>20</v>
       </c>
       <c r="AI18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AJ18" t="s">
         <v>13</v>
@@ -3063,7 +3056,7 @@
         <v>20</v>
       </c>
       <c r="AM18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AN18" t="s">
         <v>13</v>
@@ -3072,7 +3065,7 @@
         <v>20</v>
       </c>
       <c r="AQ18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AR18" t="s">
         <v>13</v>
@@ -3081,7 +3074,7 @@
         <v>20</v>
       </c>
       <c r="AU18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AV18" t="s">
         <v>13</v>
@@ -3090,7 +3083,7 @@
         <v>20</v>
       </c>
       <c r="AY18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="AZ18" t="s">
         <v>13</v>
@@ -3099,7 +3092,7 @@
         <v>20</v>
       </c>
       <c r="BC18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="BD18" t="s">
         <v>13</v>
@@ -3108,7 +3101,7 @@
         <v>20</v>
       </c>
       <c r="BG18">
-        <v>46507</v>
+        <v>47632</v>
       </c>
       <c r="BH18" t="s">
         <v>13</v>
@@ -3117,7 +3110,7 @@
         <v>20</v>
       </c>
       <c r="BK18">
-        <v>2551</v>
+        <v>2565</v>
       </c>
       <c r="BL18" t="s">
         <v>13</v>
@@ -3128,7 +3121,7 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>199223</v>
+        <v>119119</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
@@ -3137,7 +3130,7 @@
         <v>21</v>
       </c>
       <c r="AA19">
-        <v>165730</v>
+        <v>166751</v>
       </c>
       <c r="AB19" t="s">
         <v>13</v>
@@ -3146,7 +3139,7 @@
         <v>21</v>
       </c>
       <c r="AE19">
-        <v>165573</v>
+        <v>166751</v>
       </c>
       <c r="AF19" t="s">
         <v>13</v>
@@ -3155,7 +3148,7 @@
         <v>21</v>
       </c>
       <c r="AI19">
-        <v>165355</v>
+        <v>166396</v>
       </c>
       <c r="AJ19" t="s">
         <v>13</v>
@@ -3164,7 +3157,7 @@
         <v>21</v>
       </c>
       <c r="AM19">
-        <v>133830</v>
+        <v>135182</v>
       </c>
       <c r="AN19" t="s">
         <v>13</v>
@@ -3173,7 +3166,7 @@
         <v>21</v>
       </c>
       <c r="AQ19">
-        <v>133786</v>
+        <v>135102</v>
       </c>
       <c r="AR19" t="s">
         <v>13</v>
@@ -3182,7 +3175,7 @@
         <v>21</v>
       </c>
       <c r="AU19">
-        <v>132600</v>
+        <v>134046</v>
       </c>
       <c r="AV19" t="s">
         <v>13</v>
@@ -3191,7 +3184,7 @@
         <v>21</v>
       </c>
       <c r="AY19">
-        <v>132385</v>
+        <v>133883</v>
       </c>
       <c r="AZ19" t="s">
         <v>13</v>
@@ -3200,7 +3193,7 @@
         <v>21</v>
       </c>
       <c r="BC19">
-        <v>62450</v>
+        <v>63189</v>
       </c>
       <c r="BD19" t="s">
         <v>13</v>
@@ -3209,7 +3202,7 @@
         <v>21</v>
       </c>
       <c r="BG19">
-        <v>62407</v>
+        <v>63116</v>
       </c>
       <c r="BH19" t="s">
         <v>13</v>
@@ -3218,7 +3211,7 @@
         <v>21</v>
       </c>
       <c r="BK19">
-        <v>18408</v>
+        <v>17148</v>
       </c>
       <c r="BL19" t="s">
         <v>13</v>
@@ -3229,7 +3222,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -3238,7 +3231,7 @@
         <v>16</v>
       </c>
       <c r="G20">
-        <v>3649</v>
+        <v>3663</v>
       </c>
       <c r="H20" t="s">
         <v>13</v>
@@ -3247,7 +3240,7 @@
         <v>16</v>
       </c>
       <c r="K20">
-        <v>3649</v>
+        <v>3663</v>
       </c>
       <c r="L20" t="s">
         <v>13</v>
@@ -3256,7 +3249,7 @@
         <v>16</v>
       </c>
       <c r="O20">
-        <v>3649</v>
+        <v>3663</v>
       </c>
       <c r="P20" t="s">
         <v>13</v>
@@ -3265,7 +3258,7 @@
         <v>16</v>
       </c>
       <c r="S20">
-        <v>3649</v>
+        <v>3663</v>
       </c>
       <c r="T20" t="s">
         <v>13</v>
@@ -3274,7 +3267,7 @@
         <v>16</v>
       </c>
       <c r="W20">
-        <v>3548</v>
+        <v>3663</v>
       </c>
       <c r="X20" t="s">
         <v>13</v>
@@ -3285,7 +3278,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>48625</v>
+        <v>49735</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
@@ -3294,7 +3287,7 @@
         <v>17</v>
       </c>
       <c r="G21">
-        <v>119223</v>
+        <v>119119</v>
       </c>
       <c r="H21" t="s">
         <v>13</v>
@@ -3303,7 +3296,7 @@
         <v>17</v>
       </c>
       <c r="K21">
-        <v>119132</v>
+        <v>119029</v>
       </c>
       <c r="L21" t="s">
         <v>13</v>
@@ -3312,7 +3305,7 @@
         <v>17</v>
       </c>
       <c r="O21">
-        <v>119132</v>
+        <v>119029</v>
       </c>
       <c r="P21" t="s">
         <v>13</v>
@@ -3321,7 +3314,7 @@
         <v>17</v>
       </c>
       <c r="S21">
-        <v>119132</v>
+        <v>119029</v>
       </c>
       <c r="T21" t="s">
         <v>13</v>
@@ -3330,7 +3323,7 @@
         <v>17</v>
       </c>
       <c r="W21">
-        <v>119130</v>
+        <v>119026</v>
       </c>
       <c r="X21" t="s">
         <v>13</v>
@@ -3341,7 +3334,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>662847</v>
+        <v>659626</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -3350,7 +3343,7 @@
         <v>18</v>
       </c>
       <c r="G22">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="H22" t="s">
         <v>13</v>
@@ -3359,7 +3352,7 @@
         <v>18</v>
       </c>
       <c r="K22">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="L22" t="s">
         <v>13</v>
@@ -3368,7 +3361,7 @@
         <v>18</v>
       </c>
       <c r="O22">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="P22" t="s">
         <v>13</v>
@@ -3377,7 +3370,7 @@
         <v>18</v>
       </c>
       <c r="S22">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="T22" t="s">
         <v>13</v>
@@ -3386,7 +3379,7 @@
         <v>18</v>
       </c>
       <c r="W22">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="X22" t="s">
         <v>13</v>
@@ -3397,7 +3390,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>2942396</v>
+        <v>2938315</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -3406,7 +3399,7 @@
         <v>19</v>
       </c>
       <c r="G23">
-        <v>48625</v>
+        <v>49735</v>
       </c>
       <c r="H23" t="s">
         <v>13</v>
@@ -3415,7 +3408,7 @@
         <v>19</v>
       </c>
       <c r="K23">
-        <v>48625</v>
+        <v>49735</v>
       </c>
       <c r="L23" t="s">
         <v>13</v>
@@ -3424,7 +3417,7 @@
         <v>19</v>
       </c>
       <c r="O23">
-        <v>48625</v>
+        <v>49735</v>
       </c>
       <c r="P23" t="s">
         <v>13</v>
@@ -3433,7 +3426,7 @@
         <v>19</v>
       </c>
       <c r="S23">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="T23" t="s">
         <v>13</v>
@@ -3442,7 +3435,7 @@
         <v>19</v>
       </c>
       <c r="W23">
-        <v>44572</v>
+        <v>45693</v>
       </c>
       <c r="X23" t="s">
         <v>13</v>
@@ -3453,7 +3446,7 @@
         <v>20</v>
       </c>
       <c r="G24">
-        <v>173432</v>
+        <v>174456</v>
       </c>
       <c r="H24" t="s">
         <v>13</v>
@@ -3462,7 +3455,7 @@
         <v>20</v>
       </c>
       <c r="K24">
-        <v>173048</v>
+        <v>174365</v>
       </c>
       <c r="L24" t="s">
         <v>13</v>
@@ -3471,7 +3464,7 @@
         <v>20</v>
       </c>
       <c r="O24">
-        <v>173342</v>
+        <v>174365</v>
       </c>
       <c r="P24" t="s">
         <v>13</v>
@@ -3480,7 +3473,7 @@
         <v>20</v>
       </c>
       <c r="S24">
-        <v>169288</v>
+        <v>170324</v>
       </c>
       <c r="T24" t="s">
         <v>13</v>
@@ -3489,7 +3482,7 @@
         <v>20</v>
       </c>
       <c r="W24">
-        <v>169286</v>
+        <v>170322</v>
       </c>
       <c r="X24" t="s">
         <v>13</v>
@@ -3500,7 +3493,7 @@
         <v>21</v>
       </c>
       <c r="G25">
-        <v>662847</v>
+        <v>659626</v>
       </c>
       <c r="H25" t="s">
         <v>13</v>
@@ -3509,7 +3502,7 @@
         <v>21</v>
       </c>
       <c r="K25">
-        <v>660807</v>
+        <v>658363</v>
       </c>
       <c r="L25" t="s">
         <v>13</v>
@@ -3518,7 +3511,7 @@
         <v>21</v>
       </c>
       <c r="O25">
-        <v>660690</v>
+        <v>657459</v>
       </c>
       <c r="P25" t="s">
         <v>13</v>
@@ -3527,7 +3520,7 @@
         <v>21</v>
       </c>
       <c r="S25">
-        <v>214432</v>
+        <v>213888</v>
       </c>
       <c r="T25" t="s">
         <v>13</v>
@@ -3536,7 +3529,7 @@
         <v>21</v>
       </c>
       <c r="W25">
-        <v>214258</v>
+        <v>213757</v>
       </c>
       <c r="X25" t="s">
         <v>13</v>
@@ -3548,7 +3541,7 @@
       </c>
       <c r="B28">
         <f>C3+C5+C6+C8</f>
-        <v>2118585</v>
+        <v>2120631</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -3560,7 +3553,7 @@
       </c>
       <c r="B29">
         <f>G8+G10+G11+G13</f>
-        <v>444786</v>
+        <v>442658</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
@@ -3572,7 +3565,7 @@
       </c>
       <c r="B30">
         <f>AA3+AA5+AA6+AA8+AA10</f>
-        <v>106969</v>
+        <v>107240</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
@@ -3584,7 +3577,7 @@
       </c>
       <c r="B31">
         <f>C2+C9+C10+C11+C13+B36</f>
-        <v>135517</v>
+        <v>132596</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
@@ -3596,7 +3589,7 @@
       </c>
       <c r="B32">
         <f>G7+G9+G12+G16+G17</f>
-        <v>39116</v>
+        <v>37048</v>
       </c>
       <c r="C32" t="s">
         <v>13</v>
@@ -3608,7 +3601,7 @@
       </c>
       <c r="B33">
         <f>AA2+AA4+AA7+AA11+AA12+AA14</f>
-        <v>12063</v>
+        <v>11688</v>
       </c>
       <c r="C33" t="s">
         <v>13</v>
@@ -3620,7 +3613,7 @@
       </c>
       <c r="B34">
         <f>C16</f>
-        <v>5255</v>
+        <v>5206</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -3668,7 +3661,7 @@
       </c>
       <c r="B39">
         <f>AA10</f>
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
@@ -3682,9 +3675,3105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BL39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC1" s="1"/>
+      <c r="BD1" s="1"/>
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BG1" s="1"/>
+      <c r="BH1" s="1"/>
+      <c r="BI1" s="1"/>
+      <c r="BJ1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="BK1" s="1"/>
+      <c r="BL1" s="1"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>133344</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>611</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA2">
+        <v>11648</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2">
+        <v>11625</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2">
+        <v>11625</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM2">
+        <v>11563</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ2">
+        <v>11563</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU2">
+        <v>11563</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY2">
+        <v>11563</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC2">
+        <v>11563</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BG2">
+        <v>11563</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BK2">
+        <v>11563</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1477050</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>4033</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>4033</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3">
+        <v>4033</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>86964</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>86964</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>86801</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>60548</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>60516</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>60375</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>60211</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC3">
+        <v>2244</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG3">
+        <v>2212</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BK3">
+        <v>2212</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>21087</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>610</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>309</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>166</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4">
+        <v>166</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI4">
+        <v>180</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM4">
+        <v>180</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ4">
+        <v>180</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU4">
+        <v>166</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY4">
+        <v>180</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC4">
+        <v>180</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG4">
+        <v>180</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK4">
+        <v>166</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>191</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <f>SUM(G2:G4)</f>
+        <v>5254</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <f>SUM(K2:K4)</f>
+        <v>4342</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5">
+        <f>SUM(O2:O4)</f>
+        <v>4033</v>
+      </c>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5">
+        <f>SUM(S2:S4)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5">
+        <f>SUM(W2:W4)</f>
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>22</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE5">
+        <v>22</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI5">
+        <v>23</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM5">
+        <v>100</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ5">
+        <v>101</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU5">
+        <v>156</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AY5">
+        <v>158</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC5">
+        <v>269</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BG5">
+        <v>269</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK5">
+        <v>269</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>641271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA6">
+        <v>19659</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6">
+        <v>19654</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI6">
+        <v>19598</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM6">
+        <v>14291</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ6">
+        <v>14277</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU6">
+        <v>13180</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY6">
+        <v>13116</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>32</v>
+      </c>
+      <c r="BC6">
+        <v>973</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>32</v>
+      </c>
+      <c r="BG6">
+        <v>961</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>32</v>
+      </c>
+      <c r="BK6">
+        <v>961</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>4306</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7">
+        <v>38226</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7">
+        <v>38226</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7">
+        <v>38226</v>
+      </c>
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7">
+        <v>38226</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W7">
+        <v>38226</v>
+      </c>
+      <c r="X7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA7">
+        <v>22</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE7">
+        <v>26</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI7">
+        <v>26</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM7">
+        <v>26</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ7">
+        <v>26</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU7">
+        <v>26</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY7">
+        <v>26</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC7">
+        <v>26</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>33</v>
+      </c>
+      <c r="BG7">
+        <v>26</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>33</v>
+      </c>
+      <c r="BK7">
+        <v>22</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>372717</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>372717</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>372270</v>
+      </c>
+      <c r="P8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>816</v>
+      </c>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>689</v>
+      </c>
+      <c r="X8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA8">
+        <v>21</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE8">
+        <v>21</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI8">
+        <v>21</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM8">
+        <v>65</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ8">
+        <v>66</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU8">
+        <v>143</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY8">
+        <v>144</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC8">
+        <v>274</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF8" t="s">
+        <v>34</v>
+      </c>
+      <c r="BG8">
+        <v>274</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>34</v>
+      </c>
+      <c r="BK8">
+        <v>274</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>737</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>737</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>800</v>
+      </c>
+      <c r="P9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>787</v>
+      </c>
+      <c r="T9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" t="s">
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <v>787</v>
+      </c>
+      <c r="X9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA9">
+        <v>54</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE9">
+        <v>10</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM9">
+        <v>1</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ9">
+        <v>1</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>45</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>45</v>
+      </c>
+      <c r="BK9">
+        <v>0</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>288</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>184</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>184</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>186</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>2444</v>
+      </c>
+      <c r="T10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <v>2444</v>
+      </c>
+      <c r="X10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA10">
+        <v>303</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE10">
+        <v>303</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI10">
+        <v>303</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM10">
+        <v>298</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ10">
+        <v>298</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU10">
+        <v>246</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY10">
+        <v>246</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC10">
+        <v>241</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG10">
+        <v>241</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>46</v>
+      </c>
+      <c r="BK10">
+        <v>206</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>635</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>71808</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11">
+        <v>17801</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11">
+        <v>71592</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11">
+        <v>1973</v>
+      </c>
+      <c r="T11" t="s">
+        <v>13</v>
+      </c>
+      <c r="V11" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11">
+        <v>1930</v>
+      </c>
+      <c r="X11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA11">
+        <v>200</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE11">
+        <v>200</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI11">
+        <v>200</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM11">
+        <v>176</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ11">
+        <v>176</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU11">
+        <v>163</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY11">
+        <v>163</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC11">
+        <v>99</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>47</v>
+      </c>
+      <c r="BG11">
+        <v>99</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>47</v>
+      </c>
+      <c r="BK11">
+        <v>99</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1027</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12">
+        <v>105</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12">
+        <v>112</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12">
+        <v>128</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12">
+        <v>123</v>
+      </c>
+      <c r="T12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" t="s">
+        <v>33</v>
+      </c>
+      <c r="W12">
+        <v>123</v>
+      </c>
+      <c r="X12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA12">
+        <v>2</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE12">
+        <v>2</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM12">
+        <v>3</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ12">
+        <v>3</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU12">
+        <v>2</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC12">
+        <v>3</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG12">
+        <v>3</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK12">
+        <v>3</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>239</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13">
+        <v>77</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13">
+        <v>78</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" t="s">
+        <v>34</v>
+      </c>
+      <c r="S13">
+        <v>737</v>
+      </c>
+      <c r="T13" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13">
+        <v>737</v>
+      </c>
+      <c r="X13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13">
+        <v>136</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE13">
+        <v>45</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI13">
+        <v>45</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM13">
+        <v>45</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ13">
+        <v>45</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU13">
+        <v>45</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY13">
+        <v>45</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC13">
+        <v>45</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG13">
+        <v>45</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK13">
+        <v>45</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C2:C13)</f>
+        <v>2279547</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" t="s">
+        <v>35</v>
+      </c>
+      <c r="T14" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" t="s">
+        <v>35</v>
+      </c>
+      <c r="X14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14">
+        <v>25</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE14">
+        <v>25</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI14">
+        <v>25</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM14">
+        <v>25</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ14">
+        <v>25</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU14">
+        <v>25</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY14">
+        <v>25</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC14">
+        <v>25</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG14">
+        <v>25</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>11</v>
+      </c>
+      <c r="BK14">
+        <v>25</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>204</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="R15" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" t="s">
+        <v>13</v>
+      </c>
+      <c r="V15" t="s">
+        <v>9</v>
+      </c>
+      <c r="X15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA15">
+        <f>SUM(AA2:AA14)</f>
+        <v>119222</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE15">
+        <f>SUM(AE2:AE14)</f>
+        <v>119063</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI15">
+        <f>SUM(AI2:AI14)</f>
+        <v>118848</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM15">
+        <f>SUM(AM2:AM14)</f>
+        <v>87321</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ15">
+        <f>SUM(AQ2:AQ14)</f>
+        <v>87277</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU15">
+        <f>SUM(AU2:AU14)</f>
+        <v>86090</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AY15">
+        <f>SUM(AY2:AY14)</f>
+        <v>85877</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC15">
+        <f>SUM(BC2:BC14)</f>
+        <v>15942</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>17</v>
+      </c>
+      <c r="BG15">
+        <f>SUM(BG2:BG14)</f>
+        <v>15898</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>17</v>
+      </c>
+      <c r="BK15">
+        <f>SUM(BK2:BK14)</f>
+        <v>15845</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>5255</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" t="s">
+        <v>36</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+      <c r="X16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16">
+        <v>1935</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE16">
+        <v>1935</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI16">
+        <v>1935</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM16">
+        <v>1935</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ16">
+        <v>1935</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU16">
+        <v>1935</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AY16">
+        <v>1935</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC16">
+        <v>1935</v>
+      </c>
+      <c r="BD16" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>18</v>
+      </c>
+      <c r="BG16">
+        <v>1935</v>
+      </c>
+      <c r="BH16" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>18</v>
+      </c>
+      <c r="BK16">
+        <v>1935</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>484159</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17">
+        <v>34</v>
+      </c>
+      <c r="P17" t="s">
+        <v>13</v>
+      </c>
+      <c r="R17" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <v>34</v>
+      </c>
+      <c r="T17" t="s">
+        <v>13</v>
+      </c>
+      <c r="V17" t="s">
+        <v>11</v>
+      </c>
+      <c r="W17">
+        <v>34</v>
+      </c>
+      <c r="X17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA17">
+        <v>44572</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE17">
+        <v>44572</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI17">
+        <v>44572</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM17">
+        <v>44572</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ17">
+        <v>44572</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU17">
+        <v>44572</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY17">
+        <v>44572</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC17">
+        <v>44572</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>19</v>
+      </c>
+      <c r="BG17">
+        <v>44572</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>19</v>
+      </c>
+      <c r="BK17">
+        <v>626</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>3649</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <f>SUM(G7:G17)</f>
+        <v>484160</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <f>SUM(K7:K17)</f>
+        <v>429902</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18">
+        <f>SUM(O7:O17)</f>
+        <v>483316</v>
+      </c>
+      <c r="P18" t="s">
+        <v>13</v>
+      </c>
+      <c r="R18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18">
+        <f>SUM(S7:S17)</f>
+        <v>45142</v>
+      </c>
+      <c r="T18" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" t="s">
+        <v>15</v>
+      </c>
+      <c r="W18">
+        <f>SUM(W7:W17)</f>
+        <v>44972</v>
+      </c>
+      <c r="X18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA18">
+        <v>46507</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE18">
+        <v>46507</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI18">
+        <v>46507</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM18">
+        <v>46507</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ18">
+        <v>46507</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AU18">
+        <v>46507</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AY18">
+        <v>46507</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>20</v>
+      </c>
+      <c r="BC18">
+        <v>46507</v>
+      </c>
+      <c r="BD18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>20</v>
+      </c>
+      <c r="BG18">
+        <v>46507</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>20</v>
+      </c>
+      <c r="BK18">
+        <v>2551</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>199223</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA19">
+        <v>165730</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE19">
+        <v>165573</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI19">
+        <v>165355</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM19">
+        <v>133830</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ19">
+        <v>133786</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU19">
+        <v>132600</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY19">
+        <v>132385</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>21</v>
+      </c>
+      <c r="BC19">
+        <v>62450</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>21</v>
+      </c>
+      <c r="BG19">
+        <v>62407</v>
+      </c>
+      <c r="BH19" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ19" t="s">
+        <v>21</v>
+      </c>
+      <c r="BK19">
+        <v>18408</v>
+      </c>
+      <c r="BL19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>1935</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>3649</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20">
+        <v>3649</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O20">
+        <v>3649</v>
+      </c>
+      <c r="P20" t="s">
+        <v>13</v>
+      </c>
+      <c r="R20" t="s">
+        <v>16</v>
+      </c>
+      <c r="S20">
+        <v>3649</v>
+      </c>
+      <c r="T20" t="s">
+        <v>13</v>
+      </c>
+      <c r="V20" t="s">
+        <v>16</v>
+      </c>
+      <c r="W20">
+        <v>3548</v>
+      </c>
+      <c r="X20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>48625</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>119223</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21">
+        <v>119132</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21">
+        <v>119132</v>
+      </c>
+      <c r="P21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R21" t="s">
+        <v>17</v>
+      </c>
+      <c r="S21">
+        <v>119132</v>
+      </c>
+      <c r="T21" t="s">
+        <v>13</v>
+      </c>
+      <c r="V21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W21">
+        <v>119130</v>
+      </c>
+      <c r="X21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>662847</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22">
+        <v>1935</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22">
+        <v>1935</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" t="s">
+        <v>18</v>
+      </c>
+      <c r="O22">
+        <v>1935</v>
+      </c>
+      <c r="P22" t="s">
+        <v>13</v>
+      </c>
+      <c r="R22" t="s">
+        <v>18</v>
+      </c>
+      <c r="S22">
+        <v>1935</v>
+      </c>
+      <c r="T22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" t="s">
+        <v>18</v>
+      </c>
+      <c r="W22">
+        <v>1935</v>
+      </c>
+      <c r="X22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>2942396</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23">
+        <v>48625</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23">
+        <v>48625</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23">
+        <v>48625</v>
+      </c>
+      <c r="P23" t="s">
+        <v>13</v>
+      </c>
+      <c r="R23" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23">
+        <v>44572</v>
+      </c>
+      <c r="T23" t="s">
+        <v>13</v>
+      </c>
+      <c r="V23" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23">
+        <v>44572</v>
+      </c>
+      <c r="X23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24">
+        <v>173432</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24">
+        <v>173048</v>
+      </c>
+      <c r="L24" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24">
+        <v>173342</v>
+      </c>
+      <c r="P24" t="s">
+        <v>13</v>
+      </c>
+      <c r="R24" t="s">
+        <v>20</v>
+      </c>
+      <c r="S24">
+        <v>169288</v>
+      </c>
+      <c r="T24" t="s">
+        <v>13</v>
+      </c>
+      <c r="V24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W24">
+        <v>169286</v>
+      </c>
+      <c r="X24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25">
+        <v>662847</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25">
+        <v>660807</v>
+      </c>
+      <c r="L25" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25">
+        <v>660690</v>
+      </c>
+      <c r="P25" t="s">
+        <v>13</v>
+      </c>
+      <c r="R25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S25">
+        <v>214432</v>
+      </c>
+      <c r="T25" t="s">
+        <v>13</v>
+      </c>
+      <c r="V25" t="s">
+        <v>21</v>
+      </c>
+      <c r="W25">
+        <v>214258</v>
+      </c>
+      <c r="X25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28">
+        <f>C3+C5+C6+C8</f>
+        <v>2118585</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29">
+        <f>G8+G10+G11+G13</f>
+        <v>444786</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <f>AA3+AA5+AA6+AA8+AA10</f>
+        <v>106969</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31">
+        <f>C2+C9+C10+C11+C13+B36</f>
+        <v>135517</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32">
+        <f>G7+G9+G12+G16+G17</f>
+        <v>39116</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33">
+        <f>AA2+AA4+AA7+AA11+AA12+AA14</f>
+        <v>12063</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <f>C16</f>
+        <v>5255</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <f>C11+G15+AA13</f>
+        <v>975</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <f>C12</f>
+        <v>1027</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38">
+        <f>AA9</f>
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <f>AA10</f>
+        <v>303</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -6408,7 +9497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL25"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Saturn/Spacecraft mass documents.  Added Apollo 11 masses to launch scn.
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="64">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -251,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -259,15 +259,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +663,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -584,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3536,86 +3625,86 @@
       </c>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <f>C3+C5+C6+C8</f>
         <v>2120631</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="8">
         <f>G8+G10+G11+G13</f>
         <v>442658</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="8">
         <f>AA3+AA5+AA6+AA8+AA10</f>
         <v>107240</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="8">
         <f>C2+C9+C10+C11+C13+B36</f>
         <v>132596</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="8">
         <f>G7+G9+G12+G16+G17</f>
         <v>37048</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="8">
         <f>AA2+AA4+AA7+AA11+AA12+AA14</f>
         <v>11688</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="11">
         <f>C16</f>
         <v>5206</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3677,8 +3766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6632,86 +6721,86 @@
       </c>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <f>C3+C5+C6+C8</f>
         <v>2118585</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="8">
         <f>G8+G10+G11+G13</f>
         <v>444786</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="8">
         <f>AA3+AA5+AA6+AA8+AA10</f>
         <v>106969</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="8">
         <f>C2+C9+C10+C11+C13+B36</f>
         <v>135517</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="8">
         <f>G7+G9+G12+G16+G17</f>
         <v>39116</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="8">
         <f>AA2+AA4+AA7+AA11+AA12+AA14</f>
         <v>12063</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="11">
         <f>C16</f>
         <v>5255</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6773,8 +6862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9360,86 +9449,86 @@
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <f>C3+C5+C6+C8</f>
         <v>2121638</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="8">
         <f>G8+G10+G11+G13</f>
         <v>443987</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="8">
         <f>AA3+AA5+AA6+AA8+AA10</f>
         <v>106017</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="8">
         <f>C2+C9+C10+C11+C13+B36</f>
         <v>135734</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="8">
         <f>G7+G9+G12+G16+G17</f>
         <v>39133</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="8">
         <f>AA2+AA4+AA7+AA11+AA12+AA14</f>
         <v>11795</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="11">
         <f>C16</f>
         <v>5258</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -9499,10 +9588,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL25"/>
+  <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11133,7 +11222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -11231,7 +11320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -11349,7 +11438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -11417,7 +11506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -11455,7 +11544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -11493,7 +11582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -11531,7 +11620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -11569,7 +11658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>20</v>
       </c>
@@ -11601,7 +11690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>21</v>
       </c>
@@ -11630,6 +11719,138 @@
         <v>21</v>
       </c>
       <c r="X25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="5">
+        <f>C3+C5+C6+C8</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="8">
+        <f>G8+G10+G11+G13</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="8">
+        <f>AA3+AA5+AA6+AA8+AA10</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="8">
+        <f>C2+C9+C10+C11+C13+B36</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="8">
+        <f>G7+G9+G12+G16+G17</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="8">
+        <f>AA2+AA4+AA7+AA11+AA12+AA14</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="11">
+        <f>C16</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <f>C11+G15+AA13</f>
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <f>C12</f>
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38">
+        <f>AA9</f>
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <f>AA10</f>
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Spacecraft Masses To Individual Missions
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 11" sheetId="5" r:id="rId1"/>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,8 +3766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C34"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6862,8 +6862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD39"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9590,8 +9590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9610,7 +9610,7 @@
     <col min="34" max="34" width="17.28515625" customWidth="1"/>
     <col min="38" max="38" width="17.28515625" customWidth="1"/>
     <col min="42" max="42" width="17.28515625" customWidth="1"/>
-    <col min="45" max="45" width="20.5703125" customWidth="1"/>
+    <col min="45" max="45" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="17.28515625" customWidth="1"/>
     <col min="50" max="50" width="17.28515625" customWidth="1"/>
     <col min="54" max="54" width="17.28515625" customWidth="1"/>
@@ -9692,7 +9692,7 @@
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="AT1" s="2" t="s">
         <v>40</v>
@@ -9728,12 +9728,18 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>138451</v>
+      </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
       </c>
+      <c r="G2">
+        <v>654</v>
+      </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
@@ -9764,59 +9770,89 @@
       <c r="Z2" t="s">
         <v>44</v>
       </c>
+      <c r="AA2">
+        <v>11760</v>
+      </c>
       <c r="AB2" t="s">
         <v>13</v>
       </c>
       <c r="AD2" t="s">
         <v>44</v>
       </c>
+      <c r="AE2">
+        <v>11736</v>
+      </c>
       <c r="AF2" t="s">
         <v>13</v>
       </c>
       <c r="AH2" t="s">
         <v>44</v>
       </c>
+      <c r="AI2">
+        <v>11736</v>
+      </c>
       <c r="AJ2" t="s">
         <v>13</v>
       </c>
       <c r="AL2" t="s">
         <v>44</v>
       </c>
+      <c r="AM2">
+        <v>11673</v>
+      </c>
       <c r="AN2" t="s">
         <v>13</v>
       </c>
       <c r="AP2" t="s">
         <v>44</v>
       </c>
+      <c r="AQ2">
+        <v>11673</v>
+      </c>
       <c r="AR2" t="s">
         <v>13</v>
       </c>
       <c r="AT2" t="s">
         <v>44</v>
       </c>
+      <c r="AU2">
+        <v>11673</v>
+      </c>
       <c r="AV2" t="s">
         <v>13</v>
       </c>
       <c r="AX2" t="s">
         <v>44</v>
       </c>
+      <c r="AY2">
+        <v>11673</v>
+      </c>
       <c r="AZ2" t="s">
         <v>13</v>
       </c>
       <c r="BB2" t="s">
         <v>44</v>
       </c>
+      <c r="BC2">
+        <v>11673</v>
+      </c>
       <c r="BD2" t="s">
         <v>13</v>
       </c>
       <c r="BF2" t="s">
         <v>44</v>
       </c>
+      <c r="BG2">
+        <v>11673</v>
+      </c>
       <c r="BH2" t="s">
         <v>13</v>
       </c>
       <c r="BJ2" t="s">
         <v>44</v>
+      </c>
+      <c r="BK2">
+        <v>11673</v>
       </c>
       <c r="BL2" t="s">
         <v>13</v>
@@ -9826,24 +9862,36 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>1397925</v>
+      </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
       </c>
+      <c r="G3">
+        <v>4376</v>
+      </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
+      <c r="K3">
+        <v>4376</v>
+      </c>
       <c r="L3" t="s">
         <v>13</v>
       </c>
       <c r="N3" t="s">
         <v>29</v>
       </c>
+      <c r="O3">
+        <v>4376</v>
+      </c>
       <c r="P3" t="s">
         <v>13</v>
       </c>
@@ -9862,59 +9910,89 @@
       <c r="Z3" t="s">
         <v>1</v>
       </c>
+      <c r="AA3">
+        <v>87304</v>
+      </c>
       <c r="AB3" t="s">
         <v>13</v>
       </c>
       <c r="AD3" t="s">
         <v>1</v>
       </c>
+      <c r="AE3">
+        <v>87304</v>
+      </c>
       <c r="AF3" t="s">
         <v>13</v>
       </c>
       <c r="AH3" t="s">
         <v>1</v>
       </c>
+      <c r="AI3">
+        <v>87170</v>
+      </c>
       <c r="AJ3" t="s">
         <v>13</v>
       </c>
       <c r="AL3" t="s">
         <v>1</v>
       </c>
+      <c r="AM3">
+        <v>59794</v>
+      </c>
       <c r="AN3" t="s">
         <v>13</v>
       </c>
       <c r="AP3" t="s">
         <v>1</v>
       </c>
+      <c r="AQ3">
+        <v>59732</v>
+      </c>
       <c r="AR3" t="s">
         <v>13</v>
       </c>
       <c r="AT3" t="s">
         <v>1</v>
       </c>
+      <c r="AU3">
+        <v>59696</v>
+      </c>
       <c r="AV3" t="s">
         <v>13</v>
       </c>
       <c r="AX3" t="s">
         <v>1</v>
       </c>
+      <c r="AY3">
+        <v>59562</v>
+      </c>
       <c r="AZ3" t="s">
         <v>13</v>
       </c>
       <c r="BB3" t="s">
         <v>1</v>
       </c>
+      <c r="BC3">
+        <v>3478</v>
+      </c>
       <c r="BD3" t="s">
         <v>13</v>
       </c>
       <c r="BF3" t="s">
         <v>1</v>
       </c>
+      <c r="BG3">
+        <v>3416</v>
+      </c>
       <c r="BH3" t="s">
         <v>13</v>
       </c>
       <c r="BJ3" t="s">
         <v>1</v>
+      </c>
+      <c r="BK3">
+        <v>3416</v>
       </c>
       <c r="BL3" t="s">
         <v>13</v>
@@ -9924,18 +10002,27 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>20928</v>
+      </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>611</v>
+      </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
       </c>
+      <c r="K4">
+        <v>300</v>
+      </c>
       <c r="L4" t="s">
         <v>13</v>
       </c>
@@ -9960,59 +10047,89 @@
       <c r="Z4" t="s">
         <v>2</v>
       </c>
+      <c r="AA4">
+        <v>166</v>
+      </c>
       <c r="AB4" t="s">
         <v>13</v>
       </c>
       <c r="AD4" t="s">
         <v>2</v>
       </c>
+      <c r="AE4">
+        <v>166</v>
+      </c>
       <c r="AF4" t="s">
         <v>13</v>
       </c>
       <c r="AH4" t="s">
         <v>2</v>
       </c>
+      <c r="AI4">
+        <v>180</v>
+      </c>
       <c r="AJ4" t="s">
         <v>13</v>
       </c>
       <c r="AL4" t="s">
         <v>2</v>
       </c>
+      <c r="AM4">
+        <v>180</v>
+      </c>
       <c r="AN4" t="s">
         <v>13</v>
       </c>
       <c r="AP4" t="s">
         <v>2</v>
       </c>
+      <c r="AQ4">
+        <v>180</v>
+      </c>
       <c r="AR4" t="s">
         <v>13</v>
       </c>
       <c r="AT4" t="s">
         <v>2</v>
       </c>
+      <c r="AU4">
+        <v>166</v>
+      </c>
       <c r="AV4" t="s">
         <v>13</v>
       </c>
       <c r="AX4" t="s">
         <v>2</v>
       </c>
+      <c r="AY4">
+        <v>180</v>
+      </c>
       <c r="AZ4" t="s">
         <v>13</v>
       </c>
       <c r="BB4" t="s">
         <v>2</v>
       </c>
+      <c r="BC4">
+        <v>180</v>
+      </c>
       <c r="BD4" t="s">
         <v>13</v>
       </c>
       <c r="BF4" t="s">
         <v>2</v>
       </c>
+      <c r="BG4">
+        <v>180</v>
+      </c>
       <c r="BH4" t="s">
         <v>13</v>
       </c>
       <c r="BJ4" t="s">
         <v>2</v>
+      </c>
+      <c r="BK4">
+        <v>166</v>
       </c>
       <c r="BL4" t="s">
         <v>13</v>
@@ -10022,6 +10139,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5">
+        <v>498</v>
+      </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
@@ -10030,7 +10150,7 @@
       </c>
       <c r="G5">
         <f>SUM(G2:G4)</f>
-        <v>0</v>
+        <v>5641</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -10040,7 +10160,7 @@
       </c>
       <c r="K5">
         <f>SUM(K2:K4)</f>
-        <v>0</v>
+        <v>4676</v>
       </c>
       <c r="L5" t="s">
         <v>13</v>
@@ -10050,7 +10170,7 @@
       </c>
       <c r="O5">
         <f>SUM(O2:O4)</f>
-        <v>0</v>
+        <v>4376</v>
       </c>
       <c r="P5" t="s">
         <v>13</v>
@@ -10078,59 +10198,89 @@
       <c r="Z5" t="s">
         <v>3</v>
       </c>
+      <c r="AA5">
+        <v>19</v>
+      </c>
       <c r="AB5" t="s">
         <v>13</v>
       </c>
       <c r="AD5" t="s">
         <v>3</v>
       </c>
+      <c r="AE5">
+        <v>19</v>
+      </c>
       <c r="AF5" t="s">
         <v>13</v>
       </c>
       <c r="AH5" t="s">
         <v>3</v>
       </c>
+      <c r="AI5">
+        <v>20</v>
+      </c>
       <c r="AJ5" t="s">
         <v>13</v>
       </c>
       <c r="AL5" t="s">
         <v>3</v>
       </c>
+      <c r="AM5">
+        <v>108</v>
+      </c>
       <c r="AN5" t="s">
         <v>13</v>
       </c>
       <c r="AP5" t="s">
         <v>3</v>
       </c>
+      <c r="AQ5">
+        <v>108</v>
+      </c>
       <c r="AR5" t="s">
         <v>13</v>
       </c>
       <c r="AT5" t="s">
         <v>3</v>
       </c>
+      <c r="AU5">
+        <v>140</v>
+      </c>
       <c r="AV5" t="s">
         <v>13</v>
       </c>
       <c r="AX5" t="s">
         <v>3</v>
       </c>
+      <c r="AY5">
+        <v>141</v>
+      </c>
       <c r="AZ5" t="s">
         <v>13</v>
       </c>
       <c r="BB5" t="s">
         <v>3</v>
       </c>
+      <c r="BC5">
+        <v>255</v>
+      </c>
       <c r="BD5" t="s">
         <v>13</v>
       </c>
       <c r="BF5" t="s">
         <v>3</v>
       </c>
+      <c r="BG5">
+        <v>256</v>
+      </c>
       <c r="BH5" t="s">
         <v>13</v>
       </c>
       <c r="BJ5" t="s">
         <v>3</v>
+      </c>
+      <c r="BK5">
+        <v>256</v>
       </c>
       <c r="BL5" t="s">
         <v>13</v>
@@ -10140,65 +10290,98 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="C6">
+        <v>611441</v>
+      </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="Z6" t="s">
         <v>32</v>
       </c>
+      <c r="AA6">
+        <v>19662</v>
+      </c>
       <c r="AB6" t="s">
         <v>13</v>
       </c>
       <c r="AD6" t="s">
         <v>32</v>
       </c>
+      <c r="AE6">
+        <v>19657</v>
+      </c>
       <c r="AF6" t="s">
         <v>13</v>
       </c>
       <c r="AH6" t="s">
         <v>32</v>
       </c>
+      <c r="AI6">
+        <v>19607</v>
+      </c>
       <c r="AJ6" t="s">
         <v>13</v>
       </c>
       <c r="AL6" t="s">
         <v>32</v>
       </c>
+      <c r="AM6">
+        <v>13889</v>
+      </c>
       <c r="AN6" t="s">
         <v>13</v>
       </c>
       <c r="AP6" t="s">
         <v>32</v>
       </c>
+      <c r="AQ6">
+        <v>13877</v>
+      </c>
       <c r="AR6" t="s">
         <v>13</v>
       </c>
       <c r="AT6" t="s">
         <v>32</v>
       </c>
+      <c r="AU6">
+        <v>12837</v>
+      </c>
       <c r="AV6" t="s">
         <v>13</v>
       </c>
       <c r="AX6" t="s">
         <v>32</v>
       </c>
+      <c r="AY6">
+        <v>12784</v>
+      </c>
       <c r="AZ6" t="s">
         <v>13</v>
       </c>
       <c r="BB6" t="s">
         <v>32</v>
       </c>
+      <c r="BC6">
+        <v>1225</v>
+      </c>
       <c r="BD6" t="s">
         <v>13</v>
       </c>
       <c r="BF6" t="s">
         <v>32</v>
       </c>
+      <c r="BG6">
+        <v>1213</v>
+      </c>
       <c r="BH6" t="s">
         <v>13</v>
       </c>
       <c r="BJ6" t="s">
         <v>32</v>
+      </c>
+      <c r="BK6">
+        <v>1213</v>
       </c>
       <c r="BL6" t="s">
         <v>13</v>
@@ -10208,95 +10391,143 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
+      <c r="C7">
+        <v>6372</v>
+      </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>31</v>
       </c>
+      <c r="G7">
+        <v>40143</v>
+      </c>
       <c r="H7" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
         <v>31</v>
       </c>
+      <c r="K7">
+        <v>40143</v>
+      </c>
       <c r="L7" t="s">
         <v>13</v>
       </c>
       <c r="N7" t="s">
         <v>31</v>
       </c>
+      <c r="O7">
+        <v>40143</v>
+      </c>
       <c r="P7" t="s">
         <v>13</v>
       </c>
       <c r="R7" t="s">
         <v>31</v>
       </c>
+      <c r="S7">
+        <v>40143</v>
+      </c>
       <c r="T7" t="s">
         <v>13</v>
       </c>
       <c r="V7" t="s">
         <v>31</v>
       </c>
+      <c r="W7">
+        <v>40143</v>
+      </c>
       <c r="X7" t="s">
         <v>13</v>
       </c>
       <c r="Z7" t="s">
         <v>33</v>
       </c>
+      <c r="AA7">
+        <v>22</v>
+      </c>
       <c r="AB7" t="s">
         <v>13</v>
       </c>
       <c r="AD7" t="s">
         <v>33</v>
       </c>
+      <c r="AE7">
+        <v>26</v>
+      </c>
       <c r="AF7" t="s">
         <v>13</v>
       </c>
       <c r="AH7" t="s">
         <v>33</v>
       </c>
+      <c r="AI7">
+        <v>26</v>
+      </c>
       <c r="AJ7" t="s">
         <v>13</v>
       </c>
       <c r="AL7" t="s">
         <v>33</v>
       </c>
+      <c r="AM7">
+        <v>26</v>
+      </c>
       <c r="AN7" t="s">
         <v>13</v>
       </c>
       <c r="AP7" t="s">
         <v>33</v>
       </c>
+      <c r="AQ7">
+        <v>26</v>
+      </c>
       <c r="AR7" t="s">
         <v>13</v>
       </c>
       <c r="AT7" t="s">
         <v>33</v>
       </c>
+      <c r="AU7">
+        <v>26</v>
+      </c>
       <c r="AV7" t="s">
         <v>13</v>
       </c>
       <c r="AX7" t="s">
         <v>33</v>
       </c>
+      <c r="AY7">
+        <v>26</v>
+      </c>
       <c r="AZ7" t="s">
         <v>13</v>
       </c>
       <c r="BB7" t="s">
         <v>33</v>
       </c>
+      <c r="BC7">
+        <v>26</v>
+      </c>
       <c r="BD7" t="s">
         <v>13</v>
       </c>
       <c r="BF7" t="s">
         <v>33</v>
       </c>
+      <c r="BG7">
+        <v>26</v>
+      </c>
       <c r="BH7" t="s">
         <v>13</v>
       </c>
       <c r="BJ7" t="s">
         <v>33</v>
+      </c>
+      <c r="BK7">
+        <v>22</v>
       </c>
       <c r="BL7" t="s">
         <v>13</v>
@@ -10306,95 +10537,143 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
+      <c r="C8">
+        <v>99</v>
+      </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
+      <c r="G8">
+        <v>359322</v>
+      </c>
       <c r="H8" t="s">
         <v>13</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
       </c>
+      <c r="K8">
+        <v>359322</v>
+      </c>
       <c r="L8" t="s">
         <v>13</v>
       </c>
       <c r="N8" t="s">
         <v>1</v>
       </c>
+      <c r="O8">
+        <v>359006</v>
+      </c>
       <c r="P8" t="s">
         <v>13</v>
       </c>
       <c r="R8" t="s">
         <v>1</v>
       </c>
+      <c r="S8">
+        <v>1544</v>
+      </c>
       <c r="T8" t="s">
         <v>13</v>
       </c>
       <c r="V8" t="s">
         <v>1</v>
       </c>
+      <c r="W8">
+        <v>1396</v>
+      </c>
       <c r="X8" t="s">
         <v>13</v>
       </c>
       <c r="Z8" t="s">
         <v>34</v>
       </c>
+      <c r="AA8">
+        <v>7</v>
+      </c>
       <c r="AB8" t="s">
         <v>13</v>
       </c>
       <c r="AD8" t="s">
         <v>34</v>
       </c>
+      <c r="AE8">
+        <v>7</v>
+      </c>
       <c r="AF8" t="s">
         <v>13</v>
       </c>
       <c r="AH8" t="s">
         <v>34</v>
       </c>
+      <c r="AI8">
+        <v>8</v>
+      </c>
       <c r="AJ8" t="s">
         <v>13</v>
       </c>
       <c r="AL8" t="s">
         <v>34</v>
       </c>
+      <c r="AM8">
+        <v>50</v>
+      </c>
       <c r="AN8" t="s">
         <v>13</v>
       </c>
       <c r="AP8" t="s">
         <v>34</v>
       </c>
+      <c r="AQ8">
+        <v>50</v>
+      </c>
       <c r="AR8" t="s">
         <v>13</v>
       </c>
       <c r="AT8" t="s">
         <v>34</v>
       </c>
+      <c r="AU8">
+        <v>107</v>
+      </c>
       <c r="AV8" t="s">
         <v>13</v>
       </c>
       <c r="AX8" t="s">
         <v>34</v>
       </c>
+      <c r="AY8">
+        <v>109</v>
+      </c>
       <c r="AZ8" t="s">
         <v>13</v>
       </c>
       <c r="BB8" t="s">
         <v>34</v>
       </c>
+      <c r="BC8">
+        <v>195</v>
+      </c>
       <c r="BD8" t="s">
         <v>13</v>
       </c>
       <c r="BF8" t="s">
         <v>34</v>
       </c>
+      <c r="BG8">
+        <v>195</v>
+      </c>
       <c r="BH8" t="s">
         <v>13</v>
       </c>
       <c r="BJ8" t="s">
         <v>34</v>
+      </c>
+      <c r="BK8">
+        <v>195</v>
       </c>
       <c r="BL8" t="s">
         <v>13</v>
@@ -10404,48 +10683,72 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
         <v>2</v>
       </c>
+      <c r="G9">
+        <v>737</v>
+      </c>
       <c r="H9" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>2</v>
       </c>
+      <c r="K9">
+        <v>737</v>
+      </c>
       <c r="L9" t="s">
         <v>13</v>
       </c>
       <c r="N9" t="s">
         <v>2</v>
       </c>
+      <c r="O9">
+        <v>800</v>
+      </c>
       <c r="P9" t="s">
         <v>13</v>
       </c>
       <c r="R9" t="s">
         <v>2</v>
       </c>
+      <c r="S9">
+        <v>800</v>
+      </c>
       <c r="T9" t="s">
         <v>13</v>
       </c>
       <c r="V9" t="s">
         <v>2</v>
       </c>
+      <c r="W9">
+        <v>800</v>
+      </c>
       <c r="X9" t="s">
         <v>13</v>
       </c>
       <c r="Z9" t="s">
         <v>45</v>
       </c>
+      <c r="AA9">
+        <v>54</v>
+      </c>
       <c r="AB9" t="s">
         <v>13</v>
       </c>
       <c r="AD9" t="s">
         <v>45</v>
       </c>
+      <c r="AE9">
+        <v>9</v>
+      </c>
       <c r="AF9" t="s">
         <v>13</v>
       </c>
@@ -10469,6 +10772,9 @@
       </c>
       <c r="AT9" t="s">
         <v>45</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
       </c>
       <c r="AV9" t="s">
         <v>13</v>
@@ -10502,95 +10808,143 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
+      <c r="C10">
+        <v>288</v>
+      </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
+      <c r="G10">
+        <v>240</v>
+      </c>
       <c r="H10" t="s">
         <v>13</v>
       </c>
       <c r="J10" t="s">
         <v>3</v>
       </c>
+      <c r="K10">
+        <v>240</v>
+      </c>
       <c r="L10" t="s">
         <v>13</v>
       </c>
       <c r="N10" t="s">
         <v>3</v>
       </c>
+      <c r="O10">
+        <v>244</v>
+      </c>
       <c r="P10" t="s">
         <v>13</v>
       </c>
       <c r="R10" t="s">
         <v>3</v>
       </c>
+      <c r="S10">
+        <v>1882</v>
+      </c>
       <c r="T10" t="s">
         <v>13</v>
       </c>
       <c r="V10" t="s">
         <v>3</v>
       </c>
+      <c r="W10">
+        <v>1882</v>
+      </c>
       <c r="X10" t="s">
         <v>13</v>
       </c>
       <c r="Z10" t="s">
         <v>46</v>
       </c>
+      <c r="AA10">
+        <v>289</v>
+      </c>
       <c r="AB10" t="s">
         <v>13</v>
       </c>
       <c r="AD10" t="s">
         <v>46</v>
       </c>
+      <c r="AE10">
+        <v>289</v>
+      </c>
       <c r="AF10" t="s">
         <v>13</v>
       </c>
       <c r="AH10" t="s">
         <v>46</v>
       </c>
+      <c r="AI10">
+        <v>289</v>
+      </c>
       <c r="AJ10" t="s">
         <v>13</v>
       </c>
       <c r="AL10" t="s">
         <v>46</v>
       </c>
+      <c r="AM10">
+        <v>288</v>
+      </c>
       <c r="AN10" t="s">
         <v>13</v>
       </c>
       <c r="AP10" t="s">
         <v>46</v>
       </c>
+      <c r="AQ10">
+        <v>288</v>
+      </c>
       <c r="AR10" t="s">
         <v>13</v>
       </c>
       <c r="AT10" t="s">
         <v>46</v>
       </c>
+      <c r="AU10">
+        <v>235</v>
+      </c>
       <c r="AV10" t="s">
         <v>13</v>
       </c>
       <c r="AX10" t="s">
         <v>46</v>
       </c>
+      <c r="AY10">
+        <v>235</v>
+      </c>
       <c r="AZ10" t="s">
         <v>13</v>
       </c>
       <c r="BB10" t="s">
         <v>46</v>
       </c>
+      <c r="BC10">
+        <v>235</v>
+      </c>
       <c r="BD10" t="s">
         <v>13</v>
       </c>
       <c r="BF10" t="s">
         <v>46</v>
       </c>
+      <c r="BG10">
+        <v>235</v>
+      </c>
       <c r="BH10" t="s">
         <v>13</v>
       </c>
       <c r="BJ10" t="s">
         <v>46</v>
+      </c>
+      <c r="BK10">
+        <v>220</v>
       </c>
       <c r="BL10" t="s">
         <v>13</v>
@@ -10600,95 +10954,143 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
+      <c r="C11">
+        <v>635</v>
+      </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
         <v>32</v>
       </c>
+      <c r="G11">
+        <v>70160</v>
+      </c>
       <c r="H11" t="s">
         <v>13</v>
       </c>
       <c r="J11" t="s">
         <v>32</v>
       </c>
+      <c r="K11">
+        <v>70160</v>
+      </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
       <c r="N11" t="s">
         <v>32</v>
       </c>
+      <c r="O11">
+        <v>69961</v>
+      </c>
       <c r="P11" t="s">
         <v>13</v>
       </c>
       <c r="R11" t="s">
         <v>32</v>
       </c>
+      <c r="S11">
+        <v>1960</v>
+      </c>
       <c r="T11" t="s">
         <v>13</v>
       </c>
       <c r="V11" t="s">
         <v>32</v>
       </c>
+      <c r="W11">
+        <v>1894</v>
+      </c>
       <c r="X11" t="s">
         <v>13</v>
       </c>
       <c r="Z11" t="s">
         <v>47</v>
       </c>
+      <c r="AA11">
+        <v>203</v>
+      </c>
       <c r="AB11" t="s">
         <v>13</v>
       </c>
       <c r="AD11" t="s">
         <v>47</v>
       </c>
+      <c r="AE11">
+        <v>203</v>
+      </c>
       <c r="AF11" t="s">
         <v>13</v>
       </c>
       <c r="AH11" t="s">
         <v>47</v>
       </c>
+      <c r="AI11">
+        <v>202</v>
+      </c>
       <c r="AJ11" t="s">
         <v>13</v>
       </c>
       <c r="AL11" t="s">
         <v>47</v>
       </c>
+      <c r="AM11">
+        <v>177</v>
+      </c>
       <c r="AN11" t="s">
         <v>13</v>
       </c>
       <c r="AP11" t="s">
         <v>47</v>
       </c>
+      <c r="AQ11">
+        <v>177</v>
+      </c>
       <c r="AR11" t="s">
         <v>13</v>
       </c>
       <c r="AT11" t="s">
         <v>47</v>
       </c>
+      <c r="AU11">
+        <v>165</v>
+      </c>
       <c r="AV11" t="s">
         <v>13</v>
       </c>
       <c r="AX11" t="s">
         <v>47</v>
       </c>
+      <c r="AY11">
+        <v>164</v>
+      </c>
       <c r="AZ11" t="s">
         <v>13</v>
       </c>
       <c r="BB11" t="s">
         <v>47</v>
       </c>
+      <c r="BC11">
+        <v>110</v>
+      </c>
       <c r="BD11" t="s">
         <v>13</v>
       </c>
       <c r="BF11" t="s">
         <v>47</v>
       </c>
+      <c r="BG11">
+        <v>110</v>
+      </c>
       <c r="BH11" t="s">
         <v>13</v>
       </c>
       <c r="BJ11" t="s">
         <v>47</v>
+      </c>
+      <c r="BK11">
+        <v>110</v>
       </c>
       <c r="BL11" t="s">
         <v>13</v>
@@ -10698,48 +11100,72 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
+      <c r="C12">
+        <v>1027</v>
+      </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
         <v>33</v>
       </c>
+      <c r="G12">
+        <v>105</v>
+      </c>
       <c r="H12" t="s">
         <v>13</v>
       </c>
       <c r="J12" t="s">
         <v>33</v>
       </c>
+      <c r="K12">
+        <v>105</v>
+      </c>
       <c r="L12" t="s">
         <v>13</v>
       </c>
       <c r="N12" t="s">
         <v>33</v>
       </c>
+      <c r="O12">
+        <v>128</v>
+      </c>
       <c r="P12" t="s">
         <v>13</v>
       </c>
       <c r="R12" t="s">
         <v>33</v>
       </c>
+      <c r="S12">
+        <v>128</v>
+      </c>
       <c r="T12" t="s">
         <v>13</v>
       </c>
       <c r="V12" t="s">
         <v>33</v>
       </c>
+      <c r="W12">
+        <v>128</v>
+      </c>
       <c r="X12" t="s">
         <v>13</v>
       </c>
       <c r="Z12" t="s">
         <v>36</v>
       </c>
+      <c r="AA12">
+        <v>2</v>
+      </c>
       <c r="AB12" t="s">
         <v>13</v>
       </c>
       <c r="AD12" t="s">
         <v>36</v>
       </c>
+      <c r="AE12">
+        <v>2</v>
+      </c>
       <c r="AF12" t="s">
         <v>13</v>
       </c>
@@ -10763,6 +11189,9 @@
       </c>
       <c r="AT12" t="s">
         <v>36</v>
+      </c>
+      <c r="AU12">
+        <v>2</v>
       </c>
       <c r="AV12" t="s">
         <v>13</v>
@@ -10796,95 +11225,143 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
+      <c r="C13">
+        <v>239</v>
+      </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
       </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
       <c r="H13" t="s">
         <v>13</v>
       </c>
       <c r="J13" t="s">
         <v>34</v>
       </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
       <c r="L13" t="s">
         <v>13</v>
       </c>
       <c r="N13" t="s">
         <v>34</v>
       </c>
+      <c r="O13">
+        <v>102</v>
+      </c>
       <c r="P13" t="s">
         <v>13</v>
       </c>
       <c r="R13" t="s">
         <v>34</v>
       </c>
+      <c r="S13">
+        <v>576</v>
+      </c>
       <c r="T13" t="s">
         <v>13</v>
       </c>
       <c r="V13" t="s">
         <v>34</v>
       </c>
+      <c r="W13">
+        <v>576</v>
+      </c>
       <c r="X13" t="s">
         <v>13</v>
       </c>
       <c r="Z13" t="s">
         <v>9</v>
       </c>
+      <c r="AA13">
+        <v>136</v>
+      </c>
       <c r="AB13" t="s">
         <v>13</v>
       </c>
       <c r="AD13" t="s">
         <v>9</v>
       </c>
+      <c r="AE13">
+        <v>45</v>
+      </c>
       <c r="AF13" t="s">
         <v>13</v>
       </c>
       <c r="AH13" t="s">
         <v>9</v>
       </c>
+      <c r="AI13">
+        <v>45</v>
+      </c>
       <c r="AJ13" t="s">
         <v>13</v>
       </c>
       <c r="AL13" t="s">
         <v>9</v>
       </c>
+      <c r="AM13">
+        <v>45</v>
+      </c>
       <c r="AN13" t="s">
         <v>13</v>
       </c>
       <c r="AP13" t="s">
         <v>9</v>
       </c>
+      <c r="AQ13">
+        <v>45</v>
+      </c>
       <c r="AR13" t="s">
         <v>13</v>
       </c>
       <c r="AT13" t="s">
         <v>9</v>
       </c>
+      <c r="AU13">
+        <v>45</v>
+      </c>
       <c r="AV13" t="s">
         <v>13</v>
       </c>
       <c r="AX13" t="s">
         <v>9</v>
       </c>
+      <c r="AY13">
+        <v>45</v>
+      </c>
       <c r="AZ13" t="s">
         <v>13</v>
       </c>
       <c r="BB13" t="s">
         <v>9</v>
       </c>
+      <c r="BC13">
+        <v>45</v>
+      </c>
       <c r="BD13" t="s">
         <v>13</v>
       </c>
       <c r="BF13" t="s">
         <v>9</v>
       </c>
+      <c r="BG13">
+        <v>45</v>
+      </c>
       <c r="BH13" t="s">
         <v>13</v>
       </c>
       <c r="BJ13" t="s">
         <v>9</v>
+      </c>
+      <c r="BK13">
+        <v>45</v>
       </c>
       <c r="BL13" t="s">
         <v>13</v>
@@ -10896,7 +11373,7 @@
       </c>
       <c r="C14">
         <f>SUM(C2:C13)</f>
-        <v>0</v>
+        <v>2177939</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -10904,6 +11381,9 @@
       <c r="F14" t="s">
         <v>35</v>
       </c>
+      <c r="G14">
+        <v>54</v>
+      </c>
       <c r="H14" t="s">
         <v>13</v>
       </c>
@@ -10934,59 +11414,89 @@
       <c r="Z14" t="s">
         <v>11</v>
       </c>
+      <c r="AA14">
+        <v>28</v>
+      </c>
       <c r="AB14" t="s">
         <v>13</v>
       </c>
       <c r="AD14" t="s">
         <v>11</v>
       </c>
+      <c r="AE14">
+        <v>28</v>
+      </c>
       <c r="AF14" t="s">
         <v>13</v>
       </c>
       <c r="AH14" t="s">
         <v>11</v>
       </c>
+      <c r="AI14">
+        <v>28</v>
+      </c>
       <c r="AJ14" t="s">
         <v>13</v>
       </c>
       <c r="AL14" t="s">
         <v>11</v>
       </c>
+      <c r="AM14">
+        <v>28</v>
+      </c>
       <c r="AN14" t="s">
         <v>13</v>
       </c>
       <c r="AP14" t="s">
         <v>11</v>
       </c>
+      <c r="AQ14">
+        <v>28</v>
+      </c>
       <c r="AR14" t="s">
         <v>13</v>
       </c>
       <c r="AT14" t="s">
         <v>11</v>
       </c>
+      <c r="AU14">
+        <v>28</v>
+      </c>
       <c r="AV14" t="s">
         <v>13</v>
       </c>
       <c r="AX14" t="s">
         <v>11</v>
       </c>
+      <c r="AY14">
+        <v>28</v>
+      </c>
       <c r="AZ14" t="s">
         <v>13</v>
       </c>
       <c r="BB14" t="s">
         <v>11</v>
       </c>
+      <c r="BC14">
+        <v>28</v>
+      </c>
       <c r="BD14" t="s">
         <v>13</v>
       </c>
       <c r="BF14" t="s">
         <v>11</v>
       </c>
+      <c r="BG14">
+        <v>28</v>
+      </c>
       <c r="BH14" t="s">
         <v>13</v>
       </c>
       <c r="BJ14" t="s">
         <v>11</v>
+      </c>
+      <c r="BK14">
+        <v>28</v>
       </c>
       <c r="BL14" t="s">
         <v>13</v>
@@ -10996,6 +11506,9 @@
       <c r="F15" t="s">
         <v>9</v>
       </c>
+      <c r="G15">
+        <v>204</v>
+      </c>
       <c r="H15" t="s">
         <v>13</v>
       </c>
@@ -11028,7 +11541,7 @@
       </c>
       <c r="AA15">
         <f>SUM(AA2:AA14)</f>
-        <v>0</v>
+        <v>119652</v>
       </c>
       <c r="AB15" t="s">
         <v>13</v>
@@ -11038,7 +11551,7 @@
       </c>
       <c r="AE15">
         <f>SUM(AE2:AE14)</f>
-        <v>0</v>
+        <v>119491</v>
       </c>
       <c r="AF15" t="s">
         <v>13</v>
@@ -11048,7 +11561,7 @@
       </c>
       <c r="AI15">
         <f>SUM(AI2:AI14)</f>
-        <v>0</v>
+        <v>119311</v>
       </c>
       <c r="AJ15" t="s">
         <v>13</v>
@@ -11058,7 +11571,7 @@
       </c>
       <c r="AM15">
         <f>SUM(AM2:AM14)</f>
-        <v>0</v>
+        <v>86258</v>
       </c>
       <c r="AN15" t="s">
         <v>13</v>
@@ -11068,7 +11581,7 @@
       </c>
       <c r="AQ15">
         <f>SUM(AQ2:AQ14)</f>
-        <v>0</v>
+        <v>86184</v>
       </c>
       <c r="AR15" t="s">
         <v>13</v>
@@ -11078,7 +11591,7 @@
       </c>
       <c r="AU15">
         <f>SUM(AU2:AU14)</f>
-        <v>0</v>
+        <v>85120</v>
       </c>
       <c r="AV15" t="s">
         <v>13</v>
@@ -11088,7 +11601,7 @@
       </c>
       <c r="AY15">
         <f>SUM(AY2:AY14)</f>
-        <v>0</v>
+        <v>84947</v>
       </c>
       <c r="AZ15" t="s">
         <v>13</v>
@@ -11098,7 +11611,7 @@
       </c>
       <c r="BC15">
         <f>SUM(BC2:BC14)</f>
-        <v>0</v>
+        <v>17450</v>
       </c>
       <c r="BD15" t="s">
         <v>13</v>
@@ -11108,7 +11621,7 @@
       </c>
       <c r="BG15">
         <f>SUM(BG2:BG14)</f>
-        <v>0</v>
+        <v>17377</v>
       </c>
       <c r="BH15" t="s">
         <v>13</v>
@@ -11118,7 +11631,7 @@
       </c>
       <c r="BK15">
         <f>SUM(BK2:BK14)</f>
-        <v>0</v>
+        <v>17344</v>
       </c>
       <c r="BL15" t="s">
         <v>13</v>
@@ -11128,95 +11641,143 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
+      <c r="C16">
+        <v>5661</v>
+      </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>
       </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
       <c r="H16" t="s">
         <v>13</v>
       </c>
       <c r="J16" t="s">
         <v>36</v>
       </c>
+      <c r="K16">
+        <v>14</v>
+      </c>
       <c r="L16" t="s">
         <v>13</v>
       </c>
       <c r="N16" t="s">
         <v>36</v>
       </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
       <c r="P16" t="s">
         <v>13</v>
       </c>
       <c r="R16" t="s">
         <v>36</v>
       </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
       <c r="T16" t="s">
         <v>13</v>
       </c>
       <c r="V16" t="s">
         <v>36</v>
       </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
       <c r="X16" t="s">
         <v>13</v>
       </c>
       <c r="Z16" t="s">
         <v>18</v>
       </c>
+      <c r="AA16">
+        <v>2196</v>
+      </c>
       <c r="AB16" t="s">
         <v>13</v>
       </c>
       <c r="AD16" t="s">
         <v>18</v>
       </c>
+      <c r="AE16">
+        <v>2196</v>
+      </c>
       <c r="AF16" t="s">
         <v>13</v>
       </c>
       <c r="AH16" t="s">
         <v>18</v>
       </c>
+      <c r="AI16">
+        <v>2196</v>
+      </c>
       <c r="AJ16" t="s">
         <v>13</v>
       </c>
       <c r="AL16" t="s">
         <v>18</v>
       </c>
+      <c r="AM16">
+        <v>2196</v>
+      </c>
       <c r="AN16" t="s">
         <v>13</v>
       </c>
       <c r="AP16" t="s">
         <v>18</v>
       </c>
+      <c r="AQ16">
+        <v>2196</v>
+      </c>
       <c r="AR16" t="s">
         <v>13</v>
       </c>
       <c r="AT16" t="s">
         <v>18</v>
       </c>
+      <c r="AU16">
+        <v>2196</v>
+      </c>
       <c r="AV16" t="s">
         <v>13</v>
       </c>
       <c r="AX16" t="s">
         <v>18</v>
       </c>
+      <c r="AY16">
+        <v>2196</v>
+      </c>
       <c r="AZ16" t="s">
         <v>13</v>
       </c>
       <c r="BB16" t="s">
         <v>18</v>
       </c>
+      <c r="BC16">
+        <v>2196</v>
+      </c>
       <c r="BD16" t="s">
         <v>13</v>
       </c>
       <c r="BF16" t="s">
         <v>18</v>
       </c>
+      <c r="BG16">
+        <v>2196</v>
+      </c>
       <c r="BH16" t="s">
         <v>13</v>
       </c>
       <c r="BJ16" t="s">
         <v>18</v>
+      </c>
+      <c r="BK16">
+        <v>2196</v>
       </c>
       <c r="BL16" t="s">
         <v>13</v>
@@ -11226,95 +11787,143 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
+      <c r="C17">
+        <v>471114</v>
+      </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
       </c>
+      <c r="G17">
+        <v>34</v>
+      </c>
       <c r="H17" t="s">
         <v>13</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
       </c>
+      <c r="K17">
+        <v>34</v>
+      </c>
       <c r="L17" t="s">
         <v>13</v>
       </c>
       <c r="N17" t="s">
         <v>11</v>
       </c>
+      <c r="O17">
+        <v>34</v>
+      </c>
       <c r="P17" t="s">
         <v>13</v>
       </c>
       <c r="R17" t="s">
         <v>11</v>
       </c>
+      <c r="S17">
+        <v>34</v>
+      </c>
       <c r="T17" t="s">
         <v>13</v>
       </c>
       <c r="V17" t="s">
         <v>11</v>
       </c>
+      <c r="W17">
+        <v>34</v>
+      </c>
       <c r="X17" t="s">
         <v>13</v>
       </c>
       <c r="Z17" t="s">
         <v>19</v>
       </c>
+      <c r="AA17">
+        <v>43665</v>
+      </c>
       <c r="AB17" t="s">
         <v>13</v>
       </c>
       <c r="AD17" t="s">
         <v>19</v>
       </c>
+      <c r="AE17">
+        <v>39636</v>
+      </c>
       <c r="AF17" t="s">
         <v>13</v>
       </c>
       <c r="AH17" t="s">
         <v>19</v>
       </c>
+      <c r="AI17">
+        <v>39636</v>
+      </c>
       <c r="AJ17" t="s">
         <v>13</v>
       </c>
       <c r="AL17" t="s">
         <v>19</v>
       </c>
+      <c r="AM17">
+        <v>39636</v>
+      </c>
       <c r="AN17" t="s">
         <v>13</v>
       </c>
       <c r="AP17" t="s">
         <v>19</v>
       </c>
+      <c r="AQ17">
+        <v>39636</v>
+      </c>
       <c r="AR17" t="s">
         <v>13</v>
       </c>
       <c r="AT17" t="s">
         <v>19</v>
       </c>
+      <c r="AU17">
+        <v>39636</v>
+      </c>
       <c r="AV17" t="s">
         <v>13</v>
       </c>
       <c r="AX17" t="s">
         <v>19</v>
       </c>
+      <c r="AY17">
+        <v>39636</v>
+      </c>
       <c r="AZ17" t="s">
         <v>13</v>
       </c>
       <c r="BB17" t="s">
         <v>19</v>
       </c>
+      <c r="BC17">
+        <v>39636</v>
+      </c>
       <c r="BD17" t="s">
         <v>13</v>
       </c>
       <c r="BF17" t="s">
         <v>19</v>
       </c>
+      <c r="BG17">
+        <v>39636</v>
+      </c>
       <c r="BH17" t="s">
         <v>13</v>
       </c>
       <c r="BJ17" t="s">
         <v>19</v>
+      </c>
+      <c r="BK17">
+        <v>9687</v>
       </c>
       <c r="BL17" t="s">
         <v>13</v>
@@ -11324,6 +11933,9 @@
       <c r="B18" t="s">
         <v>16</v>
       </c>
+      <c r="C18">
+        <v>3960</v>
+      </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -11332,7 +11944,7 @@
       </c>
       <c r="G18">
         <f>SUM(G7:G17)</f>
-        <v>0</v>
+        <v>471113</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -11342,7 +11954,7 @@
       </c>
       <c r="K18">
         <f>SUM(K7:K17)</f>
-        <v>0</v>
+        <v>470855</v>
       </c>
       <c r="L18" t="s">
         <v>13</v>
@@ -11352,7 +11964,7 @@
       </c>
       <c r="O18">
         <f>SUM(O7:O17)</f>
-        <v>0</v>
+        <v>470420</v>
       </c>
       <c r="P18" t="s">
         <v>13</v>
@@ -11362,7 +11974,7 @@
       </c>
       <c r="S18">
         <f>SUM(S7:S17)</f>
-        <v>0</v>
+        <v>47069</v>
       </c>
       <c r="T18" t="s">
         <v>13</v>
@@ -11372,7 +11984,7 @@
       </c>
       <c r="W18">
         <f>SUM(W7:W17)</f>
-        <v>0</v>
+        <v>46855</v>
       </c>
       <c r="X18" t="s">
         <v>13</v>
@@ -11380,59 +11992,89 @@
       <c r="Z18" t="s">
         <v>20</v>
       </c>
+      <c r="AA18">
+        <v>45865</v>
+      </c>
       <c r="AB18" t="s">
         <v>13</v>
       </c>
       <c r="AD18" t="s">
         <v>20</v>
       </c>
+      <c r="AE18">
+        <v>41832</v>
+      </c>
       <c r="AF18" t="s">
         <v>13</v>
       </c>
       <c r="AH18" t="s">
         <v>20</v>
       </c>
+      <c r="AI18">
+        <v>41832</v>
+      </c>
       <c r="AJ18" t="s">
         <v>13</v>
       </c>
       <c r="AL18" t="s">
         <v>20</v>
       </c>
+      <c r="AM18">
+        <v>41832</v>
+      </c>
       <c r="AN18" t="s">
         <v>13</v>
       </c>
       <c r="AP18" t="s">
         <v>20</v>
       </c>
+      <c r="AQ18">
+        <v>41832</v>
+      </c>
       <c r="AR18" t="s">
         <v>13</v>
       </c>
       <c r="AT18" t="s">
         <v>20</v>
       </c>
+      <c r="AU18">
+        <v>41832</v>
+      </c>
       <c r="AV18" t="s">
         <v>13</v>
       </c>
       <c r="AX18" t="s">
         <v>20</v>
       </c>
+      <c r="AY18">
+        <v>41832</v>
+      </c>
       <c r="AZ18" t="s">
         <v>13</v>
       </c>
       <c r="BB18" t="s">
         <v>20</v>
       </c>
+      <c r="BC18">
+        <v>41832</v>
+      </c>
       <c r="BD18" t="s">
         <v>13</v>
       </c>
       <c r="BF18" t="s">
         <v>20</v>
       </c>
+      <c r="BG18">
+        <v>41832</v>
+      </c>
       <c r="BH18" t="s">
         <v>13</v>
       </c>
       <c r="BJ18" t="s">
         <v>20</v>
+      </c>
+      <c r="BK18">
+        <v>11863</v>
       </c>
       <c r="BL18" t="s">
         <v>13</v>
@@ -11442,65 +12084,98 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
+      <c r="C19">
+        <v>119652</v>
+      </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="Z19" t="s">
         <v>21</v>
       </c>
+      <c r="AA19">
+        <v>165516</v>
+      </c>
       <c r="AB19" t="s">
         <v>13</v>
       </c>
       <c r="AD19" t="s">
         <v>21</v>
       </c>
+      <c r="AE19">
+        <v>161324</v>
+      </c>
       <c r="AF19" t="s">
         <v>13</v>
       </c>
       <c r="AH19" t="s">
         <v>21</v>
       </c>
+      <c r="AI19">
+        <v>161143</v>
+      </c>
       <c r="AJ19" t="s">
         <v>13</v>
       </c>
       <c r="AL19" t="s">
         <v>21</v>
       </c>
+      <c r="AM19">
+        <v>128095</v>
+      </c>
       <c r="AN19" t="s">
         <v>13</v>
       </c>
       <c r="AP19" t="s">
         <v>21</v>
       </c>
+      <c r="AQ19">
+        <v>128021</v>
+      </c>
       <c r="AR19" t="s">
         <v>13</v>
       </c>
       <c r="AT19" t="s">
         <v>21</v>
       </c>
+      <c r="AU19">
+        <v>126953</v>
+      </c>
       <c r="AV19" t="s">
         <v>13</v>
       </c>
       <c r="AX19" t="s">
         <v>21</v>
       </c>
+      <c r="AY19">
+        <v>126780</v>
+      </c>
       <c r="AZ19" t="s">
         <v>13</v>
       </c>
       <c r="BB19" t="s">
         <v>21</v>
       </c>
+      <c r="BC19">
+        <v>59285</v>
+      </c>
       <c r="BD19" t="s">
         <v>13</v>
       </c>
       <c r="BF19" t="s">
         <v>21</v>
       </c>
+      <c r="BG19">
+        <v>59212</v>
+      </c>
       <c r="BH19" t="s">
         <v>13</v>
       </c>
       <c r="BJ19" t="s">
         <v>21</v>
+      </c>
+      <c r="BK19">
+        <v>29210</v>
       </c>
       <c r="BL19" t="s">
         <v>13</v>
@@ -11510,35 +12185,53 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
+      <c r="C20">
+        <v>2196</v>
+      </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
       </c>
+      <c r="G20">
+        <v>3960</v>
+      </c>
       <c r="H20" t="s">
         <v>13</v>
       </c>
       <c r="J20" t="s">
         <v>16</v>
       </c>
+      <c r="K20">
+        <v>3960</v>
+      </c>
       <c r="L20" t="s">
         <v>13</v>
       </c>
       <c r="N20" t="s">
         <v>16</v>
       </c>
+      <c r="O20">
+        <v>3960</v>
+      </c>
       <c r="P20" t="s">
         <v>13</v>
       </c>
       <c r="R20" t="s">
         <v>16</v>
       </c>
+      <c r="S20">
+        <v>3960</v>
+      </c>
       <c r="T20" t="s">
         <v>13</v>
       </c>
       <c r="V20" t="s">
         <v>16</v>
+      </c>
+      <c r="W20">
+        <v>3960</v>
       </c>
       <c r="X20" t="s">
         <v>13</v>
@@ -11548,35 +12241,53 @@
       <c r="B21" t="s">
         <v>19</v>
       </c>
+      <c r="C21">
+        <v>43665</v>
+      </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
       </c>
+      <c r="G21">
+        <v>119652</v>
+      </c>
       <c r="H21" t="s">
         <v>13</v>
       </c>
       <c r="J21" t="s">
         <v>17</v>
       </c>
+      <c r="K21">
+        <v>119561</v>
+      </c>
       <c r="L21" t="s">
         <v>13</v>
       </c>
       <c r="N21" t="s">
         <v>17</v>
       </c>
+      <c r="O21">
+        <v>119561</v>
+      </c>
       <c r="P21" t="s">
         <v>13</v>
       </c>
       <c r="R21" t="s">
         <v>17</v>
       </c>
+      <c r="S21">
+        <v>119561</v>
+      </c>
       <c r="T21" t="s">
         <v>13</v>
       </c>
       <c r="V21" t="s">
         <v>17</v>
+      </c>
+      <c r="W21">
+        <v>119559</v>
       </c>
       <c r="X21" t="s">
         <v>13</v>
@@ -11586,35 +12297,53 @@
       <c r="B22" t="s">
         <v>20</v>
       </c>
+      <c r="C22">
+        <v>640590</v>
+      </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="F22" t="s">
         <v>18</v>
       </c>
+      <c r="G22">
+        <v>2196</v>
+      </c>
       <c r="H22" t="s">
         <v>13</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
       </c>
+      <c r="K22">
+        <v>2196</v>
+      </c>
       <c r="L22" t="s">
         <v>13</v>
       </c>
       <c r="N22" t="s">
         <v>18</v>
       </c>
+      <c r="O22">
+        <v>2196</v>
+      </c>
       <c r="P22" t="s">
         <v>13</v>
       </c>
       <c r="R22" t="s">
         <v>18</v>
       </c>
+      <c r="S22">
+        <v>2196</v>
+      </c>
       <c r="T22" t="s">
         <v>13</v>
       </c>
       <c r="V22" t="s">
         <v>18</v>
+      </c>
+      <c r="W22">
+        <v>2196</v>
       </c>
       <c r="X22" t="s">
         <v>13</v>
@@ -11624,35 +12353,53 @@
       <c r="B23" t="s">
         <v>21</v>
       </c>
+      <c r="C23">
+        <v>2822171</v>
+      </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="F23" t="s">
         <v>19</v>
       </c>
+      <c r="G23">
+        <v>43665</v>
+      </c>
       <c r="H23" t="s">
         <v>13</v>
       </c>
       <c r="J23" t="s">
         <v>19</v>
       </c>
+      <c r="K23">
+        <v>43665</v>
+      </c>
       <c r="L23" t="s">
         <v>13</v>
       </c>
       <c r="N23" t="s">
         <v>19</v>
       </c>
+      <c r="O23">
+        <v>43665</v>
+      </c>
       <c r="P23" t="s">
         <v>13</v>
       </c>
       <c r="R23" t="s">
         <v>19</v>
       </c>
+      <c r="S23">
+        <v>39636</v>
+      </c>
       <c r="T23" t="s">
         <v>13</v>
       </c>
       <c r="V23" t="s">
         <v>19</v>
+      </c>
+      <c r="W23">
+        <v>39636</v>
       </c>
       <c r="X23" t="s">
         <v>13</v>
@@ -11662,29 +12409,44 @@
       <c r="F24" t="s">
         <v>20</v>
       </c>
+      <c r="G24">
+        <v>169477</v>
+      </c>
       <c r="H24" t="s">
         <v>13</v>
       </c>
       <c r="J24" t="s">
         <v>20</v>
       </c>
+      <c r="K24">
+        <v>169386</v>
+      </c>
       <c r="L24" t="s">
         <v>13</v>
       </c>
       <c r="N24" t="s">
         <v>20</v>
       </c>
+      <c r="O24">
+        <v>169386</v>
+      </c>
       <c r="P24" t="s">
         <v>13</v>
       </c>
       <c r="R24" t="s">
         <v>20</v>
       </c>
+      <c r="S24">
+        <v>165353</v>
+      </c>
       <c r="T24" t="s">
         <v>13</v>
       </c>
       <c r="V24" t="s">
         <v>20</v>
+      </c>
+      <c r="W24">
+        <v>165351</v>
       </c>
       <c r="X24" t="s">
         <v>13</v>
@@ -11694,29 +12456,44 @@
       <c r="F25" t="s">
         <v>21</v>
       </c>
+      <c r="G25">
+        <v>646231</v>
+      </c>
       <c r="H25" t="s">
         <v>13</v>
       </c>
       <c r="J25" t="s">
         <v>21</v>
       </c>
+      <c r="K25">
+        <v>644918</v>
+      </c>
       <c r="L25" t="s">
         <v>13</v>
       </c>
       <c r="N25" t="s">
         <v>21</v>
       </c>
+      <c r="O25">
+        <v>344182</v>
+      </c>
       <c r="P25" t="s">
         <v>13</v>
       </c>
       <c r="R25" t="s">
         <v>21</v>
       </c>
+      <c r="S25">
+        <v>212425</v>
+      </c>
       <c r="T25" t="s">
         <v>13</v>
       </c>
       <c r="V25" t="s">
         <v>21</v>
+      </c>
+      <c r="W25">
+        <v>212267</v>
       </c>
       <c r="X25" t="s">
         <v>13</v>
@@ -11728,7 +12505,7 @@
       </c>
       <c r="B28" s="5">
         <f>C3+C4+C5+C6+C7+C8</f>
-        <v>0</v>
+        <v>2037263</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>13</v>
@@ -11740,7 +12517,7 @@
       </c>
       <c r="B29" s="8">
         <f>G8+G9+G10+G11+G12+G13</f>
-        <v>0</v>
+        <v>430664</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>13</v>
@@ -11752,7 +12529,7 @@
       </c>
       <c r="B30" s="8">
         <f>AA3+AA4+AA5+AA6+AA7+AA8+AA10</f>
-        <v>0</v>
+        <v>107469</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>13</v>
@@ -11764,7 +12541,7 @@
       </c>
       <c r="B31" s="8">
         <f>C2+C9+C10+C12+C13+B36</f>
-        <v>0</v>
+        <v>141016</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -11776,7 +12553,7 @@
       </c>
       <c r="B32" s="8">
         <f>G7+G16+G17+G20</f>
-        <v>0</v>
+        <v>44151</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>13</v>
@@ -11788,7 +12565,7 @@
       </c>
       <c r="B33" s="8">
         <f>AA2+AA11+AA12+AA14+AA16</f>
-        <v>0</v>
+        <v>14189</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>13</v>
@@ -11800,7 +12577,7 @@
       </c>
       <c r="B34" s="11">
         <f>C16</f>
-        <v>0</v>
+        <v>5661</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>13</v>
@@ -11812,7 +12589,7 @@
       </c>
       <c r="B36">
         <f>C11+G15+AA13</f>
-        <v>0</v>
+        <v>975</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
@@ -11824,7 +12601,7 @@
       </c>
       <c r="B37">
         <f>C12</f>
-        <v>0</v>
+        <v>1027</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
@@ -11836,7 +12613,7 @@
       </c>
       <c r="B38">
         <f>AA9</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
@@ -11848,7 +12625,7 @@
       </c>
       <c r="B39">
         <f>AA10</f>
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Fix Insertion FC Purge Checklist, Add S-IC IECO Times, Add Sources To Mass Spreadsheets
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 11" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="65">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -215,6 +215,9 @@
   <si>
     <t>APS Prop</t>
   </si>
+  <si>
+    <t>Data From Saturn V Launch Vehicle Evaluation Report</t>
+  </si>
 </sst>
 </file>
 
@@ -237,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +250,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -357,6 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL39"/>
+  <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,6 +3766,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3764,10 +3779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL39"/>
+  <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6852,6 +6867,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6860,10 +6880,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD39"/>
+  <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9580,6 +9600,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -9588,10 +9613,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL39"/>
+  <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12631,6 +12656,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Saturn mass spreadsheet fixes, will update and then fix launch scenarios
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter 16 Beta\Doc\Project Apollo - NASSP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="7965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 11" sheetId="5" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Apollo 9" sheetId="3" r:id="rId3"/>
     <sheet name="Apollo 8" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -207,9 +212,6 @@
     <t>S4EMPTYMASS</t>
   </si>
   <si>
-    <t>S-IC Ullage Prop</t>
-  </si>
-  <si>
     <t>S-IVB Ullage Prop</t>
   </si>
   <si>
@@ -218,11 +220,14 @@
   <si>
     <t>Data From Saturn V Launch Vehicle Evaluation Report</t>
   </si>
+  <si>
+    <t>S-IC Retromotor Prop</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -673,23 +678,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -3675,8 +3680,8 @@
         <v>58</v>
       </c>
       <c r="B31" s="8">
-        <f>C2+C9+C10+C12+C13+B36</f>
-        <v>132988</v>
+        <f>C2+C9+C10+C12+C13+B36+G2</f>
+        <v>133602</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -3687,7 +3692,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="8">
-        <f>G7+G16+G17+G20</f>
+        <f>K7+K16+K17+K20</f>
         <v>39869</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -3711,8 +3716,8 @@
         <v>55</v>
       </c>
       <c r="B34" s="11">
-        <f>C16</f>
-        <v>5206</v>
+        <f>G3</f>
+        <v>3982</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>13</v>
@@ -3732,7 +3737,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <f>C12</f>
@@ -3744,7 +3749,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38">
         <f>AA9</f>
@@ -3756,7 +3761,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39">
         <f>AA10</f>
@@ -3768,7 +3773,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3778,16 +3783,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -6776,8 +6781,8 @@
         <v>58</v>
       </c>
       <c r="B31" s="8">
-        <f>C2+C9+C10+C12+C13+B36</f>
-        <v>135909</v>
+        <f>C2+C9+C10+C12+C13+B36+G2</f>
+        <v>136520</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -6788,7 +6793,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="8">
-        <f>G7+G16+G17+G20</f>
+        <f>K7+K16+K17+K20</f>
         <v>41923</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -6812,8 +6817,8 @@
         <v>55</v>
       </c>
       <c r="B34" s="11">
-        <f>C16</f>
-        <v>5255</v>
+        <f>G3</f>
+        <v>4033</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>13</v>
@@ -6833,7 +6838,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <f>C12</f>
@@ -6845,7 +6850,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38">
         <f>AA9</f>
@@ -6857,7 +6862,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39">
         <f>AA10</f>
@@ -6869,7 +6874,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6879,16 +6884,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
@@ -9509,8 +9514,8 @@
         <v>58</v>
       </c>
       <c r="B31" s="8">
-        <f>C2+C9+C10+C12+C13+B36</f>
-        <v>136126</v>
+        <f>C2+C9+C10+C12+C13+B36+G2</f>
+        <v>136740</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -9521,7 +9526,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="8">
-        <f>G7+G16+G17+G20</f>
+        <f>K7+K16+K17+K20</f>
         <v>41919</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -9545,8 +9550,8 @@
         <v>55</v>
       </c>
       <c r="B34" s="11">
-        <f>C16</f>
-        <v>5258</v>
+        <f>G3</f>
+        <v>4033</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>13</v>
@@ -9566,7 +9571,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <f>C12</f>
@@ -9578,7 +9583,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38">
         <f>AA9</f>
@@ -9590,7 +9595,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39">
         <f>AA10</f>
@@ -9602,7 +9607,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -9612,16 +9617,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
@@ -12565,8 +12570,8 @@
         <v>58</v>
       </c>
       <c r="B31" s="8">
-        <f>C2+C9+C10+C12+C13+B36</f>
-        <v>141016</v>
+        <f>C2+C9+C10+C12+C13+B36+G2</f>
+        <v>141670</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
@@ -12577,7 +12582,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="8">
-        <f>G7+G16+G17+G20</f>
+        <f>K7+K16+K17+K20</f>
         <v>44151</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -12601,8 +12606,8 @@
         <v>55</v>
       </c>
       <c r="B34" s="11">
-        <f>C16</f>
-        <v>5661</v>
+        <f>G3</f>
+        <v>4376</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>13</v>
@@ -12622,7 +12627,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <f>C12</f>
@@ -12634,7 +12639,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38">
         <f>AA9</f>
@@ -12646,7 +12651,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39">
         <f>AA10</f>
@@ -12658,7 +12663,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add totalizing sheet to mass spreadsheets
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EB8A18-48B6-48D9-A566-E9A2291F2276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF986EEC-B126-42B9-9BBA-FCAA10909E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Apollo 9" sheetId="3" r:id="rId9"/>
     <sheet name="Apollo 8" sheetId="4" r:id="rId10"/>
     <sheet name="Apollo 7" sheetId="13" r:id="rId11"/>
+    <sheet name="Totals" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7098" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7184" uniqueCount="124">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -386,12 +387,48 @@
   <si>
     <t>Data From Saturn S-IVB-505 Stage Flight Evaluation Report &amp; Launch Vehicle Evaluation Report</t>
   </si>
+  <si>
+    <t>Apollo 7</t>
+  </si>
+  <si>
+    <t>Apollo 8</t>
+  </si>
+  <si>
+    <t>Apollo 9</t>
+  </si>
+  <si>
+    <t>Apollo 10</t>
+  </si>
+  <si>
+    <t>Apollo 11</t>
+  </si>
+  <si>
+    <t>Apollo 12</t>
+  </si>
+  <si>
+    <t>Apollo 13</t>
+  </si>
+  <si>
+    <t>Apollo 14</t>
+  </si>
+  <si>
+    <t>Apollo 15</t>
+  </si>
+  <si>
+    <t>Apollo 16</t>
+  </si>
+  <si>
+    <t>Apollo 17</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,8 +444,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,8 +470,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -516,11 +583,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -536,6 +618,27 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,7 +956,7 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3918,7 +4021,7 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6971,10 +7074,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80FCE58-7FB9-4CC7-8163-D01D25C81D7D}">
-  <dimension ref="A1:AV41"/>
+  <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9598,17 +9701,24 @@
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="7"/>
+      <c r="A29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="13">
+        <f>G13+G14+G15+G16+G17+G18</f>
+        <v>105872.99508169999</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F30" s="13">
-        <f>G13+G14+G15+G16+G17+G18</f>
-        <v>105872.99508169999</v>
+        <f>C18-F28</f>
+        <v>41858.5</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>13</v>
@@ -9616,56 +9726,63 @@
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F31" s="13">
-        <f>C18-F28</f>
-        <v>41858.5</v>
+        <f>C20-F29</f>
+        <v>10483.904918300002</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="13">
-        <f>C20-F30</f>
-        <v>10483.904918300002</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A32" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="14">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="14">
         <f>C16</f>
         <v>2514.3000000000002</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G32" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="13">
+        <f>C13</f>
+        <v>453.6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="13">
+        <f>C17</f>
+        <v>481.2</v>
+      </c>
+      <c r="G35" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F36" s="13">
-        <f>C13</f>
-        <v>453.6</v>
+        <f>G3</f>
+        <v>179.16898615000002</v>
       </c>
       <c r="G36" t="s">
         <v>13</v>
@@ -9673,50 +9790,768 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="F37" s="13">
-        <f>C17</f>
-        <v>481.2</v>
-      </c>
-      <c r="G37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="13">
-        <f>G3</f>
-        <v>179.16898615000002</v>
-      </c>
-      <c r="G38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="13">
         <f>G20</f>
         <v>61.23496995</v>
       </c>
-      <c r="G39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5F06E4-4B71-4DD5-A2F8-F472E18DC771}">
+  <dimension ref="A1:AG8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2:AF8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="18" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" style="18" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" style="18" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" style="18" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" style="18" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.5703125" style="18" customWidth="1"/>
+    <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5703125" style="18" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="23"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" s="23"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="W1" s="22"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="19"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="24">
+        <f>'Apollo 7'!F28</f>
+        <v>411967.90000000008</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="26">
+        <f>'Apollo 8'!B28</f>
+        <v>2037263</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="27">
+        <f>'Apollo 9'!B28</f>
+        <v>2147080</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="26">
+        <f>'Apollo 10'!B28</f>
+        <v>2143978</v>
+      </c>
+      <c r="L2" s="20"/>
+      <c r="M2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="27">
+        <f>'Apollo 11'!B28</f>
+        <v>2146040</v>
+      </c>
+      <c r="O2" s="20"/>
+      <c r="P2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="26">
+        <f>'Apollo 12'!B28</f>
+        <v>2147768</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="T2" s="27">
+        <f>'Apollo 13'!B28</f>
+        <v>2148494</v>
+      </c>
+      <c r="U2" s="20"/>
+      <c r="V2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" s="26">
+        <f>'Apollo 14'!B28</f>
+        <v>2150893</v>
+      </c>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="27">
+        <f>'Apollo 15'!B28</f>
+        <v>2142469</v>
+      </c>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" s="26">
+        <f>'Apollo 16'!B28</f>
+        <v>2155291</v>
+      </c>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF2" s="27">
+        <f>'Apollo 17'!B28</f>
+        <v>2153110</v>
+      </c>
+      <c r="AG2" s="20"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="24">
+        <f>'Apollo 7'!F29</f>
+        <v>105872.99508169999</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="26">
+        <f>'Apollo 8'!B29</f>
+        <v>430664</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="27">
+        <f>'Apollo 9'!B29</f>
+        <v>444829</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="26">
+        <f>'Apollo 10'!B29</f>
+        <v>445628</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="27">
+        <f>'Apollo 11'!B29</f>
+        <v>443500</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="26">
+        <f>'Apollo 12'!B29</f>
+        <v>446320</v>
+      </c>
+      <c r="R3" s="20"/>
+      <c r="S3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="T3" s="27">
+        <f>'Apollo 13'!B29</f>
+        <v>452316</v>
+      </c>
+      <c r="U3" s="20"/>
+      <c r="V3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="26">
+        <f>'Apollo 14'!B29</f>
+        <v>452308</v>
+      </c>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" s="27">
+        <f>'Apollo 15'!B29</f>
+        <v>452430</v>
+      </c>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="26">
+        <f>'Apollo 16'!B29</f>
+        <v>456812</v>
+      </c>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" s="27">
+        <f>'Apollo 17'!B29</f>
+        <v>455806</v>
+      </c>
+      <c r="AG3" s="20"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="24">
+        <f>'Apollo 7'!F30</f>
+        <v>41858.5</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="26">
+        <f>'Apollo 8'!B30</f>
+        <v>107469</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="27">
+        <f>'Apollo 9'!B30</f>
+        <v>106205</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="26">
+        <f>'Apollo 10'!B30</f>
+        <v>107157</v>
+      </c>
+      <c r="L4" s="20"/>
+      <c r="M4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="27">
+        <f>'Apollo 11'!B30</f>
+        <v>107428</v>
+      </c>
+      <c r="O4" s="20"/>
+      <c r="P4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="26">
+        <f>'Apollo 12'!B30</f>
+        <v>106591</v>
+      </c>
+      <c r="R4" s="20"/>
+      <c r="S4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="27">
+        <f>'Apollo 13'!B30</f>
+        <v>107179</v>
+      </c>
+      <c r="U4" s="20"/>
+      <c r="V4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="26">
+        <f>'Apollo 14'!B30</f>
+        <v>106488</v>
+      </c>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z4" s="27">
+        <f>'Apollo 15'!B30</f>
+        <v>108958</v>
+      </c>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC4" s="26">
+        <f>'Apollo 16'!B30</f>
+        <v>108780</v>
+      </c>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF4" s="27">
+        <f>'Apollo 17'!B30</f>
+        <v>108914</v>
+      </c>
+      <c r="AG4" s="20"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="24">
+        <f>'Apollo 7'!F31</f>
+        <v>10483.904918300002</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="26">
+        <f>'Apollo 8'!B31</f>
+        <v>141670</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="27">
+        <f>'Apollo 9'!B31</f>
+        <v>136740</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="26">
+        <f>'Apollo 10'!B31</f>
+        <v>136520</v>
+      </c>
+      <c r="L5" s="20"/>
+      <c r="M5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="27">
+        <f>'Apollo 11'!B31</f>
+        <v>133602</v>
+      </c>
+      <c r="O5" s="20"/>
+      <c r="P5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="26">
+        <f>'Apollo 12'!B31</f>
+        <v>133859</v>
+      </c>
+      <c r="R5" s="20"/>
+      <c r="S5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" s="27">
+        <f>'Apollo 13'!B31</f>
+        <v>133764</v>
+      </c>
+      <c r="U5" s="20"/>
+      <c r="V5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" s="26">
+        <f>'Apollo 14'!B31</f>
+        <v>133364</v>
+      </c>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5" s="27">
+        <f>'Apollo 15'!B31</f>
+        <v>132487</v>
+      </c>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC5" s="26">
+        <f>'Apollo 16'!B31</f>
+        <v>133748</v>
+      </c>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF5" s="27">
+        <f>'Apollo 17'!B31</f>
+        <v>133521</v>
+      </c>
+      <c r="AG5" s="20"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="24">
+        <f>'Apollo 7'!F32</f>
+        <v>2514.3000000000002</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="26">
+        <f>'Apollo 8'!B32</f>
+        <v>44151</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="27">
+        <f>'Apollo 9'!B32</f>
+        <v>41919</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="26">
+        <f>'Apollo 10'!B32</f>
+        <v>41923</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="27">
+        <f>'Apollo 11'!B32</f>
+        <v>39869</v>
+      </c>
+      <c r="O6" s="20"/>
+      <c r="P6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q6" s="26">
+        <f>'Apollo 12'!B32</f>
+        <v>40081</v>
+      </c>
+      <c r="R6" s="20"/>
+      <c r="S6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="T6" s="27">
+        <f>'Apollo 13'!B32</f>
+        <v>39068</v>
+      </c>
+      <c r="U6" s="20"/>
+      <c r="V6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="W6" s="26">
+        <f>'Apollo 14'!B32</f>
+        <v>39136</v>
+      </c>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" s="27">
+        <f>'Apollo 15'!B32</f>
+        <v>39478</v>
+      </c>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC6" s="26">
+        <f>'Apollo 16'!B32</f>
+        <v>40151</v>
+      </c>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF6" s="27">
+        <f>'Apollo 17'!B32</f>
+        <v>40163</v>
+      </c>
+      <c r="AG6" s="20"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="26">
+        <f>'Apollo 8'!B33</f>
+        <v>14189</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="27">
+        <f>'Apollo 9'!B33</f>
+        <v>13549</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="26">
+        <f>'Apollo 10'!B33</f>
+        <v>13810</v>
+      </c>
+      <c r="L7" s="20"/>
+      <c r="M7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="27">
+        <f>'Apollo 11'!B33</f>
+        <v>13439</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="P7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" s="26">
+        <f>'Apollo 12'!B33</f>
+        <v>13541</v>
+      </c>
+      <c r="R7" s="20"/>
+      <c r="S7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="27">
+        <f>'Apollo 13'!B33</f>
+        <v>13786</v>
+      </c>
+      <c r="U7" s="20"/>
+      <c r="V7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="W7" s="26">
+        <f>'Apollo 14'!B33</f>
+        <v>13762</v>
+      </c>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z7" s="27">
+        <f>'Apollo 15'!B33</f>
+        <v>13828</v>
+      </c>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC7" s="26">
+        <f>'Apollo 16'!B33</f>
+        <v>13784</v>
+      </c>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF7" s="27">
+        <f>'Apollo 17'!B33</f>
+        <v>13747</v>
+      </c>
+      <c r="AG7" s="20"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="26">
+        <f>'Apollo 8'!B34</f>
+        <v>4376</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="27">
+        <f>'Apollo 9'!B34</f>
+        <v>4033</v>
+      </c>
+      <c r="I8" s="20"/>
+      <c r="J8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="26">
+        <f>'Apollo 10'!B34</f>
+        <v>4033</v>
+      </c>
+      <c r="L8" s="20"/>
+      <c r="M8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="27">
+        <f>'Apollo 11'!B34</f>
+        <v>3982</v>
+      </c>
+      <c r="O8" s="20"/>
+      <c r="P8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="26">
+        <f>'Apollo 12'!B34</f>
+        <v>3996</v>
+      </c>
+      <c r="R8" s="20"/>
+      <c r="S8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="27">
+        <f>'Apollo 13'!B34</f>
+        <v>3972</v>
+      </c>
+      <c r="U8" s="20"/>
+      <c r="V8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8" s="26">
+        <f>'Apollo 14'!B34</f>
+        <v>3945</v>
+      </c>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="27">
+        <f>'Apollo 15'!B34</f>
+        <v>3504</v>
+      </c>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC8" s="26">
+        <f>'Apollo 16'!B34</f>
+        <v>3960</v>
+      </c>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF8" s="27">
+        <f>'Apollo 17'!B34</f>
+        <v>3908</v>
+      </c>
+      <c r="AG8" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -9727,7 +10562,7 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F25" sqref="A23:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12791,8 +13626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2065BBB-B9FF-4BBC-B1A5-8837A27B9C03}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AQ15" sqref="AQ15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15856,8 +16691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE46055-3704-4A78-944F-FFAFA9441FC4}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18921,8 +19756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8F2989-E811-4229-822B-85C41BBD0FB6}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="A23:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21986,7 +22821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF9100D-2286-4B8A-9143-152079EEE721}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -25087,8 +25922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D47" sqref="D46:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update masses accounting for "inert" masses
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF986EEC-B126-42B9-9BBA-FCAA10909E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2E1793-308E-4C2E-B55E-2E6D6F4F75E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="4545" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -602,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -621,24 +621,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9817,739 +9816,1053 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5F06E4-4B71-4DD5-A2F8-F472E18DC771}">
-  <dimension ref="A1:AG8"/>
+  <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2:AF8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" customWidth="1"/>
     <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" customWidth="1"/>
     <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.5703125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" customWidth="1"/>
     <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.5703125" style="18" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" customWidth="1"/>
     <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5703125" style="18" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.5703125" customWidth="1"/>
     <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.5703125" style="18" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.5703125" customWidth="1"/>
     <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="23" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="22" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="23" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="22" t="s">
+      <c r="N1" s="24"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="23" t="s">
+      <c r="Q1" s="25"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="22" t="s">
+      <c r="T1" s="24"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="W1" s="22"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="23" t="s">
+      <c r="W1" s="25"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="22" t="s">
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="23" t="s">
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="19"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="18"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="20">
         <f>'Apollo 7'!F28</f>
         <v>411967.90000000008</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="22">
         <f>'Apollo 8'!B28</f>
         <v>2037263</v>
       </c>
-      <c r="F2" s="20"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="23">
         <f>'Apollo 9'!B28</f>
         <v>2147080</v>
       </c>
-      <c r="I2" s="20"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="22">
         <f>'Apollo 10'!B28</f>
         <v>2143978</v>
       </c>
-      <c r="L2" s="20"/>
+      <c r="L2" s="19"/>
       <c r="M2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="27">
+      <c r="N2" s="23">
         <f>'Apollo 11'!B28</f>
         <v>2146040</v>
       </c>
-      <c r="O2" s="20"/>
+      <c r="O2" s="19"/>
       <c r="P2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="26">
+      <c r="Q2" s="22">
         <f>'Apollo 12'!B28</f>
         <v>2147768</v>
       </c>
-      <c r="R2" s="20"/>
+      <c r="R2" s="19"/>
       <c r="S2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="27">
+      <c r="T2" s="23">
         <f>'Apollo 13'!B28</f>
         <v>2148494</v>
       </c>
-      <c r="U2" s="20"/>
+      <c r="U2" s="19"/>
       <c r="V2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="26">
+      <c r="W2" s="22">
         <f>'Apollo 14'!B28</f>
         <v>2150893</v>
       </c>
-      <c r="X2" s="20"/>
+      <c r="X2" s="19"/>
       <c r="Y2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="27">
+      <c r="Z2" s="23">
         <f>'Apollo 15'!B28</f>
         <v>2142469</v>
       </c>
-      <c r="AA2" s="20"/>
+      <c r="AA2" s="19"/>
       <c r="AB2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="AC2" s="26">
+      <c r="AC2" s="22">
         <f>'Apollo 16'!B28</f>
         <v>2155291</v>
       </c>
-      <c r="AD2" s="20"/>
+      <c r="AD2" s="19"/>
       <c r="AE2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" s="27">
+      <c r="AF2" s="23">
         <f>'Apollo 17'!B28</f>
         <v>2153110</v>
       </c>
-      <c r="AG2" s="20"/>
+      <c r="AG2" s="19"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="20">
         <f>'Apollo 7'!F29</f>
         <v>105872.99508169999</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="22">
         <f>'Apollo 8'!B29</f>
         <v>430664</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="23">
         <f>'Apollo 9'!B29</f>
         <v>444829</v>
       </c>
-      <c r="I3" s="20"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="22">
         <f>'Apollo 10'!B29</f>
         <v>445628</v>
       </c>
-      <c r="L3" s="20"/>
+      <c r="L3" s="19"/>
       <c r="M3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="23">
         <f>'Apollo 11'!B29</f>
         <v>443500</v>
       </c>
-      <c r="O3" s="20"/>
+      <c r="O3" s="19"/>
       <c r="P3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3" s="22">
         <f>'Apollo 12'!B29</f>
         <v>446320</v>
       </c>
-      <c r="R3" s="20"/>
+      <c r="R3" s="19"/>
       <c r="S3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="27">
+      <c r="T3" s="23">
         <f>'Apollo 13'!B29</f>
         <v>452316</v>
       </c>
-      <c r="U3" s="20"/>
+      <c r="U3" s="19"/>
       <c r="V3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="26">
+      <c r="W3" s="22">
         <f>'Apollo 14'!B29</f>
         <v>452308</v>
       </c>
-      <c r="X3" s="20"/>
+      <c r="X3" s="19"/>
       <c r="Y3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="Z3" s="27">
+      <c r="Z3" s="23">
         <f>'Apollo 15'!B29</f>
         <v>452430</v>
       </c>
-      <c r="AA3" s="20"/>
+      <c r="AA3" s="19"/>
       <c r="AB3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="AC3" s="26">
+      <c r="AC3" s="22">
         <f>'Apollo 16'!B29</f>
         <v>456812</v>
       </c>
-      <c r="AD3" s="20"/>
+      <c r="AD3" s="19"/>
       <c r="AE3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AF3" s="27">
+      <c r="AF3" s="23">
         <f>'Apollo 17'!B29</f>
         <v>455806</v>
       </c>
-      <c r="AG3" s="20"/>
+      <c r="AG3" s="19"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="20">
         <f>'Apollo 7'!F30</f>
         <v>41858.5</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="22">
         <f>'Apollo 8'!B30</f>
         <v>107469</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="23">
         <f>'Apollo 9'!B30</f>
         <v>106205</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="22">
         <f>'Apollo 10'!B30</f>
         <v>107157</v>
       </c>
-      <c r="L4" s="20"/>
+      <c r="L4" s="19"/>
       <c r="M4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="23">
         <f>'Apollo 11'!B30</f>
         <v>107428</v>
       </c>
-      <c r="O4" s="20"/>
+      <c r="O4" s="19"/>
       <c r="P4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="22">
         <f>'Apollo 12'!B30</f>
         <v>106591</v>
       </c>
-      <c r="R4" s="20"/>
+      <c r="R4" s="19"/>
       <c r="S4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="T4" s="27">
+      <c r="T4" s="23">
         <f>'Apollo 13'!B30</f>
         <v>107179</v>
       </c>
-      <c r="U4" s="20"/>
+      <c r="U4" s="19"/>
       <c r="V4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="W4" s="26">
+      <c r="W4" s="22">
         <f>'Apollo 14'!B30</f>
         <v>106488</v>
       </c>
-      <c r="X4" s="20"/>
+      <c r="X4" s="19"/>
       <c r="Y4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="27">
+      <c r="Z4" s="23">
         <f>'Apollo 15'!B30</f>
         <v>108958</v>
       </c>
-      <c r="AA4" s="20"/>
+      <c r="AA4" s="19"/>
       <c r="AB4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="AC4" s="26">
+      <c r="AC4" s="22">
         <f>'Apollo 16'!B30</f>
         <v>108780</v>
       </c>
-      <c r="AD4" s="20"/>
+      <c r="AD4" s="19"/>
       <c r="AE4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AF4" s="27">
+      <c r="AF4" s="23">
         <f>'Apollo 17'!B30</f>
         <v>108914</v>
       </c>
-      <c r="AG4" s="20"/>
+      <c r="AG4" s="19"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="20">
         <f>'Apollo 7'!F31</f>
         <v>10483.904918300002</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="22">
         <f>'Apollo 8'!B31</f>
         <v>141670</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="23">
         <f>'Apollo 9'!B31</f>
         <v>136740</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="22">
         <f>'Apollo 10'!B31</f>
         <v>136520</v>
       </c>
-      <c r="L5" s="20"/>
+      <c r="L5" s="19"/>
       <c r="M5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="23">
         <f>'Apollo 11'!B31</f>
         <v>133602</v>
       </c>
-      <c r="O5" s="20"/>
+      <c r="O5" s="19"/>
       <c r="P5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="22">
         <f>'Apollo 12'!B31</f>
         <v>133859</v>
       </c>
-      <c r="R5" s="20"/>
+      <c r="R5" s="19"/>
       <c r="S5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="27">
+      <c r="T5" s="23">
         <f>'Apollo 13'!B31</f>
         <v>133764</v>
       </c>
-      <c r="U5" s="20"/>
+      <c r="U5" s="19"/>
       <c r="V5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="W5" s="26">
+      <c r="W5" s="22">
         <f>'Apollo 14'!B31</f>
         <v>133364</v>
       </c>
-      <c r="X5" s="20"/>
+      <c r="X5" s="19"/>
       <c r="Y5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Z5" s="27">
+      <c r="Z5" s="23">
         <f>'Apollo 15'!B31</f>
         <v>132487</v>
       </c>
-      <c r="AA5" s="20"/>
+      <c r="AA5" s="19"/>
       <c r="AB5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="26">
+      <c r="AC5" s="22">
         <f>'Apollo 16'!B31</f>
         <v>133748</v>
       </c>
-      <c r="AD5" s="20"/>
+      <c r="AD5" s="19"/>
       <c r="AE5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="AF5" s="27">
+      <c r="AF5" s="23">
         <f>'Apollo 17'!B31</f>
         <v>133521</v>
       </c>
-      <c r="AG5" s="20"/>
+      <c r="AG5" s="19"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="20">
         <f>'Apollo 7'!F32</f>
         <v>2514.3000000000002</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="22">
         <f>'Apollo 8'!B32</f>
         <v>44151</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="23">
         <f>'Apollo 9'!B32</f>
         <v>41919</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="22">
         <f>'Apollo 10'!B32</f>
         <v>41923</v>
       </c>
-      <c r="L6" s="20"/>
+      <c r="L6" s="19"/>
       <c r="M6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="23">
         <f>'Apollo 11'!B32</f>
         <v>39869</v>
       </c>
-      <c r="O6" s="20"/>
+      <c r="O6" s="19"/>
       <c r="P6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="22">
         <f>'Apollo 12'!B32</f>
         <v>40081</v>
       </c>
-      <c r="R6" s="20"/>
+      <c r="R6" s="19"/>
       <c r="S6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="T6" s="27">
+      <c r="T6" s="23">
         <f>'Apollo 13'!B32</f>
         <v>39068</v>
       </c>
-      <c r="U6" s="20"/>
+      <c r="U6" s="19"/>
       <c r="V6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="W6" s="26">
+      <c r="W6" s="22">
         <f>'Apollo 14'!B32</f>
         <v>39136</v>
       </c>
-      <c r="X6" s="20"/>
+      <c r="X6" s="19"/>
       <c r="Y6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="Z6" s="27">
+      <c r="Z6" s="23">
         <f>'Apollo 15'!B32</f>
         <v>39478</v>
       </c>
-      <c r="AA6" s="20"/>
+      <c r="AA6" s="19"/>
       <c r="AB6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AC6" s="26">
+      <c r="AC6" s="22">
         <f>'Apollo 16'!B32</f>
         <v>40151</v>
       </c>
-      <c r="AD6" s="20"/>
+      <c r="AD6" s="19"/>
       <c r="AE6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AF6" s="27">
+      <c r="AF6" s="23">
         <f>'Apollo 17'!B32</f>
         <v>40163</v>
       </c>
-      <c r="AG6" s="20"/>
+      <c r="AG6" s="19"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="22">
         <f>'Apollo 8'!B33</f>
         <v>14189</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="23">
         <f>'Apollo 9'!B33</f>
         <v>13549</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="22">
         <f>'Apollo 10'!B33</f>
         <v>13810</v>
       </c>
-      <c r="L7" s="20"/>
+      <c r="L7" s="19"/>
       <c r="M7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="23">
         <f>'Apollo 11'!B33</f>
         <v>13439</v>
       </c>
-      <c r="O7" s="20"/>
+      <c r="O7" s="19"/>
       <c r="P7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="22">
         <f>'Apollo 12'!B33</f>
         <v>13541</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="R7" s="19"/>
       <c r="S7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="T7" s="27">
+      <c r="T7" s="23">
         <f>'Apollo 13'!B33</f>
         <v>13786</v>
       </c>
-      <c r="U7" s="20"/>
+      <c r="U7" s="19"/>
       <c r="V7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="W7" s="26">
+      <c r="W7" s="22">
         <f>'Apollo 14'!B33</f>
         <v>13762</v>
       </c>
-      <c r="X7" s="20"/>
+      <c r="X7" s="19"/>
       <c r="Y7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="Z7" s="27">
+      <c r="Z7" s="23">
         <f>'Apollo 15'!B33</f>
         <v>13828</v>
       </c>
-      <c r="AA7" s="20"/>
+      <c r="AA7" s="19"/>
       <c r="AB7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AC7" s="26">
+      <c r="AC7" s="22">
         <f>'Apollo 16'!B33</f>
         <v>13784</v>
       </c>
-      <c r="AD7" s="20"/>
+      <c r="AD7" s="19"/>
       <c r="AE7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AF7" s="27">
+      <c r="AF7" s="23">
         <f>'Apollo 17'!B33</f>
         <v>13747</v>
       </c>
-      <c r="AG7" s="20"/>
+      <c r="AG7" s="19"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="22">
         <f>'Apollo 8'!B34</f>
         <v>4376</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="23">
         <f>'Apollo 9'!B34</f>
         <v>4033</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="22">
         <f>'Apollo 10'!B34</f>
         <v>4033</v>
       </c>
-      <c r="L8" s="20"/>
+      <c r="L8" s="19"/>
       <c r="M8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="23">
         <f>'Apollo 11'!B34</f>
         <v>3982</v>
       </c>
-      <c r="O8" s="20"/>
+      <c r="O8" s="19"/>
       <c r="P8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="22">
         <f>'Apollo 12'!B34</f>
         <v>3996</v>
       </c>
-      <c r="R8" s="20"/>
+      <c r="R8" s="19"/>
       <c r="S8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="27">
+      <c r="T8" s="23">
         <f>'Apollo 13'!B34</f>
         <v>3972</v>
       </c>
-      <c r="U8" s="20"/>
+      <c r="U8" s="19"/>
       <c r="V8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="W8" s="26">
+      <c r="W8" s="22">
         <f>'Apollo 14'!B34</f>
         <v>3945</v>
       </c>
-      <c r="X8" s="20"/>
+      <c r="X8" s="19"/>
       <c r="Y8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="Z8" s="27">
+      <c r="Z8" s="23">
         <f>'Apollo 15'!B34</f>
         <v>3504</v>
       </c>
-      <c r="AA8" s="20"/>
+      <c r="AA8" s="19"/>
       <c r="AB8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="AC8" s="26">
+      <c r="AC8" s="22">
         <f>'Apollo 16'!B34</f>
         <v>3960</v>
       </c>
-      <c r="AD8" s="20"/>
+      <c r="AD8" s="19"/>
       <c r="AE8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AF8" s="27">
+      <c r="AF8" s="23">
         <f>'Apollo 17'!B34</f>
         <v>3908</v>
       </c>
-      <c r="AG8" s="20"/>
+      <c r="AG8" s="19"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>A2&amp;" "&amp;B2</f>
+        <v>SIIFUELMASS 411967.9</v>
+      </c>
+      <c r="D10" t="str">
+        <f>D2&amp;" "&amp;E2</f>
+        <v>SIFUELMASS 2037263</v>
+      </c>
+      <c r="G10" t="str">
+        <f>G2&amp;" "&amp;H2</f>
+        <v>SIFUELMASS 2147080</v>
+      </c>
+      <c r="J10" t="str">
+        <f>J2&amp;" "&amp;K2</f>
+        <v>SIFUELMASS 2143978</v>
+      </c>
+      <c r="M10" t="str">
+        <f>M2&amp;" "&amp;N2</f>
+        <v>SIFUELMASS 2146040</v>
+      </c>
+      <c r="P10" t="str">
+        <f>P2&amp;" "&amp;Q2</f>
+        <v>SIFUELMASS 2147768</v>
+      </c>
+      <c r="S10" t="str">
+        <f>S2&amp;" "&amp;T2</f>
+        <v>SIFUELMASS 2148494</v>
+      </c>
+      <c r="V10" t="str">
+        <f>V2&amp;" "&amp;W2</f>
+        <v>SIFUELMASS 2150893</v>
+      </c>
+      <c r="Y10" t="str">
+        <f>Y2&amp;" "&amp;Z2</f>
+        <v>SIFUELMASS 2142469</v>
+      </c>
+      <c r="AB10" t="str">
+        <f>AB2&amp;" "&amp;AC2</f>
+        <v>SIFUELMASS 2155291</v>
+      </c>
+      <c r="AE10" t="str">
+        <f>AE2&amp;" "&amp;AF2</f>
+        <v>SIFUELMASS 2153110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" ref="A11:A14" si="0">A3&amp;" "&amp;B3</f>
+        <v>S4FUELMASS 105872.9950817</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" ref="D11:D16" si="1">D3&amp;" "&amp;E3</f>
+        <v>SIIFUELMASS 430664</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ref="G11:G15" si="2">G3&amp;" "&amp;H3</f>
+        <v>SIIFUELMASS 444829</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ref="J11:J16" si="3">J3&amp;" "&amp;K3</f>
+        <v>SIIFUELMASS 445628</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ref="M11:M16" si="4">M3&amp;" "&amp;N3</f>
+        <v>SIIFUELMASS 443500</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ref="P11:P16" si="5">P3&amp;" "&amp;Q3</f>
+        <v>SIIFUELMASS 446320</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" ref="S11:S16" si="6">S3&amp;" "&amp;T3</f>
+        <v>SIIFUELMASS 452316</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" ref="V11:V16" si="7">V3&amp;" "&amp;W3</f>
+        <v>SIIFUELMASS 452308</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" ref="Y11:Y16" si="8">Y3&amp;" "&amp;Z3</f>
+        <v>SIIFUELMASS 452430</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" ref="AB11:AB16" si="9">AB3&amp;" "&amp;AC3</f>
+        <v>SIIFUELMASS 456812</v>
+      </c>
+      <c r="AE11" t="str">
+        <f t="shared" ref="AE11:AE15" si="10">AE3&amp;" "&amp;AF3</f>
+        <v>SIIFUELMASS 455806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>SIIEMPTYMASS 41858.5</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>S4FUELMASS 107469</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>S4FUELMASS 106205</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>S4FUELMASS 107157</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="4"/>
+        <v>S4FUELMASS 107428</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="5"/>
+        <v>S4FUELMASS 106591</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="6"/>
+        <v>S4FUELMASS 107179</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="7"/>
+        <v>S4FUELMASS 106488</v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="8"/>
+        <v>S4FUELMASS 108958</v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="9"/>
+        <v>S4FUELMASS 108780</v>
+      </c>
+      <c r="AE12" t="str">
+        <f t="shared" si="10"/>
+        <v>S4FUELMASS 108914</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>S4EMPTYMASS 10483.9049183</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>SIEMPTYMASS 141670</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>SIEMPTYMASS 136740</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>SIEMPTYMASS 136520</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="4"/>
+        <v>SIEMPTYMASS 133602</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="5"/>
+        <v>SIEMPTYMASS 133859</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="6"/>
+        <v>SIEMPTYMASS 133764</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="7"/>
+        <v>SIEMPTYMASS 133364</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="8"/>
+        <v>SIEMPTYMASS 132487</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" si="9"/>
+        <v>SIEMPTYMASS 133748</v>
+      </c>
+      <c r="AE13" t="str">
+        <f t="shared" si="10"/>
+        <v>SIEMPTYMASS 133521</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>INTERSTAGE 2514.3</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>SIIEMPTYMASS 44151</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>SIIEMPTYMASS 41919</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>SIIEMPTYMASS 41923</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="4"/>
+        <v>SIIEMPTYMASS 39869</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="5"/>
+        <v>SIIEMPTYMASS 40081</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="6"/>
+        <v>SIIEMPTYMASS 39068</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="7"/>
+        <v>SIIEMPTYMASS 39136</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" si="8"/>
+        <v>SIIEMPTYMASS 39478</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="9"/>
+        <v>SIIEMPTYMASS 40151</v>
+      </c>
+      <c r="AE14" t="str">
+        <f t="shared" si="10"/>
+        <v>SIIEMPTYMASS 40163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>S4EMPTYMASS 14189</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>S4EMPTYMASS 13549</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>S4EMPTYMASS 13810</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="4"/>
+        <v>S4EMPTYMASS 13439</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="5"/>
+        <v>S4EMPTYMASS 13541</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="6"/>
+        <v>S4EMPTYMASS 13786</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="7"/>
+        <v>S4EMPTYMASS 13762</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="8"/>
+        <v>S4EMPTYMASS 13828</v>
+      </c>
+      <c r="AB15" t="str">
+        <f t="shared" si="9"/>
+        <v>S4EMPTYMASS 13784</v>
+      </c>
+      <c r="AE15" t="str">
+        <f t="shared" si="10"/>
+        <v>S4EMPTYMASS 13747</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>INTERSTAGE 4376</v>
+      </c>
+      <c r="G16" t="str">
+        <f>G8&amp;" "&amp;H8</f>
+        <v>INTERSTAGE 4033</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>INTERSTAGE 4033</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="4"/>
+        <v>INTERSTAGE 3982</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="5"/>
+        <v>INTERSTAGE 3996</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="6"/>
+        <v>INTERSTAGE 3972</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="7"/>
+        <v>INTERSTAGE 3945</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="8"/>
+        <v>INTERSTAGE 3504</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="9"/>
+        <v>INTERSTAGE 3960</v>
+      </c>
+      <c r="AE16" t="str">
+        <f>AE8&amp;" "&amp;AF8</f>
+        <v>INTERSTAGE 3908</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Include IU in Apollo 7 SIVB empty mass
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2E1793-308E-4C2E-B55E-2E6D6F4F75E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4E4FF4-F4A2-47C1-8C8E-09A92C97C00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="4545" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -629,13 +629,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7075,8 +7075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80FCE58-7FB9-4CC7-8163-D01D25C81D7D}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9728,8 +9728,8 @@
         <v>60</v>
       </c>
       <c r="F31" s="13">
-        <f>C20-F29</f>
-        <v>10483.904918300002</v>
+        <f>C20+C21-F29</f>
+        <v>12417.504918300008</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>13</v>
@@ -9819,7 +9819,7 @@
   <dimension ref="A1:AG16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9860,60 +9860,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="18"/>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="18"/>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="K1" s="25"/>
+      <c r="K1" s="24"/>
       <c r="L1" s="18"/>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="N1" s="24"/>
+      <c r="N1" s="26"/>
       <c r="O1" s="18"/>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="25"/>
+      <c r="Q1" s="24"/>
       <c r="R1" s="18"/>
-      <c r="S1" s="24" t="s">
+      <c r="S1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="T1" s="24"/>
+      <c r="T1" s="26"/>
       <c r="U1" s="18"/>
-      <c r="V1" s="25" t="s">
+      <c r="V1" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="W1" s="25"/>
+      <c r="W1" s="24"/>
       <c r="X1" s="18"/>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="24"/>
+      <c r="Z1" s="26"/>
       <c r="AA1" s="18"/>
-      <c r="AB1" s="25" t="s">
+      <c r="AB1" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="AC1" s="25"/>
+      <c r="AC1" s="24"/>
       <c r="AD1" s="18"/>
-      <c r="AE1" s="24" t="s">
+      <c r="AE1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="AF1" s="24"/>
+      <c r="AF1" s="26"/>
       <c r="AG1" s="18"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -10192,7 +10192,7 @@
       </c>
       <c r="B5" s="20">
         <f>'Apollo 7'!F31</f>
-        <v>10483.904918300002</v>
+        <v>12417.504918300008</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="16" t="s">
@@ -10677,7 +10677,7 @@
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>S4EMPTYMASS 10483.9049183</v>
+        <v>S4EMPTYMASS 12417.5049183</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
@@ -10852,17 +10852,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32434,8 +32434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update variable names for Apollo 5 and 7 masses
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2321938-A6B6-4486-8C64-7099ABA33E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EEBF20-56E5-4581-BA06-F1A99CDE64A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7688" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7693" uniqueCount="149">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -472,6 +472,30 @@
   <si>
     <t>Apollo 5</t>
   </si>
+  <si>
+    <t>APS1</t>
+  </si>
+  <si>
+    <t>APS2</t>
+  </si>
+  <si>
+    <t>APSFMASS1</t>
+  </si>
+  <si>
+    <t>APSFMASS2</t>
+  </si>
+  <si>
+    <t>FMASS</t>
+  </si>
+  <si>
+    <t>EMASS</t>
+  </si>
+  <si>
+    <t>S-IB</t>
+  </si>
+  <si>
+    <t>S-IVB</t>
+  </si>
 </sst>
 </file>
 
@@ -654,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -681,16 +705,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7128,8 +7153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80FCE58-7FB9-4CC7-8163-D01D25C81D7D}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7259,7 +7284,7 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="24"/>
       <c r="F2" t="s">
         <v>108</v>
       </c>
@@ -7269,7 +7294,7 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="27"/>
+      <c r="I2" s="24"/>
       <c r="J2" t="s">
         <v>108</v>
       </c>
@@ -7279,7 +7304,7 @@
       <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="27"/>
+      <c r="M2" s="24"/>
       <c r="N2" t="s">
         <v>108</v>
       </c>
@@ -7289,7 +7314,7 @@
       <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="27"/>
+      <c r="Q2" s="24"/>
       <c r="R2" t="s">
         <v>108</v>
       </c>
@@ -7299,7 +7324,7 @@
       <c r="T2" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="27"/>
+      <c r="U2" s="24"/>
       <c r="V2" t="s">
         <v>108</v>
       </c>
@@ -7309,7 +7334,7 @@
       <c r="X2" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="27"/>
+      <c r="Y2" s="24"/>
       <c r="Z2" t="s">
         <v>108</v>
       </c>
@@ -7319,7 +7344,7 @@
       <c r="AB2" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="27"/>
+      <c r="AC2" s="24"/>
       <c r="AD2" t="s">
         <v>108</v>
       </c>
@@ -7329,7 +7354,7 @@
       <c r="AF2" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="27"/>
+      <c r="AG2" s="24"/>
       <c r="AH2" t="s">
         <v>108</v>
       </c>
@@ -7339,7 +7364,7 @@
       <c r="AJ2" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="27"/>
+      <c r="AK2" s="24"/>
       <c r="AL2" t="s">
         <v>108</v>
       </c>
@@ -7349,7 +7374,7 @@
       <c r="AN2" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="27"/>
+      <c r="AO2" s="24"/>
       <c r="AP2" t="s">
         <v>108</v>
       </c>
@@ -7359,7 +7384,7 @@
       <c r="AR2" t="s">
         <v>13</v>
       </c>
-      <c r="AS2" s="27"/>
+      <c r="AS2" s="24"/>
       <c r="AT2" t="s">
         <v>108</v>
       </c>
@@ -7380,7 +7405,7 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="24"/>
       <c r="F3" t="s">
         <v>77</v>
       </c>
@@ -7390,7 +7415,7 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="27"/>
+      <c r="I3" s="24"/>
       <c r="J3" t="s">
         <v>77</v>
       </c>
@@ -7400,7 +7425,7 @@
       <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="27"/>
+      <c r="M3" s="24"/>
       <c r="N3" t="s">
         <v>77</v>
       </c>
@@ -7410,7 +7435,7 @@
       <c r="P3" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="27"/>
+      <c r="Q3" s="24"/>
       <c r="R3" t="s">
         <v>77</v>
       </c>
@@ -7420,7 +7445,7 @@
       <c r="T3" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="27"/>
+      <c r="U3" s="24"/>
       <c r="V3" t="s">
         <v>77</v>
       </c>
@@ -7430,7 +7455,7 @@
       <c r="X3" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="27"/>
+      <c r="Y3" s="24"/>
       <c r="Z3" t="s">
         <v>77</v>
       </c>
@@ -7440,7 +7465,7 @@
       <c r="AB3" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="27"/>
+      <c r="AC3" s="24"/>
       <c r="AD3" t="s">
         <v>77</v>
       </c>
@@ -7450,7 +7475,7 @@
       <c r="AF3" t="s">
         <v>13</v>
       </c>
-      <c r="AG3" s="27"/>
+      <c r="AG3" s="24"/>
       <c r="AH3" t="s">
         <v>77</v>
       </c>
@@ -7460,7 +7485,7 @@
       <c r="AJ3" t="s">
         <v>13</v>
       </c>
-      <c r="AK3" s="27"/>
+      <c r="AK3" s="24"/>
       <c r="AL3" t="s">
         <v>77</v>
       </c>
@@ -7470,7 +7495,7 @@
       <c r="AN3" t="s">
         <v>13</v>
       </c>
-      <c r="AO3" s="27"/>
+      <c r="AO3" s="24"/>
       <c r="AP3" t="s">
         <v>77</v>
       </c>
@@ -7480,7 +7505,7 @@
       <c r="AR3" t="s">
         <v>13</v>
       </c>
-      <c r="AS3" s="27"/>
+      <c r="AS3" s="24"/>
       <c r="AT3" t="s">
         <v>77</v>
       </c>
@@ -7501,7 +7526,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="24"/>
       <c r="F4" t="s">
         <v>78</v>
       </c>
@@ -7511,7 +7536,7 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="27"/>
+      <c r="I4" s="24"/>
       <c r="J4" t="s">
         <v>78</v>
       </c>
@@ -7521,7 +7546,7 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="27"/>
+      <c r="M4" s="24"/>
       <c r="N4" t="s">
         <v>78</v>
       </c>
@@ -7531,7 +7556,7 @@
       <c r="P4" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="27"/>
+      <c r="Q4" s="24"/>
       <c r="R4" t="s">
         <v>78</v>
       </c>
@@ -7541,7 +7566,7 @@
       <c r="T4" t="s">
         <v>13</v>
       </c>
-      <c r="U4" s="27"/>
+      <c r="U4" s="24"/>
       <c r="V4" t="s">
         <v>78</v>
       </c>
@@ -7551,7 +7576,7 @@
       <c r="X4" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="27"/>
+      <c r="Y4" s="24"/>
       <c r="Z4" t="s">
         <v>78</v>
       </c>
@@ -7561,7 +7586,7 @@
       <c r="AB4" t="s">
         <v>13</v>
       </c>
-      <c r="AC4" s="27"/>
+      <c r="AC4" s="24"/>
       <c r="AD4" t="s">
         <v>78</v>
       </c>
@@ -7571,7 +7596,7 @@
       <c r="AF4" t="s">
         <v>13</v>
       </c>
-      <c r="AG4" s="27"/>
+      <c r="AG4" s="24"/>
       <c r="AH4" t="s">
         <v>78</v>
       </c>
@@ -7581,7 +7606,7 @@
       <c r="AJ4" t="s">
         <v>13</v>
       </c>
-      <c r="AK4" s="27"/>
+      <c r="AK4" s="24"/>
       <c r="AL4" t="s">
         <v>78</v>
       </c>
@@ -7591,7 +7616,7 @@
       <c r="AN4" t="s">
         <v>13</v>
       </c>
-      <c r="AO4" s="27"/>
+      <c r="AO4" s="24"/>
       <c r="AP4" t="s">
         <v>78</v>
       </c>
@@ -7601,7 +7626,7 @@
       <c r="AR4" t="s">
         <v>13</v>
       </c>
-      <c r="AS4" s="27"/>
+      <c r="AS4" s="24"/>
       <c r="AT4" t="s">
         <v>78</v>
       </c>
@@ -7622,7 +7647,7 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="24"/>
       <c r="F5" t="s">
         <v>79</v>
       </c>
@@ -7632,7 +7657,7 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="24"/>
       <c r="J5" t="s">
         <v>79</v>
       </c>
@@ -7642,7 +7667,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="27"/>
+      <c r="M5" s="24"/>
       <c r="N5" t="s">
         <v>79</v>
       </c>
@@ -7652,7 +7677,7 @@
       <c r="P5" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="27"/>
+      <c r="Q5" s="24"/>
       <c r="R5" t="s">
         <v>79</v>
       </c>
@@ -7662,7 +7687,7 @@
       <c r="T5" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="27"/>
+      <c r="U5" s="24"/>
       <c r="V5" t="s">
         <v>79</v>
       </c>
@@ -7672,7 +7697,7 @@
       <c r="X5" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="27"/>
+      <c r="Y5" s="24"/>
       <c r="Z5" t="s">
         <v>79</v>
       </c>
@@ -7682,7 +7707,7 @@
       <c r="AB5" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="27"/>
+      <c r="AC5" s="24"/>
       <c r="AD5" t="s">
         <v>79</v>
       </c>
@@ -7692,7 +7717,7 @@
       <c r="AF5" t="s">
         <v>13</v>
       </c>
-      <c r="AG5" s="27"/>
+      <c r="AG5" s="24"/>
       <c r="AH5" t="s">
         <v>79</v>
       </c>
@@ -7702,7 +7727,7 @@
       <c r="AJ5" t="s">
         <v>13</v>
       </c>
-      <c r="AK5" s="27"/>
+      <c r="AK5" s="24"/>
       <c r="AL5" t="s">
         <v>79</v>
       </c>
@@ -7712,7 +7737,7 @@
       <c r="AN5" t="s">
         <v>13</v>
       </c>
-      <c r="AO5" s="27"/>
+      <c r="AO5" s="24"/>
       <c r="AP5" t="s">
         <v>79</v>
       </c>
@@ -7722,7 +7747,7 @@
       <c r="AR5" t="s">
         <v>13</v>
       </c>
-      <c r="AS5" s="27"/>
+      <c r="AS5" s="24"/>
       <c r="AT5" t="s">
         <v>79</v>
       </c>
@@ -7743,7 +7768,7 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="24"/>
       <c r="F6" t="s">
         <v>80</v>
       </c>
@@ -7753,7 +7778,7 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="24"/>
       <c r="J6" t="s">
         <v>80</v>
       </c>
@@ -7763,7 +7788,7 @@
       <c r="L6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="27"/>
+      <c r="M6" s="24"/>
       <c r="N6" t="s">
         <v>80</v>
       </c>
@@ -7773,7 +7798,7 @@
       <c r="P6" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="24"/>
       <c r="R6" t="s">
         <v>80</v>
       </c>
@@ -7783,7 +7808,7 @@
       <c r="T6" t="s">
         <v>13</v>
       </c>
-      <c r="U6" s="27"/>
+      <c r="U6" s="24"/>
       <c r="V6" t="s">
         <v>80</v>
       </c>
@@ -7793,7 +7818,7 @@
       <c r="X6" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="27"/>
+      <c r="Y6" s="24"/>
       <c r="Z6" t="s">
         <v>80</v>
       </c>
@@ -7803,7 +7828,7 @@
       <c r="AB6" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="27"/>
+      <c r="AC6" s="24"/>
       <c r="AD6" t="s">
         <v>80</v>
       </c>
@@ -7813,7 +7838,7 @@
       <c r="AF6" t="s">
         <v>13</v>
       </c>
-      <c r="AG6" s="27"/>
+      <c r="AG6" s="24"/>
       <c r="AH6" t="s">
         <v>80</v>
       </c>
@@ -7823,7 +7848,7 @@
       <c r="AJ6" t="s">
         <v>13</v>
       </c>
-      <c r="AK6" s="27"/>
+      <c r="AK6" s="24"/>
       <c r="AL6" t="s">
         <v>80</v>
       </c>
@@ -7833,7 +7858,7 @@
       <c r="AN6" t="s">
         <v>13</v>
       </c>
-      <c r="AO6" s="27"/>
+      <c r="AO6" s="24"/>
       <c r="AP6" t="s">
         <v>80</v>
       </c>
@@ -7843,7 +7868,7 @@
       <c r="AR6" t="s">
         <v>13</v>
       </c>
-      <c r="AS6" s="27"/>
+      <c r="AS6" s="24"/>
       <c r="AT6" t="s">
         <v>80</v>
       </c>
@@ -7864,7 +7889,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="24"/>
       <c r="F7" t="s">
         <v>81</v>
       </c>
@@ -7874,7 +7899,7 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="27"/>
+      <c r="I7" s="24"/>
       <c r="J7" t="s">
         <v>81</v>
       </c>
@@ -7884,7 +7909,7 @@
       <c r="L7" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="27"/>
+      <c r="M7" s="24"/>
       <c r="N7" t="s">
         <v>81</v>
       </c>
@@ -7894,7 +7919,7 @@
       <c r="P7" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="27"/>
+      <c r="Q7" s="24"/>
       <c r="R7" t="s">
         <v>81</v>
       </c>
@@ -7904,7 +7929,7 @@
       <c r="T7" t="s">
         <v>13</v>
       </c>
-      <c r="U7" s="27"/>
+      <c r="U7" s="24"/>
       <c r="V7" t="s">
         <v>81</v>
       </c>
@@ -7914,7 +7939,7 @@
       <c r="X7" t="s">
         <v>13</v>
       </c>
-      <c r="Y7" s="27"/>
+      <c r="Y7" s="24"/>
       <c r="Z7" t="s">
         <v>81</v>
       </c>
@@ -7924,7 +7949,7 @@
       <c r="AB7" t="s">
         <v>13</v>
       </c>
-      <c r="AC7" s="27"/>
+      <c r="AC7" s="24"/>
       <c r="AD7" t="s">
         <v>81</v>
       </c>
@@ -7934,7 +7959,7 @@
       <c r="AF7" t="s">
         <v>13</v>
       </c>
-      <c r="AG7" s="27"/>
+      <c r="AG7" s="24"/>
       <c r="AH7" t="s">
         <v>81</v>
       </c>
@@ -7944,7 +7969,7 @@
       <c r="AJ7" t="s">
         <v>13</v>
       </c>
-      <c r="AK7" s="27"/>
+      <c r="AK7" s="24"/>
       <c r="AL7" t="s">
         <v>81</v>
       </c>
@@ -7954,7 +7979,7 @@
       <c r="AN7" t="s">
         <v>13</v>
       </c>
-      <c r="AO7" s="27"/>
+      <c r="AO7" s="24"/>
       <c r="AP7" t="s">
         <v>81</v>
       </c>
@@ -7964,7 +7989,7 @@
       <c r="AR7" t="s">
         <v>13</v>
       </c>
-      <c r="AS7" s="27"/>
+      <c r="AS7" s="24"/>
       <c r="AT7" t="s">
         <v>81</v>
       </c>
@@ -7985,7 +8010,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="24"/>
       <c r="F8" t="s">
         <v>82</v>
       </c>
@@ -7995,7 +8020,7 @@
       <c r="H8" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="I8" s="24"/>
       <c r="J8" t="s">
         <v>82</v>
       </c>
@@ -8005,7 +8030,7 @@
       <c r="L8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="27"/>
+      <c r="M8" s="24"/>
       <c r="N8" t="s">
         <v>82</v>
       </c>
@@ -8015,7 +8040,7 @@
       <c r="P8" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="27"/>
+      <c r="Q8" s="24"/>
       <c r="R8" t="s">
         <v>82</v>
       </c>
@@ -8025,7 +8050,7 @@
       <c r="T8" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="27"/>
+      <c r="U8" s="24"/>
       <c r="V8" t="s">
         <v>82</v>
       </c>
@@ -8035,7 +8060,7 @@
       <c r="X8" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="27"/>
+      <c r="Y8" s="24"/>
       <c r="Z8" t="s">
         <v>82</v>
       </c>
@@ -8045,7 +8070,7 @@
       <c r="AB8" t="s">
         <v>13</v>
       </c>
-      <c r="AC8" s="27"/>
+      <c r="AC8" s="24"/>
       <c r="AD8" t="s">
         <v>82</v>
       </c>
@@ -8055,7 +8080,7 @@
       <c r="AF8" t="s">
         <v>13</v>
       </c>
-      <c r="AG8" s="27"/>
+      <c r="AG8" s="24"/>
       <c r="AH8" t="s">
         <v>82</v>
       </c>
@@ -8065,7 +8090,7 @@
       <c r="AJ8" t="s">
         <v>13</v>
       </c>
-      <c r="AK8" s="27"/>
+      <c r="AK8" s="24"/>
       <c r="AL8" t="s">
         <v>82</v>
       </c>
@@ -8075,7 +8100,7 @@
       <c r="AN8" t="s">
         <v>13</v>
       </c>
-      <c r="AO8" s="27"/>
+      <c r="AO8" s="24"/>
       <c r="AP8" t="s">
         <v>82</v>
       </c>
@@ -8085,7 +8110,7 @@
       <c r="AR8" t="s">
         <v>13</v>
       </c>
-      <c r="AS8" s="27"/>
+      <c r="AS8" s="24"/>
       <c r="AT8" t="s">
         <v>82</v>
       </c>
@@ -8106,7 +8131,7 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="27"/>
+      <c r="E9" s="24"/>
       <c r="F9" t="s">
         <v>83</v>
       </c>
@@ -8116,7 +8141,7 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="27"/>
+      <c r="I9" s="24"/>
       <c r="J9" t="s">
         <v>83</v>
       </c>
@@ -8126,7 +8151,7 @@
       <c r="L9" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="27"/>
+      <c r="M9" s="24"/>
       <c r="N9" t="s">
         <v>83</v>
       </c>
@@ -8136,7 +8161,7 @@
       <c r="P9" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="27"/>
+      <c r="Q9" s="24"/>
       <c r="R9" t="s">
         <v>83</v>
       </c>
@@ -8146,7 +8171,7 @@
       <c r="T9" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="27"/>
+      <c r="U9" s="24"/>
       <c r="V9" t="s">
         <v>83</v>
       </c>
@@ -8156,7 +8181,7 @@
       <c r="X9" t="s">
         <v>13</v>
       </c>
-      <c r="Y9" s="27"/>
+      <c r="Y9" s="24"/>
       <c r="Z9" t="s">
         <v>83</v>
       </c>
@@ -8166,7 +8191,7 @@
       <c r="AB9" t="s">
         <v>13</v>
       </c>
-      <c r="AC9" s="27"/>
+      <c r="AC9" s="24"/>
       <c r="AD9" t="s">
         <v>83</v>
       </c>
@@ -8176,7 +8201,7 @@
       <c r="AF9" t="s">
         <v>13</v>
       </c>
-      <c r="AG9" s="27"/>
+      <c r="AG9" s="24"/>
       <c r="AH9" t="s">
         <v>83</v>
       </c>
@@ -8186,7 +8211,7 @@
       <c r="AJ9" t="s">
         <v>13</v>
       </c>
-      <c r="AK9" s="27"/>
+      <c r="AK9" s="24"/>
       <c r="AL9" t="s">
         <v>83</v>
       </c>
@@ -8196,7 +8221,7 @@
       <c r="AN9" t="s">
         <v>13</v>
       </c>
-      <c r="AO9" s="27"/>
+      <c r="AO9" s="24"/>
       <c r="AP9" t="s">
         <v>83</v>
       </c>
@@ -8206,7 +8231,7 @@
       <c r="AR9" t="s">
         <v>13</v>
       </c>
-      <c r="AS9" s="27"/>
+      <c r="AS9" s="24"/>
       <c r="AT9" t="s">
         <v>83</v>
       </c>
@@ -8227,7 +8252,7 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="24"/>
       <c r="F10" t="s">
         <v>84</v>
       </c>
@@ -8237,7 +8262,7 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="27"/>
+      <c r="I10" s="24"/>
       <c r="J10" t="s">
         <v>84</v>
       </c>
@@ -8247,7 +8272,7 @@
       <c r="L10" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="27"/>
+      <c r="M10" s="24"/>
       <c r="N10" t="s">
         <v>84</v>
       </c>
@@ -8257,7 +8282,7 @@
       <c r="P10" t="s">
         <v>13</v>
       </c>
-      <c r="Q10" s="27"/>
+      <c r="Q10" s="24"/>
       <c r="R10" t="s">
         <v>84</v>
       </c>
@@ -8267,7 +8292,7 @@
       <c r="T10" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="27"/>
+      <c r="U10" s="24"/>
       <c r="V10" t="s">
         <v>84</v>
       </c>
@@ -8277,7 +8302,7 @@
       <c r="X10" t="s">
         <v>13</v>
       </c>
-      <c r="Y10" s="27"/>
+      <c r="Y10" s="24"/>
       <c r="Z10" t="s">
         <v>84</v>
       </c>
@@ -8287,7 +8312,7 @@
       <c r="AB10" t="s">
         <v>13</v>
       </c>
-      <c r="AC10" s="27"/>
+      <c r="AC10" s="24"/>
       <c r="AD10" t="s">
         <v>84</v>
       </c>
@@ -8297,7 +8322,7 @@
       <c r="AF10" t="s">
         <v>13</v>
       </c>
-      <c r="AG10" s="27"/>
+      <c r="AG10" s="24"/>
       <c r="AH10" t="s">
         <v>84</v>
       </c>
@@ -8307,7 +8332,7 @@
       <c r="AJ10" t="s">
         <v>13</v>
       </c>
-      <c r="AK10" s="27"/>
+      <c r="AK10" s="24"/>
       <c r="AL10" t="s">
         <v>84</v>
       </c>
@@ -8317,7 +8342,7 @@
       <c r="AN10" t="s">
         <v>13</v>
       </c>
-      <c r="AO10" s="27"/>
+      <c r="AO10" s="24"/>
       <c r="AP10" t="s">
         <v>84</v>
       </c>
@@ -8327,7 +8352,7 @@
       <c r="AR10" t="s">
         <v>13</v>
       </c>
-      <c r="AS10" s="27"/>
+      <c r="AS10" s="24"/>
       <c r="AT10" t="s">
         <v>84</v>
       </c>
@@ -8348,7 +8373,7 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="27"/>
+      <c r="E11" s="24"/>
       <c r="F11" t="s">
         <v>85</v>
       </c>
@@ -8358,7 +8383,7 @@
       <c r="H11" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="27"/>
+      <c r="I11" s="24"/>
       <c r="J11" t="s">
         <v>85</v>
       </c>
@@ -8368,7 +8393,7 @@
       <c r="L11" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="27"/>
+      <c r="M11" s="24"/>
       <c r="N11" t="s">
         <v>85</v>
       </c>
@@ -8378,7 +8403,7 @@
       <c r="P11" t="s">
         <v>13</v>
       </c>
-      <c r="Q11" s="27"/>
+      <c r="Q11" s="24"/>
       <c r="R11" t="s">
         <v>85</v>
       </c>
@@ -8388,7 +8413,7 @@
       <c r="T11" t="s">
         <v>13</v>
       </c>
-      <c r="U11" s="27"/>
+      <c r="U11" s="24"/>
       <c r="V11" t="s">
         <v>85</v>
       </c>
@@ -8398,7 +8423,7 @@
       <c r="X11" t="s">
         <v>13</v>
       </c>
-      <c r="Y11" s="27"/>
+      <c r="Y11" s="24"/>
       <c r="Z11" t="s">
         <v>85</v>
       </c>
@@ -8408,7 +8433,7 @@
       <c r="AB11" t="s">
         <v>13</v>
       </c>
-      <c r="AC11" s="27"/>
+      <c r="AC11" s="24"/>
       <c r="AD11" t="s">
         <v>85</v>
       </c>
@@ -8418,7 +8443,7 @@
       <c r="AF11" t="s">
         <v>13</v>
       </c>
-      <c r="AG11" s="27"/>
+      <c r="AG11" s="24"/>
       <c r="AH11" t="s">
         <v>85</v>
       </c>
@@ -8428,7 +8453,7 @@
       <c r="AJ11" t="s">
         <v>13</v>
       </c>
-      <c r="AK11" s="27"/>
+      <c r="AK11" s="24"/>
       <c r="AL11" t="s">
         <v>85</v>
       </c>
@@ -8438,7 +8463,7 @@
       <c r="AN11" t="s">
         <v>13</v>
       </c>
-      <c r="AO11" s="27"/>
+      <c r="AO11" s="24"/>
       <c r="AP11" t="s">
         <v>85</v>
       </c>
@@ -8448,7 +8473,7 @@
       <c r="AR11" t="s">
         <v>13</v>
       </c>
-      <c r="AS11" s="27"/>
+      <c r="AS11" s="24"/>
       <c r="AT11" t="s">
         <v>85</v>
       </c>
@@ -8469,7 +8494,7 @@
       <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="24"/>
       <c r="F12" t="s">
         <v>86</v>
       </c>
@@ -8479,7 +8504,7 @@
       <c r="H12" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="27"/>
+      <c r="I12" s="24"/>
       <c r="J12" t="s">
         <v>86</v>
       </c>
@@ -8489,7 +8514,7 @@
       <c r="L12" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="27"/>
+      <c r="M12" s="24"/>
       <c r="N12" t="s">
         <v>86</v>
       </c>
@@ -8499,7 +8524,7 @@
       <c r="P12" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="27"/>
+      <c r="Q12" s="24"/>
       <c r="R12" t="s">
         <v>86</v>
       </c>
@@ -8509,7 +8534,7 @@
       <c r="T12" t="s">
         <v>13</v>
       </c>
-      <c r="U12" s="27"/>
+      <c r="U12" s="24"/>
       <c r="V12" t="s">
         <v>86</v>
       </c>
@@ -8519,7 +8544,7 @@
       <c r="X12" t="s">
         <v>13</v>
       </c>
-      <c r="Y12" s="27"/>
+      <c r="Y12" s="24"/>
       <c r="Z12" t="s">
         <v>86</v>
       </c>
@@ -8529,7 +8554,7 @@
       <c r="AB12" t="s">
         <v>13</v>
       </c>
-      <c r="AC12" s="27"/>
+      <c r="AC12" s="24"/>
       <c r="AD12" t="s">
         <v>86</v>
       </c>
@@ -8539,7 +8564,7 @@
       <c r="AF12" t="s">
         <v>13</v>
       </c>
-      <c r="AG12" s="27"/>
+      <c r="AG12" s="24"/>
       <c r="AH12" t="s">
         <v>86</v>
       </c>
@@ -8549,7 +8574,7 @@
       <c r="AJ12" t="s">
         <v>13</v>
       </c>
-      <c r="AK12" s="27"/>
+      <c r="AK12" s="24"/>
       <c r="AL12" t="s">
         <v>86</v>
       </c>
@@ -8559,7 +8584,7 @@
       <c r="AN12" t="s">
         <v>13</v>
       </c>
-      <c r="AO12" s="27"/>
+      <c r="AO12" s="24"/>
       <c r="AP12" t="s">
         <v>86</v>
       </c>
@@ -8569,7 +8594,7 @@
       <c r="AR12" t="s">
         <v>13</v>
       </c>
-      <c r="AS12" s="27"/>
+      <c r="AS12" s="24"/>
       <c r="AT12" t="s">
         <v>86</v>
       </c>
@@ -8590,7 +8615,7 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="24"/>
       <c r="F13" t="s">
         <v>87</v>
       </c>
@@ -8600,7 +8625,7 @@
       <c r="H13" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="27"/>
+      <c r="I13" s="24"/>
       <c r="J13" t="s">
         <v>87</v>
       </c>
@@ -8610,7 +8635,7 @@
       <c r="L13" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="27"/>
+      <c r="M13" s="24"/>
       <c r="N13" t="s">
         <v>87</v>
       </c>
@@ -8620,7 +8645,7 @@
       <c r="P13" t="s">
         <v>13</v>
       </c>
-      <c r="Q13" s="27"/>
+      <c r="Q13" s="24"/>
       <c r="R13" t="s">
         <v>87</v>
       </c>
@@ -8630,7 +8655,7 @@
       <c r="T13" t="s">
         <v>13</v>
       </c>
-      <c r="U13" s="27"/>
+      <c r="U13" s="24"/>
       <c r="V13" t="s">
         <v>87</v>
       </c>
@@ -8640,7 +8665,7 @@
       <c r="X13" t="s">
         <v>13</v>
       </c>
-      <c r="Y13" s="27"/>
+      <c r="Y13" s="24"/>
       <c r="Z13" t="s">
         <v>87</v>
       </c>
@@ -8650,7 +8675,7 @@
       <c r="AB13" t="s">
         <v>13</v>
       </c>
-      <c r="AC13" s="27"/>
+      <c r="AC13" s="24"/>
       <c r="AD13" t="s">
         <v>87</v>
       </c>
@@ -8660,7 +8685,7 @@
       <c r="AF13" t="s">
         <v>13</v>
       </c>
-      <c r="AG13" s="27"/>
+      <c r="AG13" s="24"/>
       <c r="AH13" t="s">
         <v>87</v>
       </c>
@@ -8670,7 +8695,7 @@
       <c r="AJ13" t="s">
         <v>13</v>
       </c>
-      <c r="AK13" s="27"/>
+      <c r="AK13" s="24"/>
       <c r="AL13" t="s">
         <v>87</v>
       </c>
@@ -8680,7 +8705,7 @@
       <c r="AN13" t="s">
         <v>13</v>
       </c>
-      <c r="AO13" s="27"/>
+      <c r="AO13" s="24"/>
       <c r="AP13" t="s">
         <v>87</v>
       </c>
@@ -8690,7 +8715,7 @@
       <c r="AR13" t="s">
         <v>13</v>
       </c>
-      <c r="AS13" s="27"/>
+      <c r="AS13" s="24"/>
       <c r="AT13" t="s">
         <v>87</v>
       </c>
@@ -8712,7 +8737,7 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="27"/>
+      <c r="E14" s="24"/>
       <c r="F14" t="s">
         <v>1</v>
       </c>
@@ -8722,7 +8747,7 @@
       <c r="H14" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="27"/>
+      <c r="I14" s="24"/>
       <c r="J14" t="s">
         <v>1</v>
       </c>
@@ -8732,7 +8757,7 @@
       <c r="L14" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="27"/>
+      <c r="M14" s="24"/>
       <c r="N14" t="s">
         <v>1</v>
       </c>
@@ -8742,7 +8767,7 @@
       <c r="P14" t="s">
         <v>13</v>
       </c>
-      <c r="Q14" s="27"/>
+      <c r="Q14" s="24"/>
       <c r="R14" t="s">
         <v>1</v>
       </c>
@@ -8752,7 +8777,7 @@
       <c r="T14" t="s">
         <v>13</v>
       </c>
-      <c r="U14" s="27"/>
+      <c r="U14" s="24"/>
       <c r="V14" t="s">
         <v>1</v>
       </c>
@@ -8762,7 +8787,7 @@
       <c r="X14" t="s">
         <v>13</v>
       </c>
-      <c r="Y14" s="27"/>
+      <c r="Y14" s="24"/>
       <c r="Z14" t="s">
         <v>1</v>
       </c>
@@ -8772,7 +8797,7 @@
       <c r="AB14" t="s">
         <v>13</v>
       </c>
-      <c r="AC14" s="27"/>
+      <c r="AC14" s="24"/>
       <c r="AD14" t="s">
         <v>1</v>
       </c>
@@ -8782,7 +8807,7 @@
       <c r="AF14" t="s">
         <v>13</v>
       </c>
-      <c r="AG14" s="27"/>
+      <c r="AG14" s="24"/>
       <c r="AH14" t="s">
         <v>1</v>
       </c>
@@ -8792,7 +8817,7 @@
       <c r="AJ14" t="s">
         <v>13</v>
       </c>
-      <c r="AK14" s="27"/>
+      <c r="AK14" s="24"/>
       <c r="AL14" t="s">
         <v>1</v>
       </c>
@@ -8802,7 +8827,7 @@
       <c r="AN14" t="s">
         <v>13</v>
       </c>
-      <c r="AO14" s="27"/>
+      <c r="AO14" s="24"/>
       <c r="AP14" t="s">
         <v>1</v>
       </c>
@@ -8812,7 +8837,7 @@
       <c r="AR14" t="s">
         <v>13</v>
       </c>
-      <c r="AS14" s="27"/>
+      <c r="AS14" s="24"/>
       <c r="AT14" t="s">
         <v>1</v>
       </c>
@@ -8824,7 +8849,7 @@
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E15" s="27"/>
+      <c r="E15" s="24"/>
       <c r="F15" t="s">
         <v>3</v>
       </c>
@@ -8834,7 +8859,7 @@
       <c r="H15" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="27"/>
+      <c r="I15" s="24"/>
       <c r="J15" t="s">
         <v>3</v>
       </c>
@@ -8844,7 +8869,7 @@
       <c r="L15" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="27"/>
+      <c r="M15" s="24"/>
       <c r="N15" t="s">
         <v>3</v>
       </c>
@@ -8854,7 +8879,7 @@
       <c r="P15" t="s">
         <v>13</v>
       </c>
-      <c r="Q15" s="27"/>
+      <c r="Q15" s="24"/>
       <c r="R15" t="s">
         <v>3</v>
       </c>
@@ -8864,7 +8889,7 @@
       <c r="T15" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="27"/>
+      <c r="U15" s="24"/>
       <c r="V15" t="s">
         <v>3</v>
       </c>
@@ -8874,7 +8899,7 @@
       <c r="X15" t="s">
         <v>13</v>
       </c>
-      <c r="Y15" s="27"/>
+      <c r="Y15" s="24"/>
       <c r="Z15" t="s">
         <v>3</v>
       </c>
@@ -8884,7 +8909,7 @@
       <c r="AB15" t="s">
         <v>13</v>
       </c>
-      <c r="AC15" s="27"/>
+      <c r="AC15" s="24"/>
       <c r="AD15" t="s">
         <v>3</v>
       </c>
@@ -8894,7 +8919,7 @@
       <c r="AF15" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="27"/>
+      <c r="AG15" s="24"/>
       <c r="AH15" t="s">
         <v>3</v>
       </c>
@@ -8904,7 +8929,7 @@
       <c r="AJ15" t="s">
         <v>13</v>
       </c>
-      <c r="AK15" s="27"/>
+      <c r="AK15" s="24"/>
       <c r="AL15" t="s">
         <v>3</v>
       </c>
@@ -8914,7 +8939,7 @@
       <c r="AN15" t="s">
         <v>13</v>
       </c>
-      <c r="AO15" s="27"/>
+      <c r="AO15" s="24"/>
       <c r="AP15" t="s">
         <v>3</v>
       </c>
@@ -8924,7 +8949,7 @@
       <c r="AR15" t="s">
         <v>13</v>
       </c>
-      <c r="AS15" s="27"/>
+      <c r="AS15" s="24"/>
       <c r="AT15" t="s">
         <v>3</v>
       </c>
@@ -8945,7 +8970,7 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="27"/>
+      <c r="E16" s="24"/>
       <c r="F16" t="s">
         <v>2</v>
       </c>
@@ -8955,7 +8980,7 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="27"/>
+      <c r="I16" s="24"/>
       <c r="J16" t="s">
         <v>2</v>
       </c>
@@ -8965,7 +8990,7 @@
       <c r="L16" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="27"/>
+      <c r="M16" s="24"/>
       <c r="N16" t="s">
         <v>2</v>
       </c>
@@ -8975,7 +9000,7 @@
       <c r="P16" t="s">
         <v>13</v>
       </c>
-      <c r="Q16" s="27"/>
+      <c r="Q16" s="24"/>
       <c r="R16" t="s">
         <v>2</v>
       </c>
@@ -8985,7 +9010,7 @@
       <c r="T16" t="s">
         <v>13</v>
       </c>
-      <c r="U16" s="27"/>
+      <c r="U16" s="24"/>
       <c r="V16" t="s">
         <v>2</v>
       </c>
@@ -8995,7 +9020,7 @@
       <c r="X16" t="s">
         <v>13</v>
       </c>
-      <c r="Y16" s="27"/>
+      <c r="Y16" s="24"/>
       <c r="Z16" t="s">
         <v>2</v>
       </c>
@@ -9005,7 +9030,7 @@
       <c r="AB16" t="s">
         <v>13</v>
       </c>
-      <c r="AC16" s="27"/>
+      <c r="AC16" s="24"/>
       <c r="AD16" t="s">
         <v>2</v>
       </c>
@@ -9015,7 +9040,7 @@
       <c r="AF16" t="s">
         <v>13</v>
       </c>
-      <c r="AG16" s="27"/>
+      <c r="AG16" s="24"/>
       <c r="AH16" t="s">
         <v>2</v>
       </c>
@@ -9025,7 +9050,7 @@
       <c r="AJ16" t="s">
         <v>13</v>
       </c>
-      <c r="AK16" s="27"/>
+      <c r="AK16" s="24"/>
       <c r="AL16" t="s">
         <v>2</v>
       </c>
@@ -9035,7 +9060,7 @@
       <c r="AN16" t="s">
         <v>13</v>
       </c>
-      <c r="AO16" s="27"/>
+      <c r="AO16" s="24"/>
       <c r="AP16" t="s">
         <v>2</v>
       </c>
@@ -9045,7 +9070,7 @@
       <c r="AR16" t="s">
         <v>13</v>
       </c>
-      <c r="AS16" s="27"/>
+      <c r="AS16" s="24"/>
       <c r="AT16" t="s">
         <v>2</v>
       </c>
@@ -9066,7 +9091,7 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="24"/>
       <c r="F17" t="s">
         <v>32</v>
       </c>
@@ -9076,7 +9101,7 @@
       <c r="H17" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="27"/>
+      <c r="I17" s="24"/>
       <c r="J17" t="s">
         <v>32</v>
       </c>
@@ -9086,7 +9111,7 @@
       <c r="L17" t="s">
         <v>13</v>
       </c>
-      <c r="M17" s="27"/>
+      <c r="M17" s="24"/>
       <c r="N17" t="s">
         <v>32</v>
       </c>
@@ -9096,7 +9121,7 @@
       <c r="P17" t="s">
         <v>13</v>
       </c>
-      <c r="Q17" s="27"/>
+      <c r="Q17" s="24"/>
       <c r="R17" t="s">
         <v>32</v>
       </c>
@@ -9106,7 +9131,7 @@
       <c r="T17" t="s">
         <v>13</v>
       </c>
-      <c r="U17" s="27"/>
+      <c r="U17" s="24"/>
       <c r="V17" t="s">
         <v>32</v>
       </c>
@@ -9116,7 +9141,7 @@
       <c r="X17" t="s">
         <v>13</v>
       </c>
-      <c r="Y17" s="27"/>
+      <c r="Y17" s="24"/>
       <c r="Z17" t="s">
         <v>32</v>
       </c>
@@ -9126,7 +9151,7 @@
       <c r="AB17" t="s">
         <v>13</v>
       </c>
-      <c r="AC17" s="27"/>
+      <c r="AC17" s="24"/>
       <c r="AD17" t="s">
         <v>32</v>
       </c>
@@ -9136,7 +9161,7 @@
       <c r="AF17" t="s">
         <v>13</v>
       </c>
-      <c r="AG17" s="27"/>
+      <c r="AG17" s="24"/>
       <c r="AH17" t="s">
         <v>32</v>
       </c>
@@ -9146,7 +9171,7 @@
       <c r="AJ17" t="s">
         <v>13</v>
       </c>
-      <c r="AK17" s="27"/>
+      <c r="AK17" s="24"/>
       <c r="AL17" t="s">
         <v>32</v>
       </c>
@@ -9156,7 +9181,7 @@
       <c r="AN17" t="s">
         <v>13</v>
       </c>
-      <c r="AO17" s="27"/>
+      <c r="AO17" s="24"/>
       <c r="AP17" t="s">
         <v>32</v>
       </c>
@@ -9166,7 +9191,7 @@
       <c r="AR17" t="s">
         <v>13</v>
       </c>
-      <c r="AS17" s="27"/>
+      <c r="AS17" s="24"/>
       <c r="AT17" t="s">
         <v>32</v>
       </c>
@@ -9188,7 +9213,7 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="27"/>
+      <c r="E18" s="24"/>
       <c r="F18" t="s">
         <v>34</v>
       </c>
@@ -9198,7 +9223,7 @@
       <c r="H18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="27"/>
+      <c r="I18" s="24"/>
       <c r="J18" t="s">
         <v>34</v>
       </c>
@@ -9208,7 +9233,7 @@
       <c r="L18" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="27"/>
+      <c r="M18" s="24"/>
       <c r="N18" t="s">
         <v>34</v>
       </c>
@@ -9218,7 +9243,7 @@
       <c r="P18" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="27"/>
+      <c r="Q18" s="24"/>
       <c r="R18" t="s">
         <v>34</v>
       </c>
@@ -9228,7 +9253,7 @@
       <c r="T18" t="s">
         <v>13</v>
       </c>
-      <c r="U18" s="27"/>
+      <c r="U18" s="24"/>
       <c r="V18" t="s">
         <v>34</v>
       </c>
@@ -9238,7 +9263,7 @@
       <c r="X18" t="s">
         <v>13</v>
       </c>
-      <c r="Y18" s="27"/>
+      <c r="Y18" s="24"/>
       <c r="Z18" t="s">
         <v>34</v>
       </c>
@@ -9248,7 +9273,7 @@
       <c r="AB18" t="s">
         <v>13</v>
       </c>
-      <c r="AC18" s="27"/>
+      <c r="AC18" s="24"/>
       <c r="AD18" t="s">
         <v>34</v>
       </c>
@@ -9258,7 +9283,7 @@
       <c r="AF18" t="s">
         <v>13</v>
       </c>
-      <c r="AG18" s="27"/>
+      <c r="AG18" s="24"/>
       <c r="AH18" t="s">
         <v>34</v>
       </c>
@@ -9268,7 +9293,7 @@
       <c r="AJ18" t="s">
         <v>13</v>
       </c>
-      <c r="AK18" s="27"/>
+      <c r="AK18" s="24"/>
       <c r="AL18" t="s">
         <v>34</v>
       </c>
@@ -9278,7 +9303,7 @@
       <c r="AN18" t="s">
         <v>13</v>
       </c>
-      <c r="AO18" s="27"/>
+      <c r="AO18" s="24"/>
       <c r="AP18" t="s">
         <v>34</v>
       </c>
@@ -9288,7 +9313,7 @@
       <c r="AR18" t="s">
         <v>13</v>
       </c>
-      <c r="AS18" s="27"/>
+      <c r="AS18" s="24"/>
       <c r="AT18" t="s">
         <v>34</v>
       </c>
@@ -9300,7 +9325,7 @@
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E19" s="27"/>
+      <c r="E19" s="24"/>
       <c r="F19" t="s">
         <v>33</v>
       </c>
@@ -9310,7 +9335,7 @@
       <c r="H19" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="27"/>
+      <c r="I19" s="24"/>
       <c r="J19" t="s">
         <v>33</v>
       </c>
@@ -9320,7 +9345,7 @@
       <c r="L19" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="27"/>
+      <c r="M19" s="24"/>
       <c r="N19" t="s">
         <v>33</v>
       </c>
@@ -9330,7 +9355,7 @@
       <c r="P19" t="s">
         <v>13</v>
       </c>
-      <c r="Q19" s="27"/>
+      <c r="Q19" s="24"/>
       <c r="R19" t="s">
         <v>33</v>
       </c>
@@ -9340,7 +9365,7 @@
       <c r="T19" t="s">
         <v>13</v>
       </c>
-      <c r="U19" s="27"/>
+      <c r="U19" s="24"/>
       <c r="V19" t="s">
         <v>33</v>
       </c>
@@ -9350,7 +9375,7 @@
       <c r="X19" t="s">
         <v>13</v>
       </c>
-      <c r="Y19" s="27"/>
+      <c r="Y19" s="24"/>
       <c r="Z19" t="s">
         <v>33</v>
       </c>
@@ -9360,7 +9385,7 @@
       <c r="AB19" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="27"/>
+      <c r="AC19" s="24"/>
       <c r="AD19" t="s">
         <v>33</v>
       </c>
@@ -9370,7 +9395,7 @@
       <c r="AF19" t="s">
         <v>13</v>
       </c>
-      <c r="AG19" s="27"/>
+      <c r="AG19" s="24"/>
       <c r="AH19" t="s">
         <v>33</v>
       </c>
@@ -9380,7 +9405,7 @@
       <c r="AJ19" t="s">
         <v>13</v>
       </c>
-      <c r="AK19" s="27"/>
+      <c r="AK19" s="24"/>
       <c r="AL19" t="s">
         <v>33</v>
       </c>
@@ -9390,7 +9415,7 @@
       <c r="AN19" t="s">
         <v>13</v>
       </c>
-      <c r="AO19" s="27"/>
+      <c r="AO19" s="24"/>
       <c r="AP19" t="s">
         <v>33</v>
       </c>
@@ -9400,7 +9425,7 @@
       <c r="AR19" t="s">
         <v>13</v>
       </c>
-      <c r="AS19" s="27"/>
+      <c r="AS19" s="24"/>
       <c r="AT19" t="s">
         <v>33</v>
       </c>
@@ -9421,7 +9446,7 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="27"/>
+      <c r="E20" s="24"/>
       <c r="F20" t="s">
         <v>88</v>
       </c>
@@ -9431,7 +9456,7 @@
       <c r="H20" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="27"/>
+      <c r="I20" s="24"/>
       <c r="J20" t="s">
         <v>88</v>
       </c>
@@ -9441,7 +9466,7 @@
       <c r="L20" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="27"/>
+      <c r="M20" s="24"/>
       <c r="N20" t="s">
         <v>88</v>
       </c>
@@ -9451,7 +9476,7 @@
       <c r="P20" t="s">
         <v>13</v>
       </c>
-      <c r="Q20" s="27"/>
+      <c r="Q20" s="24"/>
       <c r="R20" t="s">
         <v>88</v>
       </c>
@@ -9461,7 +9486,7 @@
       <c r="T20" t="s">
         <v>13</v>
       </c>
-      <c r="U20" s="27"/>
+      <c r="U20" s="24"/>
       <c r="V20" t="s">
         <v>88</v>
       </c>
@@ -9471,7 +9496,7 @@
       <c r="X20" t="s">
         <v>13</v>
       </c>
-      <c r="Y20" s="27"/>
+      <c r="Y20" s="24"/>
       <c r="Z20" t="s">
         <v>88</v>
       </c>
@@ -9481,7 +9506,7 @@
       <c r="AB20" t="s">
         <v>13</v>
       </c>
-      <c r="AC20" s="27"/>
+      <c r="AC20" s="24"/>
       <c r="AD20" t="s">
         <v>88</v>
       </c>
@@ -9491,7 +9516,7 @@
       <c r="AF20" t="s">
         <v>13</v>
       </c>
-      <c r="AG20" s="27"/>
+      <c r="AG20" s="24"/>
       <c r="AH20" t="s">
         <v>88</v>
       </c>
@@ -9501,7 +9526,7 @@
       <c r="AJ20" t="s">
         <v>13</v>
       </c>
-      <c r="AK20" s="27"/>
+      <c r="AK20" s="24"/>
       <c r="AL20" t="s">
         <v>88</v>
       </c>
@@ -9511,7 +9536,7 @@
       <c r="AN20" t="s">
         <v>13</v>
       </c>
-      <c r="AO20" s="27"/>
+      <c r="AO20" s="24"/>
       <c r="AP20" t="s">
         <v>88</v>
       </c>
@@ -9521,7 +9546,7 @@
       <c r="AR20" t="s">
         <v>13</v>
       </c>
-      <c r="AS20" s="27"/>
+      <c r="AS20" s="24"/>
       <c r="AT20" t="s">
         <v>88</v>
       </c>
@@ -9542,7 +9567,7 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="27"/>
+      <c r="E21" s="24"/>
       <c r="F21" t="s">
         <v>46</v>
       </c>
@@ -9552,7 +9577,7 @@
       <c r="H21" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="27"/>
+      <c r="I21" s="24"/>
       <c r="J21" t="s">
         <v>46</v>
       </c>
@@ -9562,7 +9587,7 @@
       <c r="L21" t="s">
         <v>13</v>
       </c>
-      <c r="M21" s="27"/>
+      <c r="M21" s="24"/>
       <c r="N21" t="s">
         <v>46</v>
       </c>
@@ -9572,7 +9597,7 @@
       <c r="P21" t="s">
         <v>13</v>
       </c>
-      <c r="Q21" s="27"/>
+      <c r="Q21" s="24"/>
       <c r="R21" t="s">
         <v>46</v>
       </c>
@@ -9582,7 +9607,7 @@
       <c r="T21" t="s">
         <v>13</v>
       </c>
-      <c r="U21" s="27"/>
+      <c r="U21" s="24"/>
       <c r="V21" t="s">
         <v>46</v>
       </c>
@@ -9592,7 +9617,7 @@
       <c r="X21" t="s">
         <v>13</v>
       </c>
-      <c r="Y21" s="27"/>
+      <c r="Y21" s="24"/>
       <c r="Z21" t="s">
         <v>46</v>
       </c>
@@ -9602,7 +9627,7 @@
       <c r="AB21" t="s">
         <v>13</v>
       </c>
-      <c r="AC21" s="27"/>
+      <c r="AC21" s="24"/>
       <c r="AD21" t="s">
         <v>46</v>
       </c>
@@ -9612,7 +9637,7 @@
       <c r="AF21" t="s">
         <v>13</v>
       </c>
-      <c r="AG21" s="27"/>
+      <c r="AG21" s="24"/>
       <c r="AH21" t="s">
         <v>46</v>
       </c>
@@ -9622,7 +9647,7 @@
       <c r="AJ21" t="s">
         <v>13</v>
       </c>
-      <c r="AK21" s="27"/>
+      <c r="AK21" s="24"/>
       <c r="AL21" t="s">
         <v>46</v>
       </c>
@@ -9632,7 +9657,7 @@
       <c r="AN21" t="s">
         <v>13</v>
       </c>
-      <c r="AO21" s="27"/>
+      <c r="AO21" s="24"/>
       <c r="AP21" t="s">
         <v>46</v>
       </c>
@@ -9642,7 +9667,7 @@
       <c r="AR21" t="s">
         <v>13</v>
       </c>
-      <c r="AS21" s="27"/>
+      <c r="AS21" s="24"/>
       <c r="AT21" t="s">
         <v>46</v>
       </c>
@@ -9663,7 +9688,7 @@
       <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="27"/>
+      <c r="E22" s="24"/>
       <c r="F22" t="s">
         <v>89</v>
       </c>
@@ -9673,7 +9698,7 @@
       <c r="H22" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="27"/>
+      <c r="I22" s="24"/>
       <c r="J22" t="s">
         <v>89</v>
       </c>
@@ -9683,7 +9708,7 @@
       <c r="L22" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="27"/>
+      <c r="M22" s="24"/>
       <c r="N22" t="s">
         <v>89</v>
       </c>
@@ -9693,7 +9718,7 @@
       <c r="P22" t="s">
         <v>13</v>
       </c>
-      <c r="Q22" s="27"/>
+      <c r="Q22" s="24"/>
       <c r="R22" t="s">
         <v>89</v>
       </c>
@@ -9703,7 +9728,7 @@
       <c r="T22" t="s">
         <v>13</v>
       </c>
-      <c r="U22" s="27"/>
+      <c r="U22" s="24"/>
       <c r="V22" t="s">
         <v>89</v>
       </c>
@@ -9713,7 +9738,7 @@
       <c r="X22" t="s">
         <v>13</v>
       </c>
-      <c r="Y22" s="27"/>
+      <c r="Y22" s="24"/>
       <c r="Z22" t="s">
         <v>89</v>
       </c>
@@ -9723,7 +9748,7 @@
       <c r="AB22" t="s">
         <v>13</v>
       </c>
-      <c r="AC22" s="27"/>
+      <c r="AC22" s="24"/>
       <c r="AD22" t="s">
         <v>89</v>
       </c>
@@ -9733,7 +9758,7 @@
       <c r="AF22" t="s">
         <v>13</v>
       </c>
-      <c r="AG22" s="27"/>
+      <c r="AG22" s="24"/>
       <c r="AH22" t="s">
         <v>89</v>
       </c>
@@ -9743,7 +9768,7 @@
       <c r="AJ22" t="s">
         <v>13</v>
       </c>
-      <c r="AK22" s="27"/>
+      <c r="AK22" s="24"/>
       <c r="AL22" t="s">
         <v>89</v>
       </c>
@@ -9753,7 +9778,7 @@
       <c r="AN22" t="s">
         <v>13</v>
       </c>
-      <c r="AO22" s="27"/>
+      <c r="AO22" s="24"/>
       <c r="AP22" t="s">
         <v>89</v>
       </c>
@@ -9763,7 +9788,7 @@
       <c r="AR22" t="s">
         <v>13</v>
       </c>
-      <c r="AS22" s="27"/>
+      <c r="AS22" s="24"/>
       <c r="AT22" t="s">
         <v>89</v>
       </c>
@@ -9785,7 +9810,7 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="27"/>
+      <c r="E23" s="24"/>
       <c r="F23" t="s">
         <v>90</v>
       </c>
@@ -9795,7 +9820,7 @@
       <c r="H23" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="27"/>
+      <c r="I23" s="24"/>
       <c r="J23" t="s">
         <v>90</v>
       </c>
@@ -9805,7 +9830,7 @@
       <c r="L23" t="s">
         <v>13</v>
       </c>
-      <c r="M23" s="27"/>
+      <c r="M23" s="24"/>
       <c r="N23" t="s">
         <v>90</v>
       </c>
@@ -9815,7 +9840,7 @@
       <c r="P23" t="s">
         <v>13</v>
       </c>
-      <c r="Q23" s="27"/>
+      <c r="Q23" s="24"/>
       <c r="R23" t="s">
         <v>90</v>
       </c>
@@ -9825,7 +9850,7 @@
       <c r="T23" t="s">
         <v>13</v>
       </c>
-      <c r="U23" s="27"/>
+      <c r="U23" s="24"/>
       <c r="V23" t="s">
         <v>90</v>
       </c>
@@ -9835,7 +9860,7 @@
       <c r="X23" t="s">
         <v>13</v>
       </c>
-      <c r="Y23" s="27"/>
+      <c r="Y23" s="24"/>
       <c r="Z23" t="s">
         <v>90</v>
       </c>
@@ -9845,7 +9870,7 @@
       <c r="AB23" t="s">
         <v>13</v>
       </c>
-      <c r="AC23" s="27"/>
+      <c r="AC23" s="24"/>
       <c r="AD23" t="s">
         <v>90</v>
       </c>
@@ -9855,7 +9880,7 @@
       <c r="AF23" t="s">
         <v>13</v>
       </c>
-      <c r="AG23" s="27"/>
+      <c r="AG23" s="24"/>
       <c r="AH23" t="s">
         <v>90</v>
       </c>
@@ -9865,7 +9890,7 @@
       <c r="AJ23" t="s">
         <v>13</v>
       </c>
-      <c r="AK23" s="27"/>
+      <c r="AK23" s="24"/>
       <c r="AL23" t="s">
         <v>90</v>
       </c>
@@ -9875,7 +9900,7 @@
       <c r="AN23" t="s">
         <v>13</v>
       </c>
-      <c r="AO23" s="27"/>
+      <c r="AO23" s="24"/>
       <c r="AP23" t="s">
         <v>90</v>
       </c>
@@ -9885,7 +9910,7 @@
       <c r="AR23" t="s">
         <v>13</v>
       </c>
-      <c r="AS23" s="27"/>
+      <c r="AS23" s="24"/>
       <c r="AT23" t="s">
         <v>90</v>
       </c>
@@ -9897,7 +9922,7 @@
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E24" s="27"/>
+      <c r="E24" s="24"/>
       <c r="F24" t="s">
         <v>9</v>
       </c>
@@ -9907,7 +9932,7 @@
       <c r="H24" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="27"/>
+      <c r="I24" s="24"/>
       <c r="J24" t="s">
         <v>9</v>
       </c>
@@ -9917,7 +9942,7 @@
       <c r="L24" t="s">
         <v>13</v>
       </c>
-      <c r="M24" s="27"/>
+      <c r="M24" s="24"/>
       <c r="N24" t="s">
         <v>9</v>
       </c>
@@ -9927,7 +9952,7 @@
       <c r="P24" t="s">
         <v>13</v>
       </c>
-      <c r="Q24" s="27"/>
+      <c r="Q24" s="24"/>
       <c r="R24" t="s">
         <v>9</v>
       </c>
@@ -9937,7 +9962,7 @@
       <c r="T24" t="s">
         <v>13</v>
       </c>
-      <c r="U24" s="27"/>
+      <c r="U24" s="24"/>
       <c r="V24" t="s">
         <v>9</v>
       </c>
@@ -9947,7 +9972,7 @@
       <c r="X24" t="s">
         <v>13</v>
       </c>
-      <c r="Y24" s="27"/>
+      <c r="Y24" s="24"/>
       <c r="Z24" t="s">
         <v>9</v>
       </c>
@@ -9957,7 +9982,7 @@
       <c r="AB24" t="s">
         <v>13</v>
       </c>
-      <c r="AC24" s="27"/>
+      <c r="AC24" s="24"/>
       <c r="AD24" t="s">
         <v>9</v>
       </c>
@@ -9967,7 +9992,7 @@
       <c r="AF24" t="s">
         <v>13</v>
       </c>
-      <c r="AG24" s="27"/>
+      <c r="AG24" s="24"/>
       <c r="AH24" t="s">
         <v>9</v>
       </c>
@@ -9977,7 +10002,7 @@
       <c r="AJ24" t="s">
         <v>13</v>
       </c>
-      <c r="AK24" s="27"/>
+      <c r="AK24" s="24"/>
       <c r="AL24" t="s">
         <v>9</v>
       </c>
@@ -9987,7 +10012,7 @@
       <c r="AN24" t="s">
         <v>13</v>
       </c>
-      <c r="AO24" s="27"/>
+      <c r="AO24" s="24"/>
       <c r="AP24" t="s">
         <v>9</v>
       </c>
@@ -9997,7 +10022,7 @@
       <c r="AR24" t="s">
         <v>13</v>
       </c>
-      <c r="AS24" s="27"/>
+      <c r="AS24" s="24"/>
       <c r="AT24" t="s">
         <v>9</v>
       </c>
@@ -10009,7 +10034,7 @@
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E25" s="27"/>
+      <c r="E25" s="24"/>
       <c r="F25" t="s">
         <v>91</v>
       </c>
@@ -10019,7 +10044,7 @@
       <c r="H25" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="27"/>
+      <c r="I25" s="24"/>
       <c r="J25" t="s">
         <v>91</v>
       </c>
@@ -10029,7 +10054,7 @@
       <c r="L25" t="s">
         <v>13</v>
       </c>
-      <c r="M25" s="27"/>
+      <c r="M25" s="24"/>
       <c r="N25" t="s">
         <v>91</v>
       </c>
@@ -10039,7 +10064,7 @@
       <c r="P25" t="s">
         <v>13</v>
       </c>
-      <c r="Q25" s="27"/>
+      <c r="Q25" s="24"/>
       <c r="R25" t="s">
         <v>91</v>
       </c>
@@ -10049,7 +10074,7 @@
       <c r="T25" t="s">
         <v>13</v>
       </c>
-      <c r="U25" s="27"/>
+      <c r="U25" s="24"/>
       <c r="V25" t="s">
         <v>91</v>
       </c>
@@ -10059,7 +10084,7 @@
       <c r="X25" t="s">
         <v>13</v>
       </c>
-      <c r="Y25" s="27"/>
+      <c r="Y25" s="24"/>
       <c r="Z25" t="s">
         <v>91</v>
       </c>
@@ -10069,7 +10094,7 @@
       <c r="AB25" t="s">
         <v>13</v>
       </c>
-      <c r="AC25" s="27"/>
+      <c r="AC25" s="24"/>
       <c r="AD25" t="s">
         <v>91</v>
       </c>
@@ -10079,7 +10104,7 @@
       <c r="AF25" t="s">
         <v>13</v>
       </c>
-      <c r="AG25" s="27"/>
+      <c r="AG25" s="24"/>
       <c r="AH25" t="s">
         <v>91</v>
       </c>
@@ -10089,7 +10114,7 @@
       <c r="AJ25" t="s">
         <v>13</v>
       </c>
-      <c r="AK25" s="27"/>
+      <c r="AK25" s="24"/>
       <c r="AL25" t="s">
         <v>91</v>
       </c>
@@ -10099,7 +10124,7 @@
       <c r="AN25" t="s">
         <v>13</v>
       </c>
-      <c r="AO25" s="27"/>
+      <c r="AO25" s="24"/>
       <c r="AP25" t="s">
         <v>91</v>
       </c>
@@ -10109,7 +10134,7 @@
       <c r="AR25" t="s">
         <v>13</v>
       </c>
-      <c r="AS25" s="27"/>
+      <c r="AS25" s="24"/>
       <c r="AT25" t="s">
         <v>91</v>
       </c>
@@ -10122,7 +10147,7 @@
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -10138,7 +10163,7 @@
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29" s="13">
         <f>G14+G15+G16+G17+G18+G19</f>
@@ -10150,7 +10175,7 @@
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" s="13">
         <f>C18-F28</f>
@@ -10159,10 +10184,11 @@
       <c r="G30" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F31" s="13">
         <f>C20+C21-F29</f>
@@ -10255,8 +10281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8612F4-CCB1-4696-8897-C4C5EFBE3F4E}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10386,7 +10412,7 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="24"/>
       <c r="F2" t="s">
         <v>124</v>
       </c>
@@ -10396,7 +10422,7 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="27"/>
+      <c r="I2" s="24"/>
       <c r="J2" t="s">
         <v>124</v>
       </c>
@@ -10406,7 +10432,7 @@
       <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="27"/>
+      <c r="M2" s="24"/>
       <c r="N2" t="s">
         <v>124</v>
       </c>
@@ -10416,7 +10442,7 @@
       <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="27"/>
+      <c r="Q2" s="24"/>
       <c r="R2" t="s">
         <v>124</v>
       </c>
@@ -10426,7 +10452,7 @@
       <c r="T2" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="27"/>
+      <c r="U2" s="24"/>
       <c r="V2" t="s">
         <v>124</v>
       </c>
@@ -10436,7 +10462,7 @@
       <c r="X2" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="27"/>
+      <c r="Y2" s="24"/>
       <c r="Z2" t="s">
         <v>124</v>
       </c>
@@ -10446,7 +10472,7 @@
       <c r="AB2" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="27"/>
+      <c r="AC2" s="24"/>
       <c r="AD2" t="s">
         <v>124</v>
       </c>
@@ -10456,7 +10482,7 @@
       <c r="AF2" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="27"/>
+      <c r="AG2" s="24"/>
       <c r="AH2" t="s">
         <v>124</v>
       </c>
@@ -10466,7 +10492,7 @@
       <c r="AJ2" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="27"/>
+      <c r="AK2" s="24"/>
       <c r="AL2" t="s">
         <v>124</v>
       </c>
@@ -10476,7 +10502,7 @@
       <c r="AN2" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="27"/>
+      <c r="AO2" s="24"/>
       <c r="AP2" t="s">
         <v>124</v>
       </c>
@@ -10486,7 +10512,7 @@
       <c r="AR2" t="s">
         <v>13</v>
       </c>
-      <c r="AS2" s="27"/>
+      <c r="AS2" s="24"/>
       <c r="AT2" t="s">
         <v>124</v>
       </c>
@@ -10507,7 +10533,7 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="24"/>
       <c r="F3" t="s">
         <v>77</v>
       </c>
@@ -10517,7 +10543,7 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="27"/>
+      <c r="I3" s="24"/>
       <c r="J3" t="s">
         <v>77</v>
       </c>
@@ -10527,7 +10553,7 @@
       <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="27"/>
+      <c r="M3" s="24"/>
       <c r="N3" t="s">
         <v>77</v>
       </c>
@@ -10537,7 +10563,7 @@
       <c r="P3" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="27"/>
+      <c r="Q3" s="24"/>
       <c r="R3" t="s">
         <v>77</v>
       </c>
@@ -10547,7 +10573,7 @@
       <c r="T3" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="27"/>
+      <c r="U3" s="24"/>
       <c r="V3" t="s">
         <v>77</v>
       </c>
@@ -10557,7 +10583,7 @@
       <c r="X3" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="27"/>
+      <c r="Y3" s="24"/>
       <c r="Z3" t="s">
         <v>127</v>
       </c>
@@ -10567,7 +10593,7 @@
       <c r="AB3" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="27"/>
+      <c r="AC3" s="24"/>
       <c r="AD3" t="s">
         <v>127</v>
       </c>
@@ -10577,7 +10603,7 @@
       <c r="AF3" t="s">
         <v>13</v>
       </c>
-      <c r="AG3" s="27"/>
+      <c r="AG3" s="24"/>
       <c r="AH3" t="s">
         <v>127</v>
       </c>
@@ -10587,7 +10613,7 @@
       <c r="AJ3" t="s">
         <v>13</v>
       </c>
-      <c r="AK3" s="27"/>
+      <c r="AK3" s="24"/>
       <c r="AL3" t="s">
         <v>127</v>
       </c>
@@ -10597,7 +10623,7 @@
       <c r="AN3" t="s">
         <v>13</v>
       </c>
-      <c r="AO3" s="27"/>
+      <c r="AO3" s="24"/>
       <c r="AP3" t="s">
         <v>127</v>
       </c>
@@ -10607,7 +10633,7 @@
       <c r="AR3" t="s">
         <v>13</v>
       </c>
-      <c r="AS3" s="27"/>
+      <c r="AS3" s="24"/>
       <c r="AT3" t="s">
         <v>127</v>
       </c>
@@ -10628,7 +10654,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="24"/>
       <c r="F4" t="s">
         <v>125</v>
       </c>
@@ -10638,7 +10664,7 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="27"/>
+      <c r="I4" s="24"/>
       <c r="J4" t="s">
         <v>125</v>
       </c>
@@ -10648,7 +10674,7 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="27"/>
+      <c r="M4" s="24"/>
       <c r="N4" t="s">
         <v>125</v>
       </c>
@@ -10658,7 +10684,7 @@
       <c r="P4" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="27"/>
+      <c r="Q4" s="24"/>
       <c r="R4" t="s">
         <v>125</v>
       </c>
@@ -10668,7 +10694,7 @@
       <c r="T4" t="s">
         <v>13</v>
       </c>
-      <c r="U4" s="27"/>
+      <c r="U4" s="24"/>
       <c r="V4" t="s">
         <v>125</v>
       </c>
@@ -10678,7 +10704,7 @@
       <c r="X4" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="27"/>
+      <c r="Y4" s="24"/>
       <c r="Z4" t="s">
         <v>2</v>
       </c>
@@ -10688,7 +10714,7 @@
       <c r="AB4" t="s">
         <v>13</v>
       </c>
-      <c r="AC4" s="27"/>
+      <c r="AC4" s="24"/>
       <c r="AD4" t="s">
         <v>2</v>
       </c>
@@ -10698,7 +10724,7 @@
       <c r="AF4" t="s">
         <v>13</v>
       </c>
-      <c r="AG4" s="27"/>
+      <c r="AG4" s="24"/>
       <c r="AH4" t="s">
         <v>2</v>
       </c>
@@ -10708,7 +10734,7 @@
       <c r="AJ4" t="s">
         <v>13</v>
       </c>
-      <c r="AK4" s="27"/>
+      <c r="AK4" s="24"/>
       <c r="AL4" t="s">
         <v>2</v>
       </c>
@@ -10718,7 +10744,7 @@
       <c r="AN4" t="s">
         <v>13</v>
       </c>
-      <c r="AO4" s="27"/>
+      <c r="AO4" s="24"/>
       <c r="AP4" t="s">
         <v>2</v>
       </c>
@@ -10728,7 +10754,7 @@
       <c r="AR4" t="s">
         <v>13</v>
       </c>
-      <c r="AS4" s="27"/>
+      <c r="AS4" s="24"/>
       <c r="AT4" t="s">
         <v>2</v>
       </c>
@@ -10749,7 +10775,7 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="24"/>
       <c r="F5" t="s">
         <v>126</v>
       </c>
@@ -10759,7 +10785,7 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="24"/>
       <c r="J5" t="s">
         <v>126</v>
       </c>
@@ -10769,7 +10795,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="27"/>
+      <c r="M5" s="24"/>
       <c r="N5" t="s">
         <v>126</v>
       </c>
@@ -10779,7 +10805,7 @@
       <c r="P5" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="27"/>
+      <c r="Q5" s="24"/>
       <c r="R5" t="s">
         <v>126</v>
       </c>
@@ -10789,7 +10815,7 @@
       <c r="T5" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="27"/>
+      <c r="U5" s="24"/>
       <c r="V5" t="s">
         <v>126</v>
       </c>
@@ -10799,7 +10825,7 @@
       <c r="X5" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="27"/>
+      <c r="Y5" s="24"/>
       <c r="Z5" t="s">
         <v>3</v>
       </c>
@@ -10809,7 +10835,7 @@
       <c r="AB5" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="27"/>
+      <c r="AC5" s="24"/>
       <c r="AD5" t="s">
         <v>3</v>
       </c>
@@ -10819,7 +10845,7 @@
       <c r="AF5" t="s">
         <v>13</v>
       </c>
-      <c r="AG5" s="27"/>
+      <c r="AG5" s="24"/>
       <c r="AH5" t="s">
         <v>3</v>
       </c>
@@ -10829,7 +10855,7 @@
       <c r="AJ5" t="s">
         <v>13</v>
       </c>
-      <c r="AK5" s="27"/>
+      <c r="AK5" s="24"/>
       <c r="AL5" t="s">
         <v>3</v>
       </c>
@@ -10839,7 +10865,7 @@
       <c r="AN5" t="s">
         <v>13</v>
       </c>
-      <c r="AO5" s="27"/>
+      <c r="AO5" s="24"/>
       <c r="AP5" t="s">
         <v>3</v>
       </c>
@@ -10849,7 +10875,7 @@
       <c r="AR5" t="s">
         <v>13</v>
       </c>
-      <c r="AS5" s="27"/>
+      <c r="AS5" s="24"/>
       <c r="AT5" t="s">
         <v>3</v>
       </c>
@@ -10870,7 +10896,7 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="24"/>
       <c r="F6" t="s">
         <v>127</v>
       </c>
@@ -10880,7 +10906,7 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="24"/>
       <c r="J6" t="s">
         <v>127</v>
       </c>
@@ -10890,7 +10916,7 @@
       <c r="L6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="27"/>
+      <c r="M6" s="24"/>
       <c r="N6" t="s">
         <v>127</v>
       </c>
@@ -10900,7 +10926,7 @@
       <c r="P6" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="24"/>
       <c r="R6" t="s">
         <v>127</v>
       </c>
@@ -10910,7 +10936,7 @@
       <c r="T6" t="s">
         <v>13</v>
       </c>
-      <c r="U6" s="27"/>
+      <c r="U6" s="24"/>
       <c r="V6" t="s">
         <v>127</v>
       </c>
@@ -10920,7 +10946,7 @@
       <c r="X6" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="27"/>
+      <c r="Y6" s="24"/>
       <c r="Z6" t="s">
         <v>128</v>
       </c>
@@ -10930,7 +10956,7 @@
       <c r="AB6" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="27"/>
+      <c r="AC6" s="24"/>
       <c r="AD6" t="s">
         <v>128</v>
       </c>
@@ -10940,7 +10966,7 @@
       <c r="AF6" t="s">
         <v>13</v>
       </c>
-      <c r="AG6" s="27"/>
+      <c r="AG6" s="24"/>
       <c r="AH6" t="s">
         <v>128</v>
       </c>
@@ -10950,7 +10976,7 @@
       <c r="AJ6" t="s">
         <v>13</v>
       </c>
-      <c r="AK6" s="27"/>
+      <c r="AK6" s="24"/>
       <c r="AL6" t="s">
         <v>128</v>
       </c>
@@ -10960,7 +10986,7 @@
       <c r="AN6" t="s">
         <v>13</v>
       </c>
-      <c r="AO6" s="27"/>
+      <c r="AO6" s="24"/>
       <c r="AP6" t="s">
         <v>128</v>
       </c>
@@ -10970,7 +10996,7 @@
       <c r="AR6" t="s">
         <v>13</v>
       </c>
-      <c r="AS6" s="27"/>
+      <c r="AS6" s="24"/>
       <c r="AT6" t="s">
         <v>128</v>
       </c>
@@ -10991,7 +11017,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="24"/>
       <c r="F7" t="s">
         <v>2</v>
       </c>
@@ -11001,7 +11027,7 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="27"/>
+      <c r="I7" s="24"/>
       <c r="J7" t="s">
         <v>2</v>
       </c>
@@ -11011,7 +11037,7 @@
       <c r="L7" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="27"/>
+      <c r="M7" s="24"/>
       <c r="N7" t="s">
         <v>2</v>
       </c>
@@ -11021,7 +11047,7 @@
       <c r="P7" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="27"/>
+      <c r="Q7" s="24"/>
       <c r="R7" t="s">
         <v>2</v>
       </c>
@@ -11031,7 +11057,7 @@
       <c r="T7" t="s">
         <v>13</v>
       </c>
-      <c r="U7" s="27"/>
+      <c r="U7" s="24"/>
       <c r="V7" t="s">
         <v>2</v>
       </c>
@@ -11041,7 +11067,7 @@
       <c r="X7" t="s">
         <v>13</v>
       </c>
-      <c r="Y7" s="27"/>
+      <c r="Y7" s="24"/>
       <c r="Z7" t="s">
         <v>33</v>
       </c>
@@ -11051,7 +11077,7 @@
       <c r="AB7" t="s">
         <v>13</v>
       </c>
-      <c r="AC7" s="27"/>
+      <c r="AC7" s="24"/>
       <c r="AD7" t="s">
         <v>33</v>
       </c>
@@ -11061,7 +11087,7 @@
       <c r="AF7" t="s">
         <v>13</v>
       </c>
-      <c r="AG7" s="27"/>
+      <c r="AG7" s="24"/>
       <c r="AH7" t="s">
         <v>33</v>
       </c>
@@ -11071,7 +11097,7 @@
       <c r="AJ7" t="s">
         <v>13</v>
       </c>
-      <c r="AK7" s="27"/>
+      <c r="AK7" s="24"/>
       <c r="AL7" t="s">
         <v>33</v>
       </c>
@@ -11081,7 +11107,7 @@
       <c r="AN7" t="s">
         <v>13</v>
       </c>
-      <c r="AO7" s="27"/>
+      <c r="AO7" s="24"/>
       <c r="AP7" t="s">
         <v>33</v>
       </c>
@@ -11091,7 +11117,7 @@
       <c r="AR7" t="s">
         <v>13</v>
       </c>
-      <c r="AS7" s="27"/>
+      <c r="AS7" s="24"/>
       <c r="AT7" t="s">
         <v>33</v>
       </c>
@@ -11112,7 +11138,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="24"/>
       <c r="F8" t="s">
         <v>3</v>
       </c>
@@ -11122,7 +11148,7 @@
       <c r="H8" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="I8" s="24"/>
       <c r="J8" t="s">
         <v>3</v>
       </c>
@@ -11132,7 +11158,7 @@
       <c r="L8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="27"/>
+      <c r="M8" s="24"/>
       <c r="N8" t="s">
         <v>3</v>
       </c>
@@ -11142,7 +11168,7 @@
       <c r="P8" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="27"/>
+      <c r="Q8" s="24"/>
       <c r="R8" t="s">
         <v>3</v>
       </c>
@@ -11152,7 +11178,7 @@
       <c r="T8" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="27"/>
+      <c r="U8" s="24"/>
       <c r="V8" t="s">
         <v>3</v>
       </c>
@@ -11162,7 +11188,7 @@
       <c r="X8" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="27"/>
+      <c r="Y8" s="24"/>
       <c r="Z8" t="s">
         <v>34</v>
       </c>
@@ -11172,7 +11198,7 @@
       <c r="AB8" t="s">
         <v>13</v>
       </c>
-      <c r="AC8" s="27"/>
+      <c r="AC8" s="24"/>
       <c r="AD8" t="s">
         <v>34</v>
       </c>
@@ -11182,7 +11208,7 @@
       <c r="AF8" t="s">
         <v>13</v>
       </c>
-      <c r="AG8" s="27"/>
+      <c r="AG8" s="24"/>
       <c r="AH8" t="s">
         <v>34</v>
       </c>
@@ -11192,7 +11218,7 @@
       <c r="AJ8" t="s">
         <v>13</v>
       </c>
-      <c r="AK8" s="27"/>
+      <c r="AK8" s="24"/>
       <c r="AL8" t="s">
         <v>34</v>
       </c>
@@ -11202,7 +11228,7 @@
       <c r="AN8" t="s">
         <v>13</v>
       </c>
-      <c r="AO8" s="27"/>
+      <c r="AO8" s="24"/>
       <c r="AP8" t="s">
         <v>34</v>
       </c>
@@ -11212,7 +11238,7 @@
       <c r="AR8" t="s">
         <v>13</v>
       </c>
-      <c r="AS8" s="27"/>
+      <c r="AS8" s="24"/>
       <c r="AT8" t="s">
         <v>34</v>
       </c>
@@ -11233,7 +11259,7 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="27"/>
+      <c r="E9" s="24"/>
       <c r="F9" t="s">
         <v>128</v>
       </c>
@@ -11243,7 +11269,7 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="27"/>
+      <c r="I9" s="24"/>
       <c r="J9" t="s">
         <v>128</v>
       </c>
@@ -11253,7 +11279,7 @@
       <c r="L9" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="27"/>
+      <c r="M9" s="24"/>
       <c r="N9" t="s">
         <v>128</v>
       </c>
@@ -11263,7 +11289,7 @@
       <c r="P9" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="27"/>
+      <c r="Q9" s="24"/>
       <c r="R9" t="s">
         <v>128</v>
       </c>
@@ -11273,7 +11299,7 @@
       <c r="T9" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="27"/>
+      <c r="U9" s="24"/>
       <c r="V9" t="s">
         <v>128</v>
       </c>
@@ -11283,7 +11309,7 @@
       <c r="X9" t="s">
         <v>13</v>
       </c>
-      <c r="Y9" s="27"/>
+      <c r="Y9" s="24"/>
       <c r="Z9" t="s">
         <v>129</v>
       </c>
@@ -11293,7 +11319,7 @@
       <c r="AB9" t="s">
         <v>13</v>
       </c>
-      <c r="AC9" s="27"/>
+      <c r="AC9" s="24"/>
       <c r="AD9" t="s">
         <v>129</v>
       </c>
@@ -11303,7 +11329,7 @@
       <c r="AF9" t="s">
         <v>13</v>
       </c>
-      <c r="AG9" s="27"/>
+      <c r="AG9" s="24"/>
       <c r="AH9" t="s">
         <v>129</v>
       </c>
@@ -11313,7 +11339,7 @@
       <c r="AJ9" t="s">
         <v>13</v>
       </c>
-      <c r="AK9" s="27"/>
+      <c r="AK9" s="24"/>
       <c r="AL9" t="s">
         <v>129</v>
       </c>
@@ -11323,7 +11349,7 @@
       <c r="AN9" t="s">
         <v>13</v>
       </c>
-      <c r="AO9" s="27"/>
+      <c r="AO9" s="24"/>
       <c r="AP9" t="s">
         <v>129</v>
       </c>
@@ -11333,7 +11359,7 @@
       <c r="AR9" t="s">
         <v>13</v>
       </c>
-      <c r="AS9" s="27"/>
+      <c r="AS9" s="24"/>
       <c r="AT9" t="s">
         <v>129</v>
       </c>
@@ -11354,7 +11380,7 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="24"/>
       <c r="F10" t="s">
         <v>33</v>
       </c>
@@ -11364,7 +11390,7 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="27"/>
+      <c r="I10" s="24"/>
       <c r="J10" t="s">
         <v>33</v>
       </c>
@@ -11374,7 +11400,7 @@
       <c r="L10" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="27"/>
+      <c r="M10" s="24"/>
       <c r="N10" t="s">
         <v>33</v>
       </c>
@@ -11384,7 +11410,7 @@
       <c r="P10" t="s">
         <v>13</v>
       </c>
-      <c r="Q10" s="27"/>
+      <c r="Q10" s="24"/>
       <c r="R10" t="s">
         <v>33</v>
       </c>
@@ -11394,7 +11420,7 @@
       <c r="T10" t="s">
         <v>13</v>
       </c>
-      <c r="U10" s="27"/>
+      <c r="U10" s="24"/>
       <c r="V10" t="s">
         <v>33</v>
       </c>
@@ -11404,7 +11430,7 @@
       <c r="X10" t="s">
         <v>13</v>
       </c>
-      <c r="Y10" s="27"/>
+      <c r="Y10" s="24"/>
       <c r="Z10" t="s">
         <v>46</v>
       </c>
@@ -11414,7 +11440,7 @@
       <c r="AB10" t="s">
         <v>13</v>
       </c>
-      <c r="AC10" s="27"/>
+      <c r="AC10" s="24"/>
       <c r="AD10" t="s">
         <v>46</v>
       </c>
@@ -11424,7 +11450,7 @@
       <c r="AF10" t="s">
         <v>13</v>
       </c>
-      <c r="AG10" s="27"/>
+      <c r="AG10" s="24"/>
       <c r="AH10" t="s">
         <v>46</v>
       </c>
@@ -11434,7 +11460,7 @@
       <c r="AJ10" t="s">
         <v>13</v>
       </c>
-      <c r="AK10" s="27"/>
+      <c r="AK10" s="24"/>
       <c r="AL10" t="s">
         <v>46</v>
       </c>
@@ -11444,7 +11470,7 @@
       <c r="AN10" t="s">
         <v>13</v>
       </c>
-      <c r="AO10" s="27"/>
+      <c r="AO10" s="24"/>
       <c r="AP10" t="s">
         <v>46</v>
       </c>
@@ -11454,7 +11480,7 @@
       <c r="AR10" t="s">
         <v>13</v>
       </c>
-      <c r="AS10" s="27"/>
+      <c r="AS10" s="24"/>
       <c r="AT10" t="s">
         <v>46</v>
       </c>
@@ -11475,7 +11501,7 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="27"/>
+      <c r="E11" s="24"/>
       <c r="F11" t="s">
         <v>34</v>
       </c>
@@ -11485,7 +11511,7 @@
       <c r="H11" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="27"/>
+      <c r="I11" s="24"/>
       <c r="J11" t="s">
         <v>34</v>
       </c>
@@ -11495,7 +11521,7 @@
       <c r="L11" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="27"/>
+      <c r="M11" s="24"/>
       <c r="N11" t="s">
         <v>34</v>
       </c>
@@ -11505,7 +11531,7 @@
       <c r="P11" t="s">
         <v>13</v>
       </c>
-      <c r="Q11" s="27"/>
+      <c r="Q11" s="24"/>
       <c r="R11" t="s">
         <v>34</v>
       </c>
@@ -11515,7 +11541,7 @@
       <c r="T11" t="s">
         <v>13</v>
       </c>
-      <c r="U11" s="27"/>
+      <c r="U11" s="24"/>
       <c r="V11" t="s">
         <v>34</v>
       </c>
@@ -11525,7 +11551,7 @@
       <c r="X11" t="s">
         <v>13</v>
       </c>
-      <c r="Y11" s="27"/>
+      <c r="Y11" s="24"/>
       <c r="Z11" t="s">
         <v>90</v>
       </c>
@@ -11535,7 +11561,7 @@
       <c r="AB11" t="s">
         <v>13</v>
       </c>
-      <c r="AC11" s="27"/>
+      <c r="AC11" s="24"/>
       <c r="AD11" t="s">
         <v>90</v>
       </c>
@@ -11545,7 +11571,7 @@
       <c r="AF11" t="s">
         <v>13</v>
       </c>
-      <c r="AG11" s="27"/>
+      <c r="AG11" s="24"/>
       <c r="AH11" t="s">
         <v>90</v>
       </c>
@@ -11555,7 +11581,7 @@
       <c r="AJ11" t="s">
         <v>13</v>
       </c>
-      <c r="AK11" s="27"/>
+      <c r="AK11" s="24"/>
       <c r="AL11" t="s">
         <v>90</v>
       </c>
@@ -11565,7 +11591,7 @@
       <c r="AN11" t="s">
         <v>13</v>
       </c>
-      <c r="AO11" s="27"/>
+      <c r="AO11" s="24"/>
       <c r="AP11" t="s">
         <v>90</v>
       </c>
@@ -11575,7 +11601,7 @@
       <c r="AR11" t="s">
         <v>13</v>
       </c>
-      <c r="AS11" s="27"/>
+      <c r="AS11" s="24"/>
       <c r="AT11" t="s">
         <v>90</v>
       </c>
@@ -11596,7 +11622,7 @@
       <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="24"/>
       <c r="F12" t="s">
         <v>129</v>
       </c>
@@ -11606,7 +11632,7 @@
       <c r="H12" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="27"/>
+      <c r="I12" s="24"/>
       <c r="J12" t="s">
         <v>129</v>
       </c>
@@ -11616,7 +11642,7 @@
       <c r="L12" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="27"/>
+      <c r="M12" s="24"/>
       <c r="N12" t="s">
         <v>129</v>
       </c>
@@ -11626,7 +11652,7 @@
       <c r="P12" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="27"/>
+      <c r="Q12" s="24"/>
       <c r="R12" t="s">
         <v>129</v>
       </c>
@@ -11636,7 +11662,7 @@
       <c r="T12" t="s">
         <v>13</v>
       </c>
-      <c r="U12" s="27"/>
+      <c r="U12" s="24"/>
       <c r="V12" t="s">
         <v>129</v>
       </c>
@@ -11646,7 +11672,7 @@
       <c r="X12" t="s">
         <v>13</v>
       </c>
-      <c r="Y12" s="27"/>
+      <c r="Y12" s="24"/>
       <c r="Z12" t="s">
         <v>130</v>
       </c>
@@ -11656,7 +11682,7 @@
       <c r="AB12" t="s">
         <v>13</v>
       </c>
-      <c r="AC12" s="27"/>
+      <c r="AC12" s="24"/>
       <c r="AD12" t="s">
         <v>130</v>
       </c>
@@ -11666,7 +11692,7 @@
       <c r="AF12" t="s">
         <v>13</v>
       </c>
-      <c r="AG12" s="27"/>
+      <c r="AG12" s="24"/>
       <c r="AH12" t="s">
         <v>130</v>
       </c>
@@ -11676,7 +11702,7 @@
       <c r="AJ12" t="s">
         <v>13</v>
       </c>
-      <c r="AK12" s="27"/>
+      <c r="AK12" s="24"/>
       <c r="AL12" t="s">
         <v>130</v>
       </c>
@@ -11686,7 +11712,7 @@
       <c r="AN12" t="s">
         <v>13</v>
       </c>
-      <c r="AO12" s="27"/>
+      <c r="AO12" s="24"/>
       <c r="AP12" t="s">
         <v>130</v>
       </c>
@@ -11696,7 +11722,7 @@
       <c r="AR12" t="s">
         <v>13</v>
       </c>
-      <c r="AS12" s="27"/>
+      <c r="AS12" s="24"/>
       <c r="AT12" t="s">
         <v>130</v>
       </c>
@@ -11717,7 +11743,7 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="24"/>
       <c r="F13" t="s">
         <v>46</v>
       </c>
@@ -11727,7 +11753,7 @@
       <c r="H13" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="27"/>
+      <c r="I13" s="24"/>
       <c r="J13" t="s">
         <v>46</v>
       </c>
@@ -11737,7 +11763,7 @@
       <c r="L13" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="27"/>
+      <c r="M13" s="24"/>
       <c r="N13" t="s">
         <v>46</v>
       </c>
@@ -11747,7 +11773,7 @@
       <c r="P13" t="s">
         <v>13</v>
       </c>
-      <c r="Q13" s="27"/>
+      <c r="Q13" s="24"/>
       <c r="R13" t="s">
         <v>46</v>
       </c>
@@ -11757,7 +11783,7 @@
       <c r="T13" t="s">
         <v>13</v>
       </c>
-      <c r="U13" s="27"/>
+      <c r="U13" s="24"/>
       <c r="V13" t="s">
         <v>46</v>
       </c>
@@ -11767,7 +11793,7 @@
       <c r="X13" t="s">
         <v>13</v>
       </c>
-      <c r="Y13" s="27"/>
+      <c r="Y13" s="24"/>
       <c r="Z13" t="s">
         <v>131</v>
       </c>
@@ -11777,7 +11803,7 @@
       <c r="AB13" t="s">
         <v>13</v>
       </c>
-      <c r="AC13" s="27"/>
+      <c r="AC13" s="24"/>
       <c r="AD13" t="s">
         <v>131</v>
       </c>
@@ -11787,7 +11813,7 @@
       <c r="AF13" t="s">
         <v>13</v>
       </c>
-      <c r="AG13" s="27"/>
+      <c r="AG13" s="24"/>
       <c r="AH13" t="s">
         <v>131</v>
       </c>
@@ -11797,7 +11823,7 @@
       <c r="AJ13" t="s">
         <v>13</v>
       </c>
-      <c r="AK13" s="27"/>
+      <c r="AK13" s="24"/>
       <c r="AL13" t="s">
         <v>131</v>
       </c>
@@ -11807,7 +11833,7 @@
       <c r="AN13" t="s">
         <v>13</v>
       </c>
-      <c r="AO13" s="27"/>
+      <c r="AO13" s="24"/>
       <c r="AP13" t="s">
         <v>131</v>
       </c>
@@ -11817,7 +11843,7 @@
       <c r="AR13" t="s">
         <v>13</v>
       </c>
-      <c r="AS13" s="27"/>
+      <c r="AS13" s="24"/>
       <c r="AT13" t="s">
         <v>131</v>
       </c>
@@ -11839,7 +11865,7 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="27"/>
+      <c r="E14" s="24"/>
       <c r="F14" t="s">
         <v>90</v>
       </c>
@@ -11849,7 +11875,7 @@
       <c r="H14" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="27"/>
+      <c r="I14" s="24"/>
       <c r="J14" t="s">
         <v>90</v>
       </c>
@@ -11859,7 +11885,7 @@
       <c r="L14" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="27"/>
+      <c r="M14" s="24"/>
       <c r="N14" t="s">
         <v>90</v>
       </c>
@@ -11869,7 +11895,7 @@
       <c r="P14" t="s">
         <v>13</v>
       </c>
-      <c r="Q14" s="27"/>
+      <c r="Q14" s="24"/>
       <c r="R14" t="s">
         <v>90</v>
       </c>
@@ -11879,7 +11905,7 @@
       <c r="T14" t="s">
         <v>13</v>
       </c>
-      <c r="U14" s="27"/>
+      <c r="U14" s="24"/>
       <c r="V14" t="s">
         <v>90</v>
       </c>
@@ -11889,7 +11915,7 @@
       <c r="X14" t="s">
         <v>13</v>
       </c>
-      <c r="Y14" s="27"/>
+      <c r="Y14" s="24"/>
       <c r="Z14" t="s">
         <v>17</v>
       </c>
@@ -11900,7 +11926,7 @@
       <c r="AB14" t="s">
         <v>13</v>
       </c>
-      <c r="AC14" s="27"/>
+      <c r="AC14" s="24"/>
       <c r="AD14" t="s">
         <v>17</v>
       </c>
@@ -11911,7 +11937,7 @@
       <c r="AF14" t="s">
         <v>13</v>
       </c>
-      <c r="AG14" s="27"/>
+      <c r="AG14" s="24"/>
       <c r="AH14" t="s">
         <v>17</v>
       </c>
@@ -11922,7 +11948,7 @@
       <c r="AJ14" t="s">
         <v>13</v>
       </c>
-      <c r="AK14" s="27"/>
+      <c r="AK14" s="24"/>
       <c r="AL14" t="s">
         <v>17</v>
       </c>
@@ -11933,7 +11959,7 @@
       <c r="AN14" t="s">
         <v>13</v>
       </c>
-      <c r="AO14" s="27"/>
+      <c r="AO14" s="24"/>
       <c r="AP14" t="s">
         <v>17</v>
       </c>
@@ -11944,7 +11970,7 @@
       <c r="AR14" t="s">
         <v>13</v>
       </c>
-      <c r="AS14" s="27"/>
+      <c r="AS14" s="24"/>
       <c r="AT14" t="s">
         <v>17</v>
       </c>
@@ -11957,7 +11983,7 @@
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E15" s="27"/>
+      <c r="E15" s="24"/>
       <c r="F15" t="s">
         <v>130</v>
       </c>
@@ -11967,7 +11993,7 @@
       <c r="H15" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="27"/>
+      <c r="I15" s="24"/>
       <c r="J15" t="s">
         <v>130</v>
       </c>
@@ -11977,7 +12003,7 @@
       <c r="L15" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="27"/>
+      <c r="M15" s="24"/>
       <c r="N15" t="s">
         <v>130</v>
       </c>
@@ -11987,7 +12013,7 @@
       <c r="P15" t="s">
         <v>13</v>
       </c>
-      <c r="Q15" s="27"/>
+      <c r="Q15" s="24"/>
       <c r="R15" t="s">
         <v>130</v>
       </c>
@@ -11997,7 +12023,7 @@
       <c r="T15" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="27"/>
+      <c r="U15" s="24"/>
       <c r="V15" t="s">
         <v>130</v>
       </c>
@@ -12007,7 +12033,7 @@
       <c r="X15" t="s">
         <v>13</v>
       </c>
-      <c r="Y15" s="27"/>
+      <c r="Y15" s="24"/>
       <c r="Z15" t="s">
         <v>86</v>
       </c>
@@ -12017,7 +12043,7 @@
       <c r="AB15" t="s">
         <v>13</v>
       </c>
-      <c r="AC15" s="27"/>
+      <c r="AC15" s="24"/>
       <c r="AD15" t="s">
         <v>86</v>
       </c>
@@ -12027,7 +12053,7 @@
       <c r="AF15" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="27"/>
+      <c r="AG15" s="24"/>
       <c r="AH15" t="s">
         <v>86</v>
       </c>
@@ -12037,7 +12063,7 @@
       <c r="AJ15" t="s">
         <v>13</v>
       </c>
-      <c r="AK15" s="27"/>
+      <c r="AK15" s="24"/>
       <c r="AL15" t="s">
         <v>86</v>
       </c>
@@ -12047,7 +12073,7 @@
       <c r="AN15" t="s">
         <v>13</v>
       </c>
-      <c r="AO15" s="27"/>
+      <c r="AO15" s="24"/>
       <c r="AP15" t="s">
         <v>86</v>
       </c>
@@ -12057,7 +12083,7 @@
       <c r="AR15" t="s">
         <v>13</v>
       </c>
-      <c r="AS15" s="27"/>
+      <c r="AS15" s="24"/>
       <c r="AT15" t="s">
         <v>86</v>
       </c>
@@ -12078,7 +12104,7 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="27"/>
+      <c r="E16" s="24"/>
       <c r="F16" t="s">
         <v>131</v>
       </c>
@@ -12088,7 +12114,7 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="27"/>
+      <c r="I16" s="24"/>
       <c r="J16" t="s">
         <v>131</v>
       </c>
@@ -12098,7 +12124,7 @@
       <c r="L16" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="27"/>
+      <c r="M16" s="24"/>
       <c r="N16" t="s">
         <v>131</v>
       </c>
@@ -12108,7 +12134,7 @@
       <c r="P16" t="s">
         <v>13</v>
       </c>
-      <c r="Q16" s="27"/>
+      <c r="Q16" s="24"/>
       <c r="R16" t="s">
         <v>131</v>
       </c>
@@ -12118,7 +12144,7 @@
       <c r="T16" t="s">
         <v>13</v>
       </c>
-      <c r="U16" s="27"/>
+      <c r="U16" s="24"/>
       <c r="V16" t="s">
         <v>131</v>
       </c>
@@ -12128,7 +12154,7 @@
       <c r="X16" t="s">
         <v>13</v>
       </c>
-      <c r="Y16" s="27"/>
+      <c r="Y16" s="24"/>
       <c r="Z16" t="s">
         <v>137</v>
       </c>
@@ -12138,7 +12164,7 @@
       <c r="AB16" t="s">
         <v>13</v>
       </c>
-      <c r="AC16" s="27"/>
+      <c r="AC16" s="24"/>
       <c r="AD16" t="s">
         <v>137</v>
       </c>
@@ -12148,7 +12174,7 @@
       <c r="AF16" t="s">
         <v>13</v>
       </c>
-      <c r="AG16" s="27"/>
+      <c r="AG16" s="24"/>
       <c r="AH16" t="s">
         <v>137</v>
       </c>
@@ -12158,7 +12184,7 @@
       <c r="AJ16" t="s">
         <v>13</v>
       </c>
-      <c r="AK16" s="27"/>
+      <c r="AK16" s="24"/>
       <c r="AL16" t="s">
         <v>137</v>
       </c>
@@ -12168,7 +12194,7 @@
       <c r="AN16" t="s">
         <v>13</v>
       </c>
-      <c r="AO16" s="27"/>
+      <c r="AO16" s="24"/>
       <c r="AP16" t="s">
         <v>137</v>
       </c>
@@ -12178,7 +12204,7 @@
       <c r="AR16" t="s">
         <v>13</v>
       </c>
-      <c r="AS16" s="27"/>
+      <c r="AS16" s="24"/>
       <c r="AT16" t="s">
         <v>137</v>
       </c>
@@ -12199,7 +12225,7 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="24"/>
       <c r="F17" t="s">
         <v>9</v>
       </c>
@@ -12209,7 +12235,7 @@
       <c r="H17" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="27"/>
+      <c r="I17" s="24"/>
       <c r="J17" t="s">
         <v>9</v>
       </c>
@@ -12219,7 +12245,7 @@
       <c r="L17" t="s">
         <v>13</v>
       </c>
-      <c r="M17" s="27"/>
+      <c r="M17" s="24"/>
       <c r="N17" t="s">
         <v>9</v>
       </c>
@@ -12229,7 +12255,7 @@
       <c r="P17" t="s">
         <v>13</v>
       </c>
-      <c r="Q17" s="27"/>
+      <c r="Q17" s="24"/>
       <c r="R17" t="s">
         <v>9</v>
       </c>
@@ -12239,7 +12265,7 @@
       <c r="T17" t="s">
         <v>13</v>
       </c>
-      <c r="U17" s="27"/>
+      <c r="U17" s="24"/>
       <c r="V17" t="s">
         <v>9</v>
       </c>
@@ -12249,7 +12275,7 @@
       <c r="X17" t="s">
         <v>13</v>
       </c>
-      <c r="Y17" s="27"/>
+      <c r="Y17" s="24"/>
       <c r="Z17" t="s">
         <v>138</v>
       </c>
@@ -12259,7 +12285,7 @@
       <c r="AB17" t="s">
         <v>13</v>
       </c>
-      <c r="AC17" s="27"/>
+      <c r="AC17" s="24"/>
       <c r="AD17" t="s">
         <v>138</v>
       </c>
@@ -12269,7 +12295,7 @@
       <c r="AF17" t="s">
         <v>13</v>
       </c>
-      <c r="AG17" s="27"/>
+      <c r="AG17" s="24"/>
       <c r="AH17" t="s">
         <v>138</v>
       </c>
@@ -12279,7 +12305,7 @@
       <c r="AJ17" t="s">
         <v>13</v>
       </c>
-      <c r="AK17" s="27"/>
+      <c r="AK17" s="24"/>
       <c r="AL17" t="s">
         <v>138</v>
       </c>
@@ -12289,7 +12315,7 @@
       <c r="AN17" t="s">
         <v>13</v>
       </c>
-      <c r="AO17" s="27"/>
+      <c r="AO17" s="24"/>
       <c r="AP17" t="s">
         <v>138</v>
       </c>
@@ -12299,7 +12325,7 @@
       <c r="AR17" t="s">
         <v>13</v>
       </c>
-      <c r="AS17" s="27"/>
+      <c r="AS17" s="24"/>
       <c r="AT17" t="s">
         <v>138</v>
       </c>
@@ -12321,7 +12347,7 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="27"/>
+      <c r="E18" s="24"/>
       <c r="F18" t="s">
         <v>17</v>
       </c>
@@ -12332,7 +12358,7 @@
       <c r="H18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="27"/>
+      <c r="I18" s="24"/>
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -12343,7 +12369,7 @@
       <c r="L18" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="27"/>
+      <c r="M18" s="24"/>
       <c r="N18" t="s">
         <v>17</v>
       </c>
@@ -12354,7 +12380,7 @@
       <c r="P18" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="27"/>
+      <c r="Q18" s="24"/>
       <c r="R18" t="s">
         <v>17</v>
       </c>
@@ -12365,7 +12391,7 @@
       <c r="T18" t="s">
         <v>13</v>
       </c>
-      <c r="U18" s="27"/>
+      <c r="U18" s="24"/>
       <c r="V18" t="s">
         <v>17</v>
       </c>
@@ -12376,7 +12402,7 @@
       <c r="X18" t="s">
         <v>13</v>
       </c>
-      <c r="Y18" s="27"/>
+      <c r="Y18" s="24"/>
       <c r="Z18" t="s">
         <v>21</v>
       </c>
@@ -12387,7 +12413,7 @@
       <c r="AB18" t="s">
         <v>13</v>
       </c>
-      <c r="AC18" s="27"/>
+      <c r="AC18" s="24"/>
       <c r="AD18" t="s">
         <v>21</v>
       </c>
@@ -12398,7 +12424,7 @@
       <c r="AF18" t="s">
         <v>13</v>
       </c>
-      <c r="AG18" s="27"/>
+      <c r="AG18" s="24"/>
       <c r="AH18" t="s">
         <v>21</v>
       </c>
@@ -12409,7 +12435,7 @@
       <c r="AJ18" t="s">
         <v>13</v>
       </c>
-      <c r="AK18" s="27"/>
+      <c r="AK18" s="24"/>
       <c r="AL18" t="s">
         <v>21</v>
       </c>
@@ -12420,7 +12446,7 @@
       <c r="AN18" t="s">
         <v>13</v>
       </c>
-      <c r="AO18" s="27"/>
+      <c r="AO18" s="24"/>
       <c r="AP18" t="s">
         <v>21</v>
       </c>
@@ -12431,7 +12457,7 @@
       <c r="AR18" t="s">
         <v>13</v>
       </c>
-      <c r="AS18" s="27"/>
+      <c r="AS18" s="24"/>
       <c r="AT18" t="s">
         <v>21</v>
       </c>
@@ -12444,7 +12470,7 @@
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E19" s="27"/>
+      <c r="E19" s="24"/>
       <c r="F19" t="s">
         <v>86</v>
       </c>
@@ -12454,7 +12480,7 @@
       <c r="H19" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="27"/>
+      <c r="I19" s="24"/>
       <c r="J19" t="s">
         <v>86</v>
       </c>
@@ -12464,7 +12490,7 @@
       <c r="L19" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="27"/>
+      <c r="M19" s="24"/>
       <c r="N19" t="s">
         <v>86</v>
       </c>
@@ -12474,7 +12500,7 @@
       <c r="P19" t="s">
         <v>13</v>
       </c>
-      <c r="Q19" s="27"/>
+      <c r="Q19" s="24"/>
       <c r="R19" t="s">
         <v>86</v>
       </c>
@@ -12484,7 +12510,7 @@
       <c r="T19" t="s">
         <v>13</v>
       </c>
-      <c r="U19" s="27"/>
+      <c r="U19" s="24"/>
       <c r="V19" t="s">
         <v>86</v>
       </c>
@@ -12494,12 +12520,12 @@
       <c r="X19" t="s">
         <v>13</v>
       </c>
-      <c r="Y19" s="27"/>
-      <c r="AC19" s="27"/>
-      <c r="AG19" s="27"/>
-      <c r="AK19" s="27"/>
-      <c r="AO19" s="27"/>
-      <c r="AS19" s="27"/>
+      <c r="Y19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AG19" s="24"/>
+      <c r="AK19" s="24"/>
+      <c r="AO19" s="24"/>
+      <c r="AS19" s="24"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -12511,7 +12537,7 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="27"/>
+      <c r="E20" s="24"/>
       <c r="F20" t="s">
         <v>139</v>
       </c>
@@ -12521,7 +12547,7 @@
       <c r="H20" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="27"/>
+      <c r="I20" s="24"/>
       <c r="J20" t="s">
         <v>139</v>
       </c>
@@ -12531,7 +12557,7 @@
       <c r="L20" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="27"/>
+      <c r="M20" s="24"/>
       <c r="N20" t="s">
         <v>139</v>
       </c>
@@ -12541,7 +12567,7 @@
       <c r="P20" t="s">
         <v>13</v>
       </c>
-      <c r="Q20" s="27"/>
+      <c r="Q20" s="24"/>
       <c r="R20" t="s">
         <v>139</v>
       </c>
@@ -12551,7 +12577,7 @@
       <c r="T20" t="s">
         <v>13</v>
       </c>
-      <c r="U20" s="27"/>
+      <c r="U20" s="24"/>
       <c r="V20" t="s">
         <v>139</v>
       </c>
@@ -12561,12 +12587,12 @@
       <c r="X20" t="s">
         <v>13</v>
       </c>
-      <c r="Y20" s="27"/>
-      <c r="AC20" s="27"/>
-      <c r="AG20" s="27"/>
-      <c r="AK20" s="27"/>
-      <c r="AO20" s="27"/>
-      <c r="AS20" s="27"/>
+      <c r="Y20" s="24"/>
+      <c r="AC20" s="24"/>
+      <c r="AG20" s="24"/>
+      <c r="AK20" s="24"/>
+      <c r="AO20" s="24"/>
+      <c r="AS20" s="24"/>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -12578,7 +12604,7 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="27"/>
+      <c r="E21" s="24"/>
       <c r="F21" t="s">
         <v>132</v>
       </c>
@@ -12589,7 +12615,7 @@
       <c r="H21" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="27"/>
+      <c r="I21" s="24"/>
       <c r="J21" t="s">
         <v>132</v>
       </c>
@@ -12600,7 +12626,7 @@
       <c r="L21" t="s">
         <v>13</v>
       </c>
-      <c r="M21" s="27"/>
+      <c r="M21" s="24"/>
       <c r="N21" t="s">
         <v>132</v>
       </c>
@@ -12611,7 +12637,7 @@
       <c r="P21" t="s">
         <v>13</v>
       </c>
-      <c r="Q21" s="27"/>
+      <c r="Q21" s="24"/>
       <c r="R21" t="s">
         <v>132</v>
       </c>
@@ -12622,7 +12648,7 @@
       <c r="T21" t="s">
         <v>13</v>
       </c>
-      <c r="U21" s="27"/>
+      <c r="U21" s="24"/>
       <c r="V21" t="s">
         <v>132</v>
       </c>
@@ -12633,12 +12659,12 @@
       <c r="X21" t="s">
         <v>13</v>
       </c>
-      <c r="Y21" s="27"/>
-      <c r="AC21" s="27"/>
-      <c r="AG21" s="27"/>
-      <c r="AK21" s="27"/>
-      <c r="AO21" s="27"/>
-      <c r="AS21" s="27"/>
+      <c r="Y21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AG21" s="24"/>
+      <c r="AK21" s="24"/>
+      <c r="AO21" s="24"/>
+      <c r="AS21" s="24"/>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -12650,17 +12676,17 @@
       <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="Y22" s="27"/>
-      <c r="AC22" s="27"/>
-      <c r="AG22" s="27"/>
-      <c r="AK22" s="27"/>
-      <c r="AO22" s="27"/>
-      <c r="AS22" s="27"/>
+      <c r="E22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="Y22" s="24"/>
+      <c r="AC22" s="24"/>
+      <c r="AG22" s="24"/>
+      <c r="AK22" s="24"/>
+      <c r="AO22" s="24"/>
+      <c r="AS22" s="24"/>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -12673,43 +12699,43 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="Y23" s="27"/>
-      <c r="AC23" s="27"/>
-      <c r="AG23" s="27"/>
-      <c r="AK23" s="27"/>
-      <c r="AO23" s="27"/>
-      <c r="AS23" s="27"/>
+      <c r="E23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="Y23" s="24"/>
+      <c r="AC23" s="24"/>
+      <c r="AG23" s="24"/>
+      <c r="AK23" s="24"/>
+      <c r="AO23" s="24"/>
+      <c r="AS23" s="24"/>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="AC24" s="27"/>
-      <c r="AG24" s="27"/>
-      <c r="AK24" s="27"/>
-      <c r="AO24" s="27"/>
-      <c r="AS24" s="27"/>
+      <c r="E24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="Y24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AG24" s="24"/>
+      <c r="AK24" s="24"/>
+      <c r="AO24" s="24"/>
+      <c r="AS24" s="24"/>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="E25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="Y25" s="27"/>
-      <c r="AC25" s="27"/>
-      <c r="AG25" s="27"/>
-      <c r="AK25" s="27"/>
-      <c r="AO25" s="27"/>
-      <c r="AS25" s="27"/>
+      <c r="E25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="AC25" s="24"/>
+      <c r="AG25" s="24"/>
+      <c r="AK25" s="24"/>
+      <c r="AO25" s="24"/>
+      <c r="AS25" s="24"/>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -12846,8 +12872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5F06E4-4B71-4DD5-A2F8-F472E18DC771}">
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12902,50 +12928,50 @@
       </c>
       <c r="E1" s="25"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="18"/>
       <c r="J1" s="26" t="s">
         <v>115</v>
       </c>
       <c r="K1" s="26"/>
       <c r="L1" s="18"/>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="24"/>
+      <c r="N1" s="27"/>
       <c r="O1" s="18"/>
       <c r="P1" s="26" t="s">
         <v>117</v>
       </c>
       <c r="Q1" s="26"/>
       <c r="R1" s="18"/>
-      <c r="S1" s="24" t="s">
+      <c r="S1" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="24"/>
+      <c r="T1" s="27"/>
       <c r="U1" s="18"/>
       <c r="V1" s="26" t="s">
         <v>119</v>
       </c>
       <c r="W1" s="26"/>
       <c r="X1" s="18"/>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" s="24"/>
+      <c r="Z1" s="27"/>
       <c r="AA1" s="18"/>
       <c r="AB1" s="26" t="s">
         <v>121</v>
       </c>
       <c r="AC1" s="26"/>
       <c r="AD1" s="18"/>
-      <c r="AE1" s="24" t="s">
+      <c r="AE1" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="AF1" s="24"/>
+      <c r="AF1" s="27"/>
       <c r="AG1" s="18"/>
       <c r="AH1" s="26" t="s">
         <v>123</v>
@@ -12955,7 +12981,7 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="B2" s="20">
         <f>'Apollo 5'!F28</f>
@@ -12963,7 +12989,7 @@
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" s="20">
         <f>'Apollo 7'!F28</f>
@@ -13053,7 +13079,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="B3" s="20">
         <f>'Apollo 5'!F29</f>
@@ -13061,7 +13087,7 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="20">
         <f>'Apollo 7'!F29</f>
@@ -13150,16 +13176,11 @@
       <c r="AJ3" s="19"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="20">
-        <f>'Apollo 5'!F30</f>
-        <v>42540.699999999953</v>
-      </c>
+      <c r="A4" s="15"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="19"/>
       <c r="D4" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="20">
         <f>'Apollo 7'!F30</f>
@@ -13249,7 +13270,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="B5" s="20">
         <f>'Apollo 5'!F31</f>
@@ -13257,7 +13278,7 @@
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="20">
         <f>'Apollo 7'!F31</f>
@@ -13347,7 +13368,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="B6" s="20">
         <f>'Apollo 5'!F32</f>
@@ -13444,11 +13465,21 @@
       <c r="AJ6" s="19"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="20">
+        <f>'Apollo 5'!G13/2</f>
+        <v>29.25</v>
+      </c>
       <c r="C7" s="19"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="20">
+        <f>'Apollo 7'!G21/2</f>
+        <v>30.617484975</v>
+      </c>
       <c r="F7" s="19"/>
       <c r="G7" s="16" t="s">
         <v>60</v>
@@ -13532,11 +13563,21 @@
       <c r="AJ7" s="19"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="20">
+        <f>'Apollo 5'!G13/2</f>
+        <v>29.25</v>
+      </c>
       <c r="C8" s="19"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="20">
+        <f>'Apollo 7'!G21/2</f>
+        <v>30.617484975</v>
+      </c>
       <c r="F8" s="19"/>
       <c r="G8" s="16" t="s">
         <v>55</v>
@@ -13620,6 +13661,9 @@
       <c r="AJ8" s="19"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>147</v>
+      </c>
       <c r="C9"/>
       <c r="E9" s="21"/>
       <c r="F9"/>
@@ -13647,12 +13691,12 @@
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>A2&amp;" "&amp;B2</f>
-        <v>SIIFUELMASS 413696.1</v>
+        <v>FMASS 413696.1</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="str">
         <f>D2&amp;" "&amp;E2</f>
-        <v>SIIFUELMASS 411967.9</v>
+        <v>SIFUELMASS 411967.9</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10"/>
@@ -13719,13 +13763,13 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" ref="A11:A14" si="0">A3&amp;" "&amp;B3</f>
-        <v>S4FUELMASS 105034.4</v>
+        <f t="shared" ref="A11:A16" si="0">A3&amp;" "&amp;B3</f>
+        <v>FMASS 105034.4</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="str">
-        <f t="shared" ref="D11:D14" si="1">D3&amp;" "&amp;E3</f>
-        <v>S4FUELMASS 105872.9950817</v>
+        <f t="shared" ref="D11:D16" si="1">D3&amp;" "&amp;E3</f>
+        <v>SIIFUELMASS 105872.9950817</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11"/>
@@ -13791,14 +13835,13 @@
       <c r="AJ11"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>SIIEMPTYMASS 42540.6999999999</v>
+      <c r="A12" s="28" t="s">
+        <v>148</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
-        <v>SIIEMPTYMASS 41858.5</v>
+        <v>SIEMPTYMASS 41858.5</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12"/>
@@ -13865,13 +13908,13 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>S4EMPTYMASS 13216.7</v>
+        <f>A5&amp;" "&amp;B5</f>
+        <v>EMASS 13216.7</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
-        <v>S4EMPTYMASS 12417.5049183</v>
+        <v>SIIEMPTYMASS 12417.5049183</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13"/>
@@ -13938,8 +13981,8 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>INTERSTAGE 2615.9</v>
+        <f>A6&amp;" "&amp;B6</f>
+        <v>EMASS 2615.9</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="str">
@@ -14010,7 +14053,15 @@
       <c r="AJ14"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>APSFMASS1 29.25</v>
+      </c>
       <c r="C15"/>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>APS1 30.617484975</v>
+      </c>
       <c r="E15" s="21"/>
       <c r="F15"/>
       <c r="G15" t="str">
@@ -14075,7 +14126,15 @@
       <c r="AJ15"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>APSFMASS2 29.25</v>
+      </c>
       <c r="C16"/>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>APS2 30.617484975</v>
+      </c>
       <c r="E16" s="21"/>
       <c r="F16"/>
       <c r="G16" t="str">
@@ -14141,11 +14200,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
@@ -14153,6 +14207,11 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add padloaded masses into comparison tables
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EEBF20-56E5-4581-BA06-F1A99CDE64A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F99C9B-F8F6-4CDF-B8C5-053851B2E4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -706,16 +706,16 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7153,8 +7153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80FCE58-7FB9-4CC7-8163-D01D25C81D7D}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10281,8 +10281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8612F4-CCB1-4696-8897-C4C5EFBE3F4E}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12872,8 +12872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5F06E4-4B71-4DD5-A2F8-F472E18DC771}">
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12918,15 +12918,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="18"/>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="18"/>
       <c r="G1" s="27" t="s">
         <v>114</v>
@@ -13273,8 +13273,8 @@
         <v>146</v>
       </c>
       <c r="B5" s="20">
-        <f>'Apollo 5'!F31</f>
-        <v>13216.700000000012</v>
+        <f>'Apollo 5'!F30</f>
+        <v>42540.699999999953</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="15" t="s">
@@ -13371,8 +13371,8 @@
         <v>146</v>
       </c>
       <c r="B6" s="20">
-        <f>'Apollo 5'!F32</f>
-        <v>2615.9</v>
+        <f>'Apollo 5'!F31</f>
+        <v>13216.700000000012</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="15" t="s">
@@ -13661,7 +13661,7 @@
       <c r="AJ8" s="19"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="25" t="s">
         <v>147</v>
       </c>
       <c r="C9"/>
@@ -13763,144 +13763,144 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" ref="A11:A16" si="0">A3&amp;" "&amp;B3</f>
-        <v>FMASS 105034.4</v>
+        <f>A5&amp;" "&amp;B5</f>
+        <v>EMASS 42540.6999999999</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="str">
-        <f t="shared" ref="D11:D16" si="1">D3&amp;" "&amp;E3</f>
+        <f t="shared" ref="D11:D16" si="0">D3&amp;" "&amp;E3</f>
         <v>SIIFUELMASS 105872.9950817</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11"/>
       <c r="G11" t="str">
-        <f t="shared" ref="G11:G16" si="2">G3&amp;" "&amp;H3</f>
+        <f t="shared" ref="G11:G16" si="1">G3&amp;" "&amp;H3</f>
         <v>SIIFUELMASS 430664</v>
       </c>
       <c r="H11" s="21"/>
       <c r="I11"/>
       <c r="J11" t="str">
-        <f t="shared" ref="J11:J15" si="3">J3&amp;" "&amp;K3</f>
+        <f t="shared" ref="J11:J15" si="2">J3&amp;" "&amp;K3</f>
         <v>SIIFUELMASS 444829</v>
       </c>
       <c r="K11" s="21"/>
       <c r="L11"/>
       <c r="M11" t="str">
-        <f t="shared" ref="M11:M16" si="4">M3&amp;" "&amp;N3</f>
+        <f t="shared" ref="M11:M16" si="3">M3&amp;" "&amp;N3</f>
         <v>SIIFUELMASS 445628</v>
       </c>
       <c r="N11" s="21"/>
       <c r="O11"/>
       <c r="P11" t="str">
-        <f t="shared" ref="P11:P16" si="5">P3&amp;" "&amp;Q3</f>
+        <f t="shared" ref="P11:P16" si="4">P3&amp;" "&amp;Q3</f>
         <v>SIIFUELMASS 443500</v>
       </c>
       <c r="Q11" s="21"/>
       <c r="R11"/>
       <c r="S11" t="str">
-        <f t="shared" ref="S11:S16" si="6">S3&amp;" "&amp;T3</f>
+        <f t="shared" ref="S11:S16" si="5">S3&amp;" "&amp;T3</f>
         <v>SIIFUELMASS 446320</v>
       </c>
       <c r="T11" s="21"/>
       <c r="U11"/>
       <c r="V11" t="str">
-        <f t="shared" ref="V11:V16" si="7">V3&amp;" "&amp;W3</f>
+        <f t="shared" ref="V11:V16" si="6">V3&amp;" "&amp;W3</f>
         <v>SIIFUELMASS 452316</v>
       </c>
       <c r="W11" s="21"/>
       <c r="X11"/>
       <c r="Y11" t="str">
-        <f t="shared" ref="Y11:Y16" si="8">Y3&amp;" "&amp;Z3</f>
+        <f t="shared" ref="Y11:Y16" si="7">Y3&amp;" "&amp;Z3</f>
         <v>SIIFUELMASS 452308</v>
       </c>
       <c r="Z11" s="21"/>
       <c r="AA11"/>
       <c r="AB11" t="str">
-        <f t="shared" ref="AB11:AB16" si="9">AB3&amp;" "&amp;AC3</f>
+        <f t="shared" ref="AB11:AB16" si="8">AB3&amp;" "&amp;AC3</f>
         <v>SIIFUELMASS 452430</v>
       </c>
       <c r="AC11" s="21"/>
       <c r="AD11"/>
       <c r="AE11" t="str">
-        <f t="shared" ref="AE11:AE16" si="10">AE3&amp;" "&amp;AF3</f>
+        <f t="shared" ref="AE11:AE16" si="9">AE3&amp;" "&amp;AF3</f>
         <v>SIIFUELMASS 456812</v>
       </c>
       <c r="AF11" s="21"/>
       <c r="AG11"/>
       <c r="AH11" t="str">
-        <f t="shared" ref="AH11:AH15" si="11">AH3&amp;" "&amp;AI3</f>
+        <f t="shared" ref="AH11:AH15" si="10">AH3&amp;" "&amp;AI3</f>
         <v>SIIFUELMASS 455806</v>
       </c>
       <c r="AI11" s="21"/>
       <c r="AJ11"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>148</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>SIEMPTYMASS 41858.5</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12"/>
       <c r="G12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S4FUELMASS 107469</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12"/>
       <c r="J12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>S4FUELMASS 106205</v>
       </c>
       <c r="K12" s="21"/>
       <c r="L12"/>
       <c r="M12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S4FUELMASS 107157</v>
       </c>
       <c r="N12" s="21"/>
       <c r="O12"/>
       <c r="P12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S4FUELMASS 107428</v>
       </c>
       <c r="Q12" s="21"/>
       <c r="R12"/>
       <c r="S12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S4FUELMASS 106591</v>
       </c>
       <c r="T12" s="21"/>
       <c r="U12"/>
       <c r="V12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S4FUELMASS 107179</v>
       </c>
       <c r="W12" s="21"/>
       <c r="X12"/>
       <c r="Y12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>S4FUELMASS 106488</v>
       </c>
       <c r="Z12" s="21"/>
       <c r="AA12"/>
       <c r="AB12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>S4FUELMASS 108958</v>
       </c>
       <c r="AC12" s="21"/>
       <c r="AD12"/>
       <c r="AE12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>S4FUELMASS 108780</v>
       </c>
       <c r="AF12" s="21"/>
       <c r="AG12"/>
       <c r="AH12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>S4FUELMASS 108914</v>
       </c>
       <c r="AI12" s="21"/>
@@ -13908,72 +13908,72 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>A5&amp;" "&amp;B5</f>
-        <v>EMASS 13216.7</v>
+        <f>A3&amp;" "&amp;B3</f>
+        <v>FMASS 105034.4</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>SIIEMPTYMASS 12417.5049183</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13"/>
       <c r="G13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>SIEMPTYMASS 141670</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13"/>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SIEMPTYMASS 136740</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13"/>
       <c r="M13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>SIEMPTYMASS 136520</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13"/>
       <c r="P13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>SIEMPTYMASS 133602</v>
       </c>
       <c r="Q13" s="21"/>
       <c r="R13"/>
       <c r="S13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>SIEMPTYMASS 133859</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13"/>
       <c r="V13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>SIEMPTYMASS 133764</v>
       </c>
       <c r="W13" s="21"/>
       <c r="X13"/>
       <c r="Y13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>SIEMPTYMASS 133364</v>
       </c>
       <c r="Z13" s="21"/>
       <c r="AA13"/>
       <c r="AB13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>SIEMPTYMASS 132487</v>
       </c>
       <c r="AC13" s="21"/>
       <c r="AD13"/>
       <c r="AE13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>SIEMPTYMASS 133748</v>
       </c>
       <c r="AF13" s="21"/>
       <c r="AG13"/>
       <c r="AH13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>SIEMPTYMASS 133521</v>
       </c>
       <c r="AI13" s="21"/>
@@ -13982,71 +13982,71 @@
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>A6&amp;" "&amp;B6</f>
-        <v>EMASS 2615.9</v>
+        <v>EMASS 13216.7</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>INTERSTAGE 2514.3</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14"/>
       <c r="G14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>SIIEMPTYMASS 44151</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14"/>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>SIIEMPTYMASS 41919</v>
       </c>
       <c r="K14" s="21"/>
       <c r="L14"/>
       <c r="M14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>SIIEMPTYMASS 41923</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14"/>
       <c r="P14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>SIIEMPTYMASS 39869</v>
       </c>
       <c r="Q14" s="21"/>
       <c r="R14"/>
       <c r="S14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>SIIEMPTYMASS 40081</v>
       </c>
       <c r="T14" s="21"/>
       <c r="U14"/>
       <c r="V14" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>SIIEMPTYMASS 39068</v>
       </c>
       <c r="W14" s="21"/>
       <c r="X14"/>
       <c r="Y14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>SIIEMPTYMASS 39136</v>
       </c>
       <c r="Z14" s="21"/>
       <c r="AA14"/>
       <c r="AB14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>SIIEMPTYMASS 39478</v>
       </c>
       <c r="AC14" s="21"/>
       <c r="AD14"/>
       <c r="AE14" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>SIIEMPTYMASS 40151</v>
       </c>
       <c r="AF14" s="21"/>
       <c r="AG14"/>
       <c r="AH14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>SIIEMPTYMASS 40163</v>
       </c>
       <c r="AI14" s="21"/>
@@ -14054,72 +14054,72 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A11:A16" si="11">A7&amp;" "&amp;B7</f>
         <v>APSFMASS1 29.25</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>APS1 30.617484975</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15"/>
       <c r="G15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>S4EMPTYMASS 14189</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15"/>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>S4EMPTYMASS 13549</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15"/>
       <c r="M15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>S4EMPTYMASS 13810</v>
       </c>
       <c r="N15" s="21"/>
       <c r="O15"/>
       <c r="P15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>S4EMPTYMASS 13439</v>
       </c>
       <c r="Q15" s="21"/>
       <c r="R15"/>
       <c r="S15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>S4EMPTYMASS 13541</v>
       </c>
       <c r="T15" s="21"/>
       <c r="U15"/>
       <c r="V15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>S4EMPTYMASS 13786</v>
       </c>
       <c r="W15" s="21"/>
       <c r="X15"/>
       <c r="Y15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>S4EMPTYMASS 13762</v>
       </c>
       <c r="Z15" s="21"/>
       <c r="AA15"/>
       <c r="AB15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>S4EMPTYMASS 13828</v>
       </c>
       <c r="AC15" s="21"/>
       <c r="AD15"/>
       <c r="AE15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>S4EMPTYMASS 13784</v>
       </c>
       <c r="AF15" s="21"/>
       <c r="AG15"/>
       <c r="AH15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>S4EMPTYMASS 13747</v>
       </c>
       <c r="AI15" s="21"/>
@@ -14127,18 +14127,18 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>APSFMASS2 29.25</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>APS2 30.617484975</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16"/>
       <c r="G16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>INTERSTAGE 4376</v>
       </c>
       <c r="H16" s="21"/>
@@ -14150,43 +14150,43 @@
       <c r="K16" s="21"/>
       <c r="L16"/>
       <c r="M16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>INTERSTAGE 4033</v>
       </c>
       <c r="N16" s="21"/>
       <c r="O16"/>
       <c r="P16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>INTERSTAGE 3982</v>
       </c>
       <c r="Q16" s="21"/>
       <c r="R16"/>
       <c r="S16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>INTERSTAGE 3996</v>
       </c>
       <c r="T16" s="21"/>
       <c r="U16"/>
       <c r="V16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>INTERSTAGE 3972</v>
       </c>
       <c r="W16" s="21"/>
       <c r="X16"/>
       <c r="Y16" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>INTERSTAGE 3945</v>
       </c>
       <c r="Z16" s="21"/>
       <c r="AA16"/>
       <c r="AB16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>INTERSTAGE 3504</v>
       </c>
       <c r="AC16" s="21"/>
       <c r="AD16"/>
       <c r="AE16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>INTERSTAGE 3960</v>
       </c>
       <c r="AF16" s="21"/>
@@ -14200,6 +14200,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
@@ -14207,11 +14212,6 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>